<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx workbook with latest functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,25 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EE7AF8-9B93-4703-8045-DF42E00BF3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6D4AFD-E4C3-4FC0-87CD-DBD4D286D154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10530" yWindow="3015" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
+    <workbookView xWindow="10185" yWindow="2670" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
+    <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
     <definedName name="COINTOSS">_xlfn.LAMBDA(PICK("Heads","Tails"))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,SUM(_xlpm.x,-1))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
+    <definedName name="EQUAL">_xlfn.LAMBDA(_xlpm.this,_xlpm.that,_xlpm.this=_xlpm.that)</definedName>
+    <definedName name="FIRSTLETTER">_xlfn.LAMBDA(_xlpm.text,LEFT(_xlpm.text,1))</definedName>
     <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
+    <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4)))</definedName>
+    <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
     <definedName name="LTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x&lt;=_xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="MAGIC8BALL">_xlfn.LAMBDA(_xlop.yes_or_no_question,IF(PROVIDED(_xlpm.yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered"))</definedName>
+    <definedName name="NO">FALSE</definedName>
     <definedName name="OTHERWISE">TRUE</definedName>
     <definedName name="PICK">_xlfn.LAMBDA(_xlpm._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),CHOOSE(RANDBETWEEN(1, _xlpm.count), _xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5, _xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25)))</definedName>
     <definedName name="PROVIDED">_xlfn.LAMBDA(_xlop.argument,NOT(_xlfn.ISOMITTED(_xlpm.argument)))</definedName>
-    <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(_xlpm.throw),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cuts Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cuts Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))</definedName>
+    <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(_xlpm.throw)),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cuts Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cuts Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))</definedName>
+    <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
+    <definedName name="YES">TRUE</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with latest functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6D4AFD-E4C3-4FC0-87CD-DBD4D286D154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8ECA89-6198-4F82-89A3-7045BD48C033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10185" yWindow="2670" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
@@ -17,7 +17,9 @@
   </sheets>
   <definedNames>
     <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
+    <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
+    <definedName name="CDR">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,DECREMENT(COLUMNS(_xlpm.range)),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,INCREMENT(_xlpm.col)))),_xlfn.MAKEARRAY(DECREMENT(ROWS(_xlpm.range)),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,INCREMENT(_xlpm.row),1)))))</definedName>
     <definedName name="COINTOSS">_xlfn.LAMBDA(PICK("Heads","Tails"))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,SUM(_xlpm.x,-1))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
@@ -25,8 +27,12 @@
     <definedName name="FIRSTLETTER">_xlfn.LAMBDA(_xlpm.text,LEFT(_xlpm.text,1))</definedName>
     <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
     <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4)))</definedName>
+    <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
+    <definedName name="GTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt;= _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
+    <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,SUM(_xlpm.x,1))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
+    <definedName name="LESSTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &lt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="LTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x&lt;=_xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="MAGIC8BALL">_xlfn.LAMBDA(_xlop.yes_or_no_question,IF(PROVIDED(_xlpm.yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered"))</definedName>
     <definedName name="NO">FALSE</definedName>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with FIRSTWORD, CONTAINS, FILENAME, SHEETNAME, and CELLNAME
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191E85B5-373B-4F3A-A067-5406A86A2538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C6045-41FE-49ED-A036-67932FF34ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
+    <workbookView xWindow="10185" yWindow="2670" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,17 @@
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
     <definedName name="CDR">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,DECREMENT(COLUMNS(_xlpm.range)),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,INCREMENT(_xlpm.col)))),_xlfn.MAKEARRAY(DECREMENT(ROWS(_xlpm.range)),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,INCREMENT(_xlpm.row),1)))))</definedName>
+    <definedName name="CELLNAME">_xlfn.LAMBDA(_xlop.reference,_xlop.absolute,_xlfn.LET(_xlpm.address,IFOMITTED(_xlpm.reference,CELL("address"),CELL("address",_xlpm.reference)),_xlpm.display_absolute,DEFAULT(_xlpm.absolute,NO),IF(_xlpm.display_absolute,_xlpm.address,SUBSTITUTE(_xlpm.address,"$",""))))</definedName>
     <definedName name="COINTOSS">_xlfn.LAMBDA(PICK("Heads","Tails"))</definedName>
     <definedName name="CONS">_xlfn.LAMBDA(_xlpm.value,_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.HSTACK(_xlpm.value,_xlpm.range),_xlfn.VSTACK(_xlpm.value,_xlpm.range)))</definedName>
+    <definedName name="CONTAINS">_xlfn.LAMBDA(_xlpm.haystack,_xlpm.needle,IF(AND(EQUAL(COUNTA(_xlpm.haystack),1),EQUAL(COUNTA(_xlpm.needle),1)),ISNUMBER(SEARCH(_xlpm.needle,_xlpm.haystack)),OR(EXACT(_xlpm.needle,_xlpm.haystack))))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(-1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
     <definedName name="EQUAL">_xlfn.LAMBDA(_xlpm.this,_xlpm.that,_xlpm.this=_xlpm.that)</definedName>
+    <definedName name="FILENAME">_xlfn.LAMBDA(_xlop.reference,CELL("filename",DEFAULT(_xlpm.reference,INDIRECT(_xlfn.CONCAT("A1")))))</definedName>
     <definedName name="FIRST">_xlfn.LAMBDA(_xlpm.range,CAR(_xlpm.range))</definedName>
     <definedName name="FIRSTLETTER">_xlfn.LAMBDA(_xlpm.text,LEFT(_xlpm.text,1))</definedName>
+    <definedName name="FIRSTWORD">_xlfn.LAMBDA(_xlpm.text,LEFT(TRIM(_xlpm.text),DECREMENT(FIND(" ",TRIM(_xlpm.text)))))</definedName>
     <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
     <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4)))</definedName>
     <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
@@ -49,6 +53,7 @@
     <definedName name="REST">_xlfn.LAMBDA(_xlpm.range,CDR(_xlpm.range))</definedName>
     <definedName name="REVERSE">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.col))))),_xlfn.MAKEARRAY(ROWS(_xlpm.range),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.row)),1)))))</definedName>
     <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cuts Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cuts Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))</definedName>
+    <definedName name="SHEETNAME">_xlfn.LAMBDA(_xlop.reference,_xlfn.LET(_xlpm.filename,FILENAME(_xlpm.reference),_xlpm.bracket_position,FIND("]",_xlpm.filename),RIGHT(_xlpm.filename,DECREMENT(LEN(_xlpm.filename),_xlpm.bracket_position))))</definedName>
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
     <definedName name="YES">TRUE</definedName>
   </definedNames>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with FOREACH
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C6045-41FE-49ED-A036-67932FF34ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADB378D-D05A-4434-99E0-07C85ED758C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10185" yWindow="2670" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
@@ -32,6 +32,7 @@
     <definedName name="FIRSTLETTER">_xlfn.LAMBDA(_xlpm.text,LEFT(_xlpm.text,1))</definedName>
     <definedName name="FIRSTWORD">_xlfn.LAMBDA(_xlpm.text,LEFT(TRIM(_xlpm.text),DECREMENT(FIND(" ",TRIM(_xlpm.text)))))</definedName>
     <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
+    <definedName name="FOREACH">_xlfn.LAMBDA(_xlpm.range,_xlpm.function_to_apply,_xlfn.MAP(_xlpm.range,_xlpm.function_to_apply))</definedName>
     <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4)))</definedName>
     <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="GTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt;= _xlpm.y,TRUE,FALSE))</definedName>
@@ -75,6 +76,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -445,12 +468,73 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921C2094-74FC-46E7-B7CC-8CA3714EA1A5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="str" cm="1">
+        <f t="array" aca="1" ref="A1:A10" ca="1">FLIPCOIN(10)</f>
+        <v>Heads</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f ca="1"/>
+        <v>Heads</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f ca="1"/>
+        <v>Heads</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with VLIST and HLIST functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADB378D-D05A-4434-99E0-07C85ED758C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3F82E9-7C0E-470E-9107-34B84985E3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="2670" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="CONTAINS">_xlfn.LAMBDA(_xlpm.haystack,_xlpm.needle,IF(AND(EQUAL(COUNTA(_xlpm.haystack),1),EQUAL(COUNTA(_xlpm.needle),1)),ISNUMBER(SEARCH(_xlpm.needle,_xlpm.haystack)),OR(EXACT(_xlpm.needle,_xlpm.haystack))))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(-1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
-    <definedName name="EQUAL">_xlfn.LAMBDA(_xlpm.this,_xlpm.that,_xlpm.this=_xlpm.that)</definedName>
+    <definedName name="EQUAL">_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm.a=_xlpm.b)</definedName>
     <definedName name="FILENAME">_xlfn.LAMBDA(_xlop.reference,CELL("filename",DEFAULT(_xlpm.reference,INDIRECT(_xlfn.CONCAT("A1")))))</definedName>
     <definedName name="FIRST">_xlfn.LAMBDA(_xlpm.range,CAR(_xlpm.range))</definedName>
     <definedName name="FIRSTLETTER">_xlfn.LAMBDA(_xlpm.text,LEFT(_xlpm.text,1))</definedName>
@@ -36,13 +36,14 @@
     <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4)))</definedName>
     <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="GTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt;= _xlpm.y,TRUE,FALSE))</definedName>
+    <definedName name="HLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.column_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.column_count,0),"()",_xlfn.MAKEARRAY(1,_xlpm.column_count,_xlfn.LAMBDA(_xlpm._row,_xlpm.col,CHOOSE(_xlpm.col,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
     <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
     <definedName name="ISHORIZONTAL">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),TRUE,FALSE))</definedName>
     <definedName name="ISVERTICAL">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(ROWS(_xlpm.range),COLUMNS(_xlpm.range)),TRUE,FALSE))</definedName>
     <definedName name="LAST">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),INDEX(_xlpm.range,1,COUNTA(_xlpm.range)),INDEX(_xlpm.range,COUNTA(_xlpm.range),1)))</definedName>
-    <definedName name="LENGTH">_xlfn.LAMBDA(_xlpm.input,IF(EQUAL(COUNTA(_xlpm.input),1),LEN(_xlpm.input),COUNTA(_xlpm.input)))</definedName>
+    <definedName name="LENGTH">_xlfn.LAMBDA(_xlpm.input,IF(EQUAL(COUNTA(_xlpm.input),1),IF(EQUAL(_xlpm.input,"()"),0,LEN(_xlpm.input)),COUNTA(_xlpm.input)))</definedName>
     <definedName name="LESSTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &lt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="LTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x&lt;=_xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="MAGIC8BALL">_xlfn.LAMBDA(_xlop.yes_or_no_question,IF(PROVIDED(_xlpm.yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered"))</definedName>
@@ -56,6 +57,7 @@
     <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cuts Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cuts Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))</definedName>
     <definedName name="SHEETNAME">_xlfn.LAMBDA(_xlop.reference,_xlfn.LET(_xlpm.filename,FILENAME(_xlpm.reference),_xlpm.bracket_position,FIND("]",_xlpm.filename),RIGHT(_xlpm.filename,DECREMENT(LEN(_xlpm.filename),_xlpm.bracket_position))))</definedName>
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
+    <definedName name="VLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.row_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.row_count,0),"()",_xlfn.MAKEARRAY(_xlpm.row_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,CHOOSE(_xlpm.row,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="YES">TRUE</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -131,8 +133,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,70 +471,73 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921C2094-74FC-46E7-B7CC-8CA3714EA1A5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="str" cm="1">
         <f t="array" aca="1" ref="A1:A10" ca="1">FLIPCOIN(10)</f>
+        <v>Tails</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f ca="1"/>
         <v>Heads</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f ca="1"/>
-        <v>Tails</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f ca="1"/>
-        <v>Tails</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f ca="1"/>
         <v>Heads</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f ca="1"/>
-        <v>Tails</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f ca="1"/>
-        <v>Tails</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with TYPESTRING, ISRANGE, ISATOM, and MEMBER functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3F82E9-7C0E-470E-9107-34B84985E3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53E6A6F-038C-4E21-9049-86D1ABAB28DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="ALL">_xlfn.LAMBDA(_xlpm.truth_values,AND(_xlpm.truth_values))</definedName>
     <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
@@ -40,13 +41,16 @@
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
     <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
+    <definedName name="ISATOM">_xlfn.LAMBDA(_xlpm.input,MEMBER(TYPESTRING(_xlpm.input),VLIST("Number","String","Error")))</definedName>
     <definedName name="ISHORIZONTAL">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),TRUE,FALSE))</definedName>
+    <definedName name="ISRANGE">_xlfn.LAMBDA(_xlpm.input,EQUAL(TYPESTRING(_xlpm.input),"Range"))</definedName>
     <definedName name="ISVERTICAL">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(ROWS(_xlpm.range),COLUMNS(_xlpm.range)),TRUE,FALSE))</definedName>
     <definedName name="LAST">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),INDEX(_xlpm.range,1,COUNTA(_xlpm.range)),INDEX(_xlpm.range,COUNTA(_xlpm.range),1)))</definedName>
     <definedName name="LENGTH">_xlfn.LAMBDA(_xlpm.input,IF(EQUAL(COUNTA(_xlpm.input),1),IF(EQUAL(_xlpm.input,"()"),0,LEN(_xlpm.input)),COUNTA(_xlpm.input)))</definedName>
     <definedName name="LESSTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &lt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="LTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x&lt;=_xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="MAGIC8BALL">_xlfn.LAMBDA(_xlop.yes_or_no_question,IF(PROVIDED(_xlpm.yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered"))</definedName>
+    <definedName name="MEMBER">_xlfn.LAMBDA(_xlpm.needle,_xlpm.haystack,OR(EXACT(_xlpm.needle, _xlpm.haystack)))</definedName>
     <definedName name="NO">FALSE</definedName>
     <definedName name="OTHERWISE">TRUE</definedName>
     <definedName name="PICK">_xlfn.LAMBDA(_xlpm._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),CHOOSE(RANDBETWEEN(1, _xlpm.count), _xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5, _xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25)))</definedName>
@@ -57,6 +61,7 @@
     <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cuts Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cuts Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))</definedName>
     <definedName name="SHEETNAME">_xlfn.LAMBDA(_xlop.reference,_xlfn.LET(_xlpm.filename,FILENAME(_xlpm.reference),_xlpm.bracket_position,FIND("]",_xlpm.filename),RIGHT(_xlpm.filename,DECREMENT(LEN(_xlpm.filename),_xlpm.bracket_position))))</definedName>
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
+    <definedName name="TYPESTRING">_xlfn.LAMBDA(_xlpm.input,_xlop.recursive,_xlfn.SWITCH(TYPE(_xlpm.input),1,"Number",2,"String",4,"Boolean",16,"Error",64,IF(DEFAULT(_xlpm.recursive,FALSE),_xlfn.MAP(_xlpm.input,_xlfn.LAMBDA(_xlpm.each,TYPESTRING(_xlpm.each))),"Range"),128,"Function",OTHERWISE,"Unknown"))</definedName>
     <definedName name="VLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.row_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.row_count,0),"()",_xlfn.MAKEARRAY(_xlpm.row_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,CHOOSE(_xlpm.row,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="YES">TRUE</definedName>
   </definedNames>
@@ -474,7 +479,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,6 +489,10 @@
         <f t="array" aca="1" ref="A1:A10" ca="1">FLIPCOIN(10)</f>
         <v>Tails</v>
       </c>
+      <c r="B1" t="str" cm="1">
+        <f t="array" aca="1" ref="B1:B10" ca="1">TYPESTRING(_xlfn.ANCHORARRAY(A1), YES)</f>
+        <v>String</v>
+      </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -491,17 +500,29 @@
         <f ca="1"/>
         <v>Tails</v>
       </c>
+      <c r="B2" t="str">
+        <f ca="1"/>
+        <v>String</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
+      <c r="B3" t="str">
+        <f ca="1"/>
+        <v>String</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
+      </c>
+      <c r="B4" t="str">
+        <f ca="1"/>
+        <v>String</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,11 +530,19 @@
         <f ca="1"/>
         <v>Tails</v>
       </c>
+      <c r="B5" t="str">
+        <f ca="1"/>
+        <v>String</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
+      </c>
+      <c r="B6" t="str">
+        <f ca="1"/>
+        <v>String</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -521,23 +550,39 @@
         <f ca="1"/>
         <v>Heads</v>
       </c>
+      <c r="B7" t="str">
+        <f ca="1"/>
+        <v>String</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
+      <c r="B8" t="str">
+        <f ca="1"/>
+        <v>String</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
+      </c>
+      <c r="B9" t="str">
+        <f ca="1"/>
+        <v>String</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
+      </c>
+      <c r="B10" t="str">
+        <f ca="1"/>
+        <v>String</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with ID function
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53E6A6F-038C-4E21-9049-86D1ABAB28DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF5E4AF-19EC-43AA-BEEC-79BDCEABE458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
@@ -38,6 +38,7 @@
     <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="GTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt;= _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="HLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.column_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.column_count,0),"()",_xlfn.MAKEARRAY(1,_xlpm.column_count,_xlfn.LAMBDA(_xlpm._row,_xlpm.col,CHOOSE(_xlpm.col,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
+    <definedName name="ID">_xlfn.LAMBDA(_xlpm.input,_xlpm.input)</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
     <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
@@ -518,7 +519,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B4" t="str">
         <f ca="1"/>
@@ -528,7 +529,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B5" t="str">
         <f ca="1"/>
@@ -568,7 +569,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B9" t="str">
         <f ca="1"/>
@@ -578,7 +579,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B10" t="str">
         <f ca="1"/>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with TRIMALL and updated ROCKPAPERSCISSORS functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF5E4AF-19EC-43AA-BEEC-79BDCEABE458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F135C196-4C18-4E95-B54E-D31B065EEF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
@@ -59,9 +59,10 @@
     <definedName name="RATIO">_xlfn.LAMBDA(_xlpm.numerator,_xlpm.denominator,_xlpm.numerator / _xlpm.denominator)</definedName>
     <definedName name="REST">_xlfn.LAMBDA(_xlpm.range,CDR(_xlpm.range))</definedName>
     <definedName name="REVERSE">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.col))))),_xlfn.MAKEARRAY(ROWS(_xlpm.range),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.row)),1)))))</definedName>
-    <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cuts Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cuts Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))</definedName>
+    <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.CONCAT(FORMAT("You threw {1}. SL threw {2}. ",_xlpm.human,_xlpm.robot),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cut Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cut Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors."))))</definedName>
     <definedName name="SHEETNAME">_xlfn.LAMBDA(_xlop.reference,_xlfn.LET(_xlpm.filename,FILENAME(_xlpm.reference),_xlpm.bracket_position,FIND("]",_xlpm.filename),RIGHT(_xlpm.filename,DECREMENT(LEN(_xlpm.filename),_xlpm.bracket_position))))</definedName>
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
+    <definedName name="TRIMALL">_xlfn.LAMBDA(_xlpm.range,_xlfn.MAKEARRAY(ROWS(_xlpm.range),COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm.row,_xlpm.col,TRIM(INDEX(_xlpm.range,_xlpm.row,_xlpm.col)))))</definedName>
     <definedName name="TYPESTRING">_xlfn.LAMBDA(_xlpm.input,_xlop.recursive,_xlfn.SWITCH(TYPE(_xlpm.input),1,"Number",2,"String",4,"Boolean",16,"Error",64,IF(DEFAULT(_xlpm.recursive,FALSE),_xlfn.MAP(_xlpm.input,_xlfn.LAMBDA(_xlpm.each,TYPESTRING(_xlpm.each))),"Range"),128,"Function",OTHERWISE,"Unknown"))</definedName>
     <definedName name="VLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.row_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.row_count,0),"()",_xlfn.MAKEARRAY(_xlpm.row_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,CHOOSE(_xlpm.row,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="YES">TRUE</definedName>
@@ -509,7 +510,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B3" t="str">
         <f ca="1"/>
@@ -519,7 +520,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B4" t="str">
         <f ca="1"/>
@@ -549,7 +550,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B7" t="str">
         <f ca="1"/>
@@ -559,7 +560,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B8" t="str">
         <f ca="1"/>

</xml_diff>

<commit_message>
Fixing minor function typos and updating pre-installed SpreadsheetLisp.xlsx workbook with APPEND, ALPHABET, DICEROLL, ROLLDICE, and FULLDECK functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F135C196-4C18-4E95-B54E-D31B065EEF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC61922-149A-4DB3-9457-FC9FB77D085A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
+    <workbookView xWindow="10185" yWindow="2670" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="ALL">_xlfn.LAMBDA(_xlpm.truth_values,AND(_xlpm.truth_values))</definedName>
+    <definedName name="ALPHABET">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.alphabet,_xlfn.HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(_xlpm.vertical,NO),TRANSPOSE(_xlpm.alphabet),_xlpm.alphabet)))</definedName>
+    <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
     <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
@@ -27,6 +29,7 @@
     <definedName name="CONTAINS">_xlfn.LAMBDA(_xlpm.haystack,_xlpm.needle,IF(AND(EQUAL(COUNTA(_xlpm.haystack),1),EQUAL(COUNTA(_xlpm.needle),1)),ISNUMBER(SEARCH(_xlpm.needle,_xlpm.haystack)),OR(EXACT(_xlpm.needle,_xlpm.haystack))))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(-1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
+    <definedName name="DICEROLL">_xlfn.LAMBDA(PICK(1,2,3,4,5,6))</definedName>
     <definedName name="EQUAL">_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm.a=_xlpm.b)</definedName>
     <definedName name="FILENAME">_xlfn.LAMBDA(_xlop.reference,CELL("filename",DEFAULT(_xlpm.reference,INDIRECT(_xlfn.CONCAT("A1")))))</definedName>
     <definedName name="FIRST">_xlfn.LAMBDA(_xlpm.range,CAR(_xlpm.range))</definedName>
@@ -35,6 +38,7 @@
     <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
     <definedName name="FOREACH">_xlfn.LAMBDA(_xlpm.range,_xlpm.function_to_apply,_xlfn.MAP(_xlpm.range,_xlpm.function_to_apply))</definedName>
     <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4)))</definedName>
+    <definedName name="FULLDECK">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.full_deck,_xlfn.HSTACK({"AS","KS","QS","JS","XS","9S","8S","7S","6S","5S","4S","3S","2S"},{"AH","KH","QH","JH","XH","9H","8H","7H","6H","5H","4H","3H","2H"},{"AD","KD","QD","JD","XD","9D","8D","7D","6D","5D","4D","3D","2D"},{"AC","KC","QC","JC","XC","9C","8C","7C","6C","5C","4C","3C","2C"}),IF(DEFAULT(_xlpm.vertical,FALSE),TRANSPOSE(_xlpm.full_deck),_xlpm.full_deck)))</definedName>
     <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="GTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt;= _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="HLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.column_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.column_count,0),"()",_xlfn.MAKEARRAY(1,_xlpm.column_count,_xlfn.LAMBDA(_xlpm._row,_xlpm.col,CHOOSE(_xlpm.col,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
@@ -60,6 +64,7 @@
     <definedName name="REST">_xlfn.LAMBDA(_xlpm.range,CDR(_xlpm.range))</definedName>
     <definedName name="REVERSE">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.col))))),_xlfn.MAKEARRAY(ROWS(_xlpm.range),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.row)),1)))))</definedName>
     <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.CONCAT(FORMAT("You threw {1}. SL threw {2}. ",_xlpm.human,_xlpm.robot),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cut Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cut Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors."))))</definedName>
+    <definedName name="ROLLDICE">_xlfn.LAMBDA(_xlop.times,IF(LTE(DEFAULT(_xlpm.times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(_xlpm.times)))))</definedName>
     <definedName name="SHEETNAME">_xlfn.LAMBDA(_xlop.reference,_xlfn.LET(_xlpm.filename,FILENAME(_xlpm.reference),_xlpm.bracket_position,FIND("]",_xlpm.filename),RIGHT(_xlpm.filename,DECREMENT(LEN(_xlpm.filename),_xlpm.bracket_position))))</definedName>
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
     <definedName name="TRIMALL">_xlfn.LAMBDA(_xlpm.range,_xlfn.MAKEARRAY(ROWS(_xlpm.range),COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm.row,_xlpm.col,TRIM(INDEX(_xlpm.range,_xlpm.row,_xlpm.col)))))</definedName>
@@ -68,6 +73,7 @@
     <definedName name="YES">TRUE</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,10 +115,188 @@
 </metadata>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+  <si>
+    <t>DEFINE(ALL,LAMBDA(truth_values,AND(truth_values)))</t>
+  </si>
+  <si>
+    <t>DEFINE(OTHERWISE,TRUE)</t>
+  </si>
+  <si>
+    <t>DEFINE(NO,FALSE)</t>
+  </si>
+  <si>
+    <t>DEFINE(YES,TRUE)</t>
+  </si>
+  <si>
+    <t>DEFINE(CAPITALIZE,LAMBDA(text,CONCAT(UPPER(FIRSTLETTER(text)),RIGHT(text, DECREMENT(LEN(text))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(CAR,LAMBDA(range,INDEX(range,1,1)))</t>
+  </si>
+  <si>
+    <t>DEFINE(CASE,LAMBDA(_1a, _1b, [_2a], [_2b], [_3a], [_3b], [_4a], [_4b], [_5a], [_5b],[_6a], [_6b], [_7a], [_7b], [_8a], [_8b], [_9a], [_9b], [_10a], [_10b],LET(case1,EQUAL(_1a, _1b),case2,IFOMITTED(_2a, TRUE, EQUAL(_2a, _2b)),case3,IFOMITTED(_3a, TRUE, EQUAL(_3a, _3b)),case4,IFOMITTED(_4a, TRUE, EQUAL(_4a, _4b)),case5,IFOMITTED(_5a, TRUE, EQUAL(_5a, _5b)),case6,IFOMITTED(_6a, TRUE, EQUAL(_6a, _6b)),case7,IFOMITTED(_7a, TRUE, EQUAL(_7a, _7b)),case8,IFOMITTED(_8a, TRUE, EQUAL(_8a, _8b)),case9,IFOMITTED(_9a, TRUE, EQUAL(_9a, _9b)),case10,IFOMITTED(_10a, TRUE, EQUAL(_10a, _10b)),AND(case1,case2,case3,case4,case5,case6,case7,case8,case9,case10))))</t>
+  </si>
+  <si>
+    <t>DEFINE(CELLNAME,LAMBDA([reference],[absolute],LET(address,IFOMITTED(reference,CELL("address"),CELL("address",reference)),display_absolute,DEFAULT(absolute,NO),IF(display_absolute,address,SUBSTITUTE(address,"$","")))))</t>
+  </si>
+  <si>
+    <t>DEFINE(CDR,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),MAKEARRAY(1,DECREMENT(COLUMNS(range)),LAMBDA(_row,col,INDEX(range,1,INCREMENT(col)))),MAKEARRAY(DECREMENT(ROWS(range)),1,LAMBDA(row,_col,INDEX(range,INCREMENT(row),1))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(COINTOSS,LAMBDA(PICK("Heads","Tails")))</t>
+  </si>
+  <si>
+    <t>DEFINE(CONS,LAMBDA(value,range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),HSTACK(value,range),VSTACK(value,range))))</t>
+  </si>
+  <si>
+    <t>DEFINE(CONTAINS,LAMBDA(haystack,needle,IF(AND(EQUAL(COUNTA(haystack),1),EQUAL(COUNTA(needle),1)),ISNUMBER(SEARCH(needle,haystack)),OR(EXACT(needle,haystack)))))</t>
+  </si>
+  <si>
+    <t>DEFINE(DECREMENT,LAMBDA(x,[times],SUM(x,PRODUCT(-1,DEFAULT(times,1)))))</t>
+  </si>
+  <si>
+    <t>DEFINE(DEFAULT,LAMBDA(optional_argument,fallback_value,IF(PROVIDED(optional_argument),optional_argument,fallback_value)))</t>
+  </si>
+  <si>
+    <t>DEFINE(EQUAL,LAMBDA(a,b,a=b))</t>
+  </si>
+  <si>
+    <t>DEFINE(FILENAME,LAMBDA([reference],CELL("filename",DEFAULT(reference,INDIRECT(CONCAT("A1"))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(FIRST,LAMBDA(range,CAR(range)))</t>
+  </si>
+  <si>
+    <t>DEFINE(FIRSTLETTER,LAMBDA(text,LEFT(text,1)))</t>
+  </si>
+  <si>
+    <t>DEFINE(FIRSTWORD,LAMBDA(text,LEFT(TRIM(text),DECREMENT(FIND(" ",TRIM(text))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(FLIPCOIN,LAMBDA([times],LET(counter,DEFAULT(times, 1),IF(LTE(counter, 1),COINTOSS(),VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(counter)))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(FOREACH,LAMBDA(range,function_to_apply,MAP(range,function_to_apply)))</t>
+  </si>
+  <si>
+    <t>DEFINE(FORMAT,LAMBDA(template_text,first_value,[second_value],[third_value],[fourth_value],[fifth_value],LET(_after1,SUBSTITUTE(template_text,"{1}", first_value),_after2,IF(PROVIDED(second_value),SUBSTITUTE(_after1,"{2}", second_value),_after1),_after3,IF(PROVIDED(third_value),SUBSTITUTE(_after2,"{3}", third_value),_after2),_after4,IF(PROVIDED(fourth_value),SUBSTITUTE(_after3,"{4}", fourth_value),_after3),IF(PROVIDED(fifth_value),SUBSTITUTE(_after4,"{5}", fifth_value),_after4))))</t>
+  </si>
+  <si>
+    <t>DEFINE(GREATERTHAN,LAMBDA(x,y,IF(x &gt; y,TRUE,FALSE)))</t>
+  </si>
+  <si>
+    <t>DEFINE(GTE,LAMBDA(x,y,IF(x &gt;= y,TRUE,FALSE)))</t>
+  </si>
+  <si>
+    <t>DEFINE(HLIST,LAMBDA([_1], [_2], [_3], [_4], [_5],[_6], [_7], [_8], [_9], [_10],[_11], [_12], [_13], [_14], [_15],[_16], [_17], [_18], [_19], [_20],[_21], [_22], [_23], [_24], [_25],LET(column_count,SUM(IS(_1), IS(_2), IS(_3), IS(_4), IS(_5),IS(_6), IS(_7), IS(_8), IS(_9), IS(_10),IS(_11), IS(_12), IS(_13), IS(_14), IS(_15),IS(_16), IS(_17), IS(_18), IS(_19), IS(_20),IS(_21), IS(_22), IS(_23), IS(_24), IS(_25)),IF(EQUAL(column_count,0),"()",MAKEARRAY(1,column_count,LAMBDA(_row,col,CHOOSE(col,_1, _2, _3, _4, _5,_6, _7, _8, _9, _10,_11, _12, _13, _14, _15,_16, _17, _18, _19, _20,_21, _22, _23, _24, _25)))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(ID,LAMBDA(input,input))</t>
+  </si>
+  <si>
+    <t>DEFINE(IFOMITTED,LAMBDA(optional_argument,value_if_omitted,value_if_provided,IF(ISOMITTED(optional_argument),value_if_omitted,value_if_provided)))</t>
+  </si>
+  <si>
+    <t>DEFINE(INCREMENT,LAMBDA(x,[times],SUM(x,PRODUCT(1,DEFAULT(times,1)))))</t>
+  </si>
+  <si>
+    <t>DEFINE(IS,LAMBDA(argument,IF(ISOMITTED(argument), 0, 1)))</t>
+  </si>
+  <si>
+    <t>DEFINE(ISATOM,LAMBDA(input,MEMBER(TYPESTRING(input),VLIST("Number","String","Error"))))</t>
+  </si>
+  <si>
+    <t>DEFINE(ISHORIZONTAL,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),TRUE,FALSE)))</t>
+  </si>
+  <si>
+    <t>DEFINE(ISRANGE,LAMBDA(input,EQUAL(TYPESTRING(input),"Range")))</t>
+  </si>
+  <si>
+    <t>DEFINE(ISVERTICAL,LAMBDA(range,IF(GREATERTHAN(ROWS(range),COLUMNS(range)),TRUE,FALSE)))</t>
+  </si>
+  <si>
+    <t>DEFINE(LAST,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),INDEX(range,1,COUNTA(range)),INDEX(range,COUNTA(range),1))))</t>
+  </si>
+  <si>
+    <t>DEFINE(LENGTH,LAMBDA(input,IF(EQUAL(COUNTA(input),1),IF(EQUAL(input,"()"),0,LEN(input)),COUNTA(input))))</t>
+  </si>
+  <si>
+    <t>DEFINE(LESSTHAN,LAMBDA(x,y,IF(x &lt; y,TRUE,FALSE)))</t>
+  </si>
+  <si>
+    <t>DEFINE(LTE,LAMBDA(x,y,IF(x&lt;=y,TRUE,FALSE)))</t>
+  </si>
+  <si>
+    <t>DEFINE(MAGIC8BALL,LAMBDA([yes_or_no_question],IF(PROVIDED(yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered")))</t>
+  </si>
+  <si>
+    <t>DEFINE(MEMBER,LAMBDA(needle,haystack,OR(EXACT(needle, haystack))))</t>
+  </si>
+  <si>
+    <t>DEFINE(RATIO,LAMBDA(numerator,denominator,numerator / denominator))</t>
+  </si>
+  <si>
+    <t>DEFINE(REST,LAMBDA(range,CDR(range)))</t>
+  </si>
+  <si>
+    <t>DEFINE(REVERSE,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),MAKEARRAY(1,COLUMNS(range),LAMBDA(_row,col,INDEX(range,1,DECREMENT(LENGTH(range),DECREMENT(col))))),MAKEARRAY(ROWS(range),1,LAMBDA(row,_col,INDEX(range,DECREMENT(LENGTH(range),DECREMENT(row)),1))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(ROCKPAPERSCISSORS,LAMBDA(throw,LET(human,CAPITALIZE(LOWER(DEFAULT(throw,""))),robot,PICK("Rock","Paper","Scissors"),CONCAT(FORMAT("You threw {1}. SL threw {2}. ",human,robot),IFS(CASE(human,robot),FORMAT("It's a tie! {1} vs. {1}",human),CASE(human,"Paper",robot,"Rock"),"You win! Paper covers Rock.",CASE(human,"Paper",robot,"Scissors"),"You lose! Scissors cut Paper.",CASE(human,"Rock",robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(human,"Rock",robot,"Paper"),"You lose! Paper covers Rock.",CASE(human,"Scissors",robot,"Paper"),"You win! Scissors cut Paper.",CASE(human,"Scissors",robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))))</t>
+  </si>
+  <si>
+    <t>DEFINE(PICK,LAMBDA(_1, [_2], [_3], [_4], [_5],[_6], [_7], [_8], [_9], [_10],[_11], [_12], [_13], [_14], [_15],[_16], [_17], [_18], [_19], [_20],[_21], [_22], [_23], [_24], [_25],LET(count,SUM(IS(_1), IS(_2), IS(_3), IS(_4), IS(_5),IS(_6), IS(_7), IS(_8), IS(_9), IS(_10),IS(_11), IS(_12), IS(_13), IS(_14), IS(_15),IS(_16), IS(_17), IS(_18), IS(_19), IS(_20),IS(_21), IS(_22), IS(_23), IS(_24), IS(_25)),CHOOSE(RANDBETWEEN(1, count), _1, _2, _3, _4, _5, _6, _7, _8, _9, _10,_11, _12, _13, _14, _15,_16, _17, _18, _19, _20,_21, _22, _23, _24, _25))))</t>
+  </si>
+  <si>
+    <t>DEFINE(PROVIDED,LAMBDA([argument],NOT(ISOMITTED(argument))))</t>
+  </si>
+  <si>
+    <t>DEFINE(SHEETNAME,LAMBDA([reference],LET(filename,FILENAME(reference),bracket_position,FIND("]",filename),RIGHT(filename,DECREMENT(LEN(filename),bracket_position)))))</t>
+  </si>
+  <si>
+    <t>DEFINE(SQUAREROOT,LAMBDA(x,POWER(x,0.5)))</t>
+  </si>
+  <si>
+    <t>DEFINE(TRIMALL,LAMBDA(range,MAKEARRAY(ROWS(range),COLUMNS(range),LAMBDA(row,col,TRIM(INDEX(range,row,col))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(TYPESTRING,LAMBDA(input,[recursive],SWITCH(TYPE(input),1,"Number",2,"String",4,"Boolean",16,"Error",64,IF(DEFAULT(recursive,FALSE),MAP(input,LAMBDA(each,TYPESTRING(each))),"Range"),128,"Function",OTHERWISE,"Unknown")))</t>
+  </si>
+  <si>
+    <t>DEFINE(VLIST,LAMBDA([_1], [_2], [_3], [_4], [_5],[_6], [_7], [_8], [_9], [_10],[_11], [_12], [_13], [_14], [_15],[_16], [_17], [_18], [_19], [_20],[_21], [_22], [_23], [_24], [_25],LET(row_count,SUM(IS(_1), IS(_2), IS(_3), IS(_4), IS(_5),IS(_6), IS(_7), IS(_8), IS(_9), IS(_10),IS(_11), IS(_12), IS(_13), IS(_14), IS(_15),IS(_16), IS(_17), IS(_18), IS(_19), IS(_20),IS(_21), IS(_22), IS(_23), IS(_24), IS(_25)),IF(EQUAL(row_count,0),"()",MAKEARRAY(row_count,1,LAMBDA(row,_col,CHOOSE(row,_1, _2, _3, _4, _5,_6, _7, _8, _9, _10,_11, _12, _13, _14, _15,_16, _17, _18, _19, _20,_21, _22, _23, _24, _25)))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(ALPHABET,LAMBDA([vertical],LET(alphabet,HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(vertical,NO),TRANSPOSE(alphabet),alphabet))))</t>
+  </si>
+  <si>
+    <t>DEFINE(APPEND,LAMBDA(head,body,IF(GREATERTHAN(COLUMNS(body),ROWS(body)),HSTACK(head,body),VSTACK(head,body))))</t>
+  </si>
+  <si>
+    <t>DEFINE(DICEROLL,LAMBDA(PICK(1,2,3,4,5,6)))</t>
+  </si>
+  <si>
+    <t>DEFINE(FULLDECK,LAMBDA([vertical],LET(full_deck,HSTACK({"AS","KS","QS","JS","XS","9S","8S","7S","6S","5S","4S","3S","2S"},{"AH","KH","QH","JH","XH","9H","8H","7H","6H","5H","4H","3H","2H"},{"AD","KD","QD","JD","XD","9D","8D","7D","6D","5D","4D","3D","2D"},{"AC","KC","QC","JC","XC","9C","8C","7C","6C","5C","4C","3C","2C"}),IF(DEFAULT(vertical,FALSE),TRANSPOSE(full_deck),full_deck))))</t>
+  </si>
+  <si>
+    <t>DEFINE(ROLLDICE,LAMBDA([times],IF(LTE(DEFAULT(times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(times))))))</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -140,9 +324,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,13 +663,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921C2094-74FC-46E7-B7CC-8CA3714EA1A5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="str" cm="1">
@@ -495,7 +681,9 @@
         <f t="array" aca="1" ref="B1:B10" ca="1">TYPESTRING(_xlfn.ANCHORARRAY(A1), YES)</f>
         <v>String</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
@@ -510,17 +698,20 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B3" t="str">
         <f ca="1"/>
         <v>String</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B4" t="str">
         <f ca="1"/>
@@ -530,11 +721,14 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B5" t="str">
         <f ca="1"/>
         <v>String</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,6 +750,9 @@
         <f ca="1"/>
         <v>String</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
@@ -576,6 +773,9 @@
         <f ca="1"/>
         <v>String</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
@@ -585,6 +785,256 @@
       <c r="B10" t="str">
         <f ca="1"/>
         <v>String</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with ARITY, APPLY, and TEXTBETWEEN functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC61922-149A-4DB3-9457-FC9FB77D085A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580A83BC-BB47-4BE0-A67A-EBA8D02AB4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="2670" windowWidth="38700" windowHeight="15885" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <definedName name="ALL">_xlfn.LAMBDA(_xlpm.truth_values,AND(_xlpm.truth_values))</definedName>
     <definedName name="ALPHABET">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.alphabet,_xlfn.HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(_xlpm.vertical,NO),TRANSPOSE(_xlpm.alphabet),_xlpm.alphabet)))</definedName>
     <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
+    <definedName name="APPLY">_xlfn.LAMBDA(_xlpm.function,_xlop.argument1,_xlop.argument2,_xlop.argument3,_xlop.argument4,_xlop.argument5,_xlop.argument6,_xlop.argument7,_xlop.argument8,_xlop.argument9,_xlop.argument10,_xlfn.SWITCH(ARITY(_xlpm.argument1,_xlpm.argument2,_xlpm.argument3,_xlpm.argument4,_xlpm.argument5,_xlpm.argument6,_xlpm.argument7,_xlpm.argument8,_xlpm.argument9,_xlpm.argument10),1,_xlpm.function(_xlpm.argument1),2,_xlpm.function(_xlpm.argument1, _xlpm.argument2),3,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3),4,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4),5,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5),6,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6),7,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7),8,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8),9,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9),10,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9, _xlpm.argument10),OTHERWISE,_xlpm.function()))</definedName>
+    <definedName name="ARITY">_xlfn.LAMBDA(_xlop._arg1,_xlop._arg2,_xlop._arg3,_xlop._arg4,_xlop._arg5,_xlop._arg6,_xlop._arg7,_xlop._arg8,_xlop._arg9,_xlop._arg10,_xlop._arg11,_xlop._arg12,_xlop._arg13,_xlop._arg14,_xlop._arg15,_xlop._arg16,_xlop._arg17,_xlop._arg18,_xlop._arg19,_xlop._arg20,_xlop._arg21,_xlop._arg22,_xlop._arg23,_xlop._arg24,_xlop._arg25,SUM(IS(_xlpm._arg1), IS(_xlpm._arg2), IS(_xlpm._arg3), IS(_xlpm._arg4), IS(_xlpm._arg5),IS(_xlpm._arg6), IS(_xlpm._arg7), IS(_xlpm._arg8), IS(_xlpm._arg9), IS(_xlpm._arg10),IS(_xlpm._arg11), IS(_xlpm._arg12), IS(_xlpm._arg13), IS(_xlpm._arg14), IS(_xlpm._arg15),IS(_xlpm._arg16), IS(_xlpm._arg17), IS(_xlpm._arg18), IS(_xlpm._arg19), IS(_xlpm._arg20),IS(_xlpm._arg21), IS(_xlpm._arg22), IS(_xlpm._arg23), IS(_xlpm._arg24), IS(_xlpm._arg25)))</definedName>
     <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
@@ -30,6 +32,7 @@
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(-1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
     <definedName name="DICEROLL">_xlfn.LAMBDA(PICK(1,2,3,4,5,6))</definedName>
+    <definedName name="DIFFERENCE">_xlfn.LAMBDA(_xlpm.minuend,_xlpm.subtrahend,_xlpm.minuend-_xlpm.subtrahend)</definedName>
     <definedName name="EQUAL">_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm.a=_xlpm.b)</definedName>
     <definedName name="FILENAME">_xlfn.LAMBDA(_xlop.reference,CELL("filename",DEFAULT(_xlpm.reference,INDIRECT(_xlfn.CONCAT("A1")))))</definedName>
     <definedName name="FIRST">_xlfn.LAMBDA(_xlpm.range,CAR(_xlpm.range))</definedName>
@@ -37,12 +40,13 @@
     <definedName name="FIRSTWORD">_xlfn.LAMBDA(_xlpm.text,LEFT(TRIM(_xlpm.text),DECREMENT(FIND(" ",TRIM(_xlpm.text)))))</definedName>
     <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
     <definedName name="FOREACH">_xlfn.LAMBDA(_xlpm.range,_xlpm.function_to_apply,_xlfn.MAP(_xlpm.range,_xlpm.function_to_apply))</definedName>
-    <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4)))</definedName>
+    <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlop.sixth_value,_xlop.seventh_value,_xlop.eigth_value,_xlop.ninth_value,_xlop.tenth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),_xlpm._after5,IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4),_xlpm._after6,IF(PROVIDED(_xlpm.sixth_value),SUBSTITUTE(_xlpm._after5,"{6}", _xlpm.sixth_value),_xlpm._after5),_xlpm._after7,IF(PROVIDED(_xlpm.seventh_value),SUBSTITUTE(_xlpm._after6,"{7}", _xlpm.seventh_value),_xlpm._after6),_xlpm._after8,IF(PROVIDED(_xlpm.eigth_value),SUBSTITUTE(_xlpm._after7,"{8}", _xlpm.eigth_value),_xlpm._after7),_xlpm._after9,IF(PROVIDED(_xlpm.ninth_value),SUBSTITUTE(_xlpm._after8,"{9}", _xlpm.ninth_value),_xlpm._after8),IF(PROVIDED(_xlpm.tenth_value),SUBSTITUTE(_xlpm._after9,"{10}", _xlpm.tenth_value),_xlpm._after9)))</definedName>
     <definedName name="FULLDECK">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.full_deck,_xlfn.HSTACK({"AS","KS","QS","JS","XS","9S","8S","7S","6S","5S","4S","3S","2S"},{"AH","KH","QH","JH","XH","9H","8H","7H","6H","5H","4H","3H","2H"},{"AD","KD","QD","JD","XD","9D","8D","7D","6D","5D","4D","3D","2D"},{"AC","KC","QC","JC","XC","9C","8C","7C","6C","5C","4C","3C","2C"}),IF(DEFAULT(_xlpm.vertical,FALSE),TRANSPOSE(_xlpm.full_deck),_xlpm.full_deck)))</definedName>
     <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="GTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt;= _xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="HLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.column_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.column_count,0),"()",_xlfn.MAKEARRAY(1,_xlpm.column_count,_xlfn.LAMBDA(_xlpm._row,_xlpm.col,CHOOSE(_xlpm.col,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="ID">_xlfn.LAMBDA(_xlpm.input,_xlpm.input)</definedName>
+    <definedName name="IFBLANK">_xlfn.LAMBDA(_xlpm.cell_reference,_xlpm.value_if_blank,_xlop.value_if_not_blank,IF(OR(ISBLANK(_xlpm.cell_reference),EQUAL(_xlpm.cell_reference,""),_xlpm.value_if_blank,DEFAULT(_xlpm.value_if_not_blank, _xlpm.cell_reference))))</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
     <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
@@ -60,6 +64,7 @@
     <definedName name="OTHERWISE">TRUE</definedName>
     <definedName name="PICK">_xlfn.LAMBDA(_xlpm._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),CHOOSE(RANDBETWEEN(1, _xlpm.count), _xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5, _xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25)))</definedName>
     <definedName name="PROVIDED">_xlfn.LAMBDA(_xlop.argument,NOT(_xlfn.ISOMITTED(_xlpm.argument)))</definedName>
+    <definedName name="QUESTION">_xlfn.LAMBDA(_xlpm.knowledgebase,_xlpm.fragment1,_xlop.fragment2,_xlop.fragment3,_xlop.fragment4,_xlop.fragment5,_xlop.fragment6,_xlop.fragment7,_xlop.fragment8,_xlop.fragment9,_xlop.fragment10,_xlfn.LET(_xlpm.arity,ARITY(_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10),_xlpm.template,CHOOSE(_xlpm.arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),_xlpm.subject,_xlpm.fragment2,_xlpm.question_word,LOWER(_xlpm.fragment1),CONTAINS(_xlpm.knowledgebase,FORMAT(_xlpm.template,_xlpm.subject,_xlpm.question_word,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10))))</definedName>
     <definedName name="RATIO">_xlfn.LAMBDA(_xlpm.numerator,_xlpm.denominator,_xlpm.numerator / _xlpm.denominator)</definedName>
     <definedName name="REST">_xlfn.LAMBDA(_xlpm.range,CDR(_xlpm.range))</definedName>
     <definedName name="REVERSE">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.col))))),_xlfn.MAKEARRAY(ROWS(_xlpm.range),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.row)),1)))))</definedName>
@@ -67,6 +72,8 @@
     <definedName name="ROLLDICE">_xlfn.LAMBDA(_xlop.times,IF(LTE(DEFAULT(_xlpm.times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(_xlpm.times)))))</definedName>
     <definedName name="SHEETNAME">_xlfn.LAMBDA(_xlop.reference,_xlfn.LET(_xlpm.filename,FILENAME(_xlpm.reference),_xlpm.bracket_position,FIND("]",_xlpm.filename),RIGHT(_xlpm.filename,DECREMENT(LEN(_xlpm.filename),_xlpm.bracket_position))))</definedName>
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
+    <definedName name="STATEMENT">_xlfn.LAMBDA(_xlpm.fragment1,_xlop.fragment2,_xlop.fragment3,_xlop.fragment4,_xlop.fragment5,_xlop.fragment6,_xlop.fragment7,_xlop.fragment8,_xlop.fragment9,_xlop.fragment10,_xlfn.LET(_xlpm.arity,ARITY(_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10),_xlpm.template,CHOOSE(_xlpm.arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),FORMAT(_xlpm.template,_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10)))</definedName>
+    <definedName name="TEXTBETWEEN">_xlfn.LAMBDA(_xlpm.source_text,_xlpm.first_boundary,_xlpm.second_boundary,_xlfn.LET(_xlpm.text_after_first_boundary,RIGHT(_xlpm.source_text,DIFFERENCE(LEN(_xlpm.source_text),DECREMENT(SUM(FIND(_xlpm.first_boundary,_xlpm.source_text),LEN(_xlpm.first_boundary))))),LEFT(_xlpm.text_after_first_boundary,DECREMENT(FIND(_xlpm.second_boundary,_xlpm.text_after_first_boundary)))))</definedName>
     <definedName name="TRIMALL">_xlfn.LAMBDA(_xlpm.range,_xlfn.MAKEARRAY(ROWS(_xlpm.range),COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm.row,_xlpm.col,TRIM(INDEX(_xlpm.range,_xlpm.row,_xlpm.col)))))</definedName>
     <definedName name="TYPESTRING">_xlfn.LAMBDA(_xlpm.input,_xlop.recursive,_xlfn.SWITCH(TYPE(_xlpm.input),1,"Number",2,"String",4,"Boolean",16,"Error",64,IF(DEFAULT(_xlpm.recursive,FALSE),_xlfn.MAP(_xlpm.input,_xlfn.LAMBDA(_xlpm.each,TYPESTRING(_xlpm.each))),"Range"),128,"Function",OTHERWISE,"Unknown"))</definedName>
     <definedName name="VLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.row_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.row_count,0),"()",_xlfn.MAKEARRAY(_xlpm.row_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,CHOOSE(_xlpm.row,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
@@ -116,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>DEFINE(ALL,LAMBDA(truth_values,AND(truth_values)))</t>
   </si>
@@ -181,9 +188,6 @@
     <t>DEFINE(FOREACH,LAMBDA(range,function_to_apply,MAP(range,function_to_apply)))</t>
   </si>
   <si>
-    <t>DEFINE(FORMAT,LAMBDA(template_text,first_value,[second_value],[third_value],[fourth_value],[fifth_value],LET(_after1,SUBSTITUTE(template_text,"{1}", first_value),_after2,IF(PROVIDED(second_value),SUBSTITUTE(_after1,"{2}", second_value),_after1),_after3,IF(PROVIDED(third_value),SUBSTITUTE(_after2,"{3}", third_value),_after2),_after4,IF(PROVIDED(fourth_value),SUBSTITUTE(_after3,"{4}", fourth_value),_after3),IF(PROVIDED(fifth_value),SUBSTITUTE(_after4,"{5}", fifth_value),_after4))))</t>
-  </si>
-  <si>
     <t>DEFINE(GREATERTHAN,LAMBDA(x,y,IF(x &gt; y,TRUE,FALSE)))</t>
   </si>
   <si>
@@ -281,14 +285,49 @@
   </si>
   <si>
     <t>DEFINE(ROLLDICE,LAMBDA([times],IF(LTE(DEFAULT(times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(times))))))</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>DEFINE(APPLY,LAMBDA(function,[argument1],[argument2],[argument3],[argument4],[argument5],[argument6],[argument7],[argument8],[argument9],[argument10],SWITCH(ARITY(argument1,argument2,argument3,argument4,argument5,argument6,argument7,argument8,argument9,argument10),1,function(argument1),2,function(argument1, argument2),3,function(argument1, argument2, argument3),4,function(argument1, argument2, argument3, argument4),5,function(argument1, argument2, argument3, argument4, argument5),6,function(argument1, argument2, argument3, argument4, argument5, argument6),7,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7),8,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8),9,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9),10,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9, argument10),OTHERWISE,function())))</t>
+  </si>
+  <si>
+    <t>DEFINE(ARITY,LAMBDA([_arg1], [_arg2], [_arg3], [_arg4], [_arg5],[_arg6], [_arg7], [_arg8], [_arg9], [_arg10],[_arg11], [_arg12], [_arg13], [_arg14], [_arg15],[_arg16], [_arg17], [_arg18], [_arg19], [_arg20],[_arg21], [_arg22], [_arg23], [_arg24], [_arg25],SUM(IS(_arg1), IS(_arg2), IS(_arg3), IS(_arg4), IS(_arg5),IS(_arg6), IS(_arg7), IS(_arg8), IS(_arg9), IS(_arg10),IS(_arg11), IS(_arg12), IS(_arg13), IS(_arg14), IS(_arg15),IS(_arg16), IS(_arg17), IS(_arg18), IS(_arg19), IS(_arg20),IS(_arg21), IS(_arg22), IS(_arg23), IS(_arg24), IS(_arg25))))</t>
+  </si>
+  <si>
+    <t>DEFINE(DIFFERENCE,LAMBDA(minuend,subtrahend,minuend-subtrahend))</t>
+  </si>
+  <si>
+    <t>DEFINE(FORMAT,LAMBDA(template_text,first_value,[second_value],[third_value],[fourth_value],[fifth_value],[sixth_value],[seventh_value],[eigth_value],[ninth_value],[tenth_value],LET(_after1,SUBSTITUTE(template_text,"{1}", first_value),_after2,IF(PROVIDED(second_value),SUBSTITUTE(_after1,"{2}", second_value),_after1),_after3,IF(PROVIDED(third_value),SUBSTITUTE(_after2,"{3}", third_value),_after2),_after4,IF(PROVIDED(fourth_value),SUBSTITUTE(_after3,"{4}", fourth_value),_after3),_after5,IF(PROVIDED(fifth_value),SUBSTITUTE(_after4,"{5}", fifth_value),_after4),_after6,IF(PROVIDED(sixth_value),SUBSTITUTE(_after5,"{6}", sixth_value),_after5),_after7,IF(PROVIDED(seventh_value),SUBSTITUTE(_after6,"{7}", seventh_value),_after6),_after8,IF(PROVIDED(eigth_value),SUBSTITUTE(_after7,"{8}", eigth_value),_after7),_after9,IF(PROVIDED(ninth_value),SUBSTITUTE(_after8,"{9}", ninth_value),_after8),IF(PROVIDED(tenth_value),SUBSTITUTE(_after9,"{10}", tenth_value),_after9))))</t>
+  </si>
+  <si>
+    <t>DEFINE(IFBLANK,LAMBDA(cell_reference,value_if_blank,[value_if_not_blank],IF(OR(ISBLANK(cell_reference),EQUAL(cell_reference,""),value_if_blank,DEFAULT(value_if_not_blank, cell_reference)))))</t>
+  </si>
+  <si>
+    <t>DEFINE(QUESTION,LAMBDA(knowledgebase,fragment1,[fragment2],[fragment3],[fragment4],[fragment5],[fragment6],[fragment7],[fragment8],[fragment9],[fragment10],LET(arity,ARITY(fragment1,fragment2,fragment3,fragment4,fragment5,fragment6,fragment7,fragment8,fragment9,fragment10),template,CHOOSE(arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),subject,fragment2,question_word,LOWER(fragment1),CONTAINS(knowledgebase,FORMAT(template,subject,question_word,fragment3,fragment4,fragment5,fragment6,fragment7,fragment8,fragment9,fragment10)))))</t>
+  </si>
+  <si>
+    <t>DEFINE(STATEMENT,LAMBDA(fragment1,[fragment2],[fragment3],[fragment4],[fragment5],[fragment6],[fragment7],[fragment8],[fragment9],[fragment10],LET(arity,ARITY(fragment1,fragment2,fragment3,fragment4,fragment5,fragment6,fragment7,fragment8,fragment9,fragment10),template,CHOOSE(arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),FORMAT(template,fragment1,fragment2,fragment3,fragment4,fragment5,fragment6,fragment7,fragment8,fragment9,fragment10))))</t>
+  </si>
+  <si>
+    <t>DEFINE(TEXTBETWEEN,LAMBDA(source_text,first_boundary,second_boundary,LET(text_after_first_boundary,RIGHT(source_text,DIFFERENCE(LEN(source_text),DECREMENT(SUM(FIND(first_boundary,source_text),LEN(first_boundary))))),LEFT(text_after_first_boundary,DECREMENT(FIND(second_boundary,text_after_first_boundary))))))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -324,10 +363,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,50 +704,63 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921C2094-74FC-46E7-B7CC-8CA3714EA1A5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="str" cm="1">
         <f t="array" aca="1" ref="A1:A10" ca="1">FLIPCOIN(10)</f>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B1" t="str" cm="1">
         <f t="array" aca="1" ref="B1:B10" ca="1">TYPESTRING(_xlfn.ANCHORARRAY(A1), YES)</f>
         <v>String</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
+      <c r="C1" t="str" cm="1">
+        <f t="array" aca="1" ref="C1:C10" ca="1">FOREACH(_xlfn.ANCHORARRAY(A1), _xleta.UPPER)</f>
+        <v>HEADS</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B2" t="str">
         <f ca="1"/>
         <v>String</v>
+      </c>
+      <c r="C2" t="str">
+        <f ca="1"/>
+        <v>HEADS</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B3" t="str">
         <f ca="1"/>
         <v>String</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="C3" t="str">
+        <f ca="1"/>
+        <v>TAILS</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
@@ -717,6 +771,13 @@
         <f ca="1"/>
         <v>String</v>
       </c>
+      <c r="C4" t="str">
+        <f ca="1"/>
+        <v>TAILS</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
@@ -727,18 +788,27 @@
         <f ca="1"/>
         <v>String</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C5" t="str">
+        <f ca="1"/>
+        <v>TAILS</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B6" t="str">
         <f ca="1"/>
         <v>String</v>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1"/>
+        <v>TAILS</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,9 +820,11 @@
         <f ca="1"/>
         <v>String</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C7" t="str">
+        <f ca="1"/>
+        <v>TAILS</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
@@ -763,19 +835,28 @@
         <f ca="1"/>
         <v>String</v>
       </c>
+      <c r="C8" t="str">
+        <f ca="1"/>
+        <v>HEADS</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B9" t="str">
         <f ca="1"/>
         <v>String</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C9" t="str">
+        <f ca="1"/>
+        <v>HEADS</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
@@ -786,255 +867,468 @@
         <f ca="1"/>
         <v>String</v>
       </c>
+      <c r="C10" t="str">
+        <f ca="1"/>
+        <v>TAILS</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="s">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="1" t="s">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="1" t="s">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="1" t="s">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="1" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="1" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="1" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="1" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="1" t="s">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="1" t="s">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="1" t="s">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="1" t="s">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="1" t="s">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="1" t="s">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" s="1" t="s">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="3" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx with CURRY function
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580A83BC-BB47-4BE0-A67A-EBA8D02AB4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B866061-5024-43F4-8376-EC5FB2EF4C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="ALL">_xlfn.LAMBDA(_xlpm.truth_values,AND(_xlpm.truth_values))</definedName>
     <definedName name="ALPHABET">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.alphabet,_xlfn.HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(_xlpm.vertical,NO),TRANSPOSE(_xlpm.alphabet),_xlpm.alphabet)))</definedName>
     <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
-    <definedName name="APPLY">_xlfn.LAMBDA(_xlpm.function,_xlop.argument1,_xlop.argument2,_xlop.argument3,_xlop.argument4,_xlop.argument5,_xlop.argument6,_xlop.argument7,_xlop.argument8,_xlop.argument9,_xlop.argument10,_xlfn.SWITCH(ARITY(_xlpm.argument1,_xlpm.argument2,_xlpm.argument3,_xlpm.argument4,_xlpm.argument5,_xlpm.argument6,_xlpm.argument7,_xlpm.argument8,_xlpm.argument9,_xlpm.argument10),1,_xlpm.function(_xlpm.argument1),2,_xlpm.function(_xlpm.argument1, _xlpm.argument2),3,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3),4,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4),5,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5),6,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6),7,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7),8,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8),9,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9),10,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9, _xlpm.argument10),OTHERWISE,_xlpm.function()))</definedName>
+    <definedName name="APPLY">_xlfn.LAMBDA(_xlpm.function,_xlop.argument1,_xlop.argument2,_xlop.argument3,_xlop.argument4,_xlop.argument5,_xlop.argument6,_xlop.argument7,_xlop.argument8,_xlop.argument9,_xlop.argument10,_xlfn.SWITCH(ARITY(_xlpm.argument1,_xlpm.argument2,_xlpm.argument3,_xlpm.argument4,_xlpm.argument5,_xlpm.argument6,_xlpm.argument7,_xlpm.argument8,_xlpm.argument9,_xlpm.argument10),0,_xlpm.function(),1,_xlpm.function(_xlpm.argument1),2,_xlpm.function(_xlpm.argument1, _xlpm.argument2),3,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3),4,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4),5,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5),6,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6),7,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7),8,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8),9,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9),_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9, _xlpm.argument10)))</definedName>
     <definedName name="ARITY">_xlfn.LAMBDA(_xlop._arg1,_xlop._arg2,_xlop._arg3,_xlop._arg4,_xlop._arg5,_xlop._arg6,_xlop._arg7,_xlop._arg8,_xlop._arg9,_xlop._arg10,_xlop._arg11,_xlop._arg12,_xlop._arg13,_xlop._arg14,_xlop._arg15,_xlop._arg16,_xlop._arg17,_xlop._arg18,_xlop._arg19,_xlop._arg20,_xlop._arg21,_xlop._arg22,_xlop._arg23,_xlop._arg24,_xlop._arg25,SUM(IS(_xlpm._arg1), IS(_xlpm._arg2), IS(_xlpm._arg3), IS(_xlpm._arg4), IS(_xlpm._arg5),IS(_xlpm._arg6), IS(_xlpm._arg7), IS(_xlpm._arg8), IS(_xlpm._arg9), IS(_xlpm._arg10),IS(_xlpm._arg11), IS(_xlpm._arg12), IS(_xlpm._arg13), IS(_xlpm._arg14), IS(_xlpm._arg15),IS(_xlpm._arg16), IS(_xlpm._arg17), IS(_xlpm._arg18), IS(_xlpm._arg19), IS(_xlpm._arg20),IS(_xlpm._arg21), IS(_xlpm._arg22), IS(_xlpm._arg23), IS(_xlpm._arg24), IS(_xlpm._arg25)))</definedName>
     <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
@@ -29,6 +29,7 @@
     <definedName name="COINTOSS">_xlfn.LAMBDA(PICK("Heads","Tails"))</definedName>
     <definedName name="CONS">_xlfn.LAMBDA(_xlpm.value,_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.HSTACK(_xlpm.value,_xlpm.range),_xlfn.VSTACK(_xlpm.value,_xlpm.range)))</definedName>
     <definedName name="CONTAINS">_xlfn.LAMBDA(_xlpm.haystack,_xlpm.needle,IF(AND(EQUAL(COUNTA(_xlpm.haystack),1),EQUAL(COUNTA(_xlpm.needle),1)),ISNUMBER(SEARCH(_xlpm.needle,_xlpm.haystack)),OR(EXACT(_xlpm.needle,_xlpm.haystack))))</definedName>
+    <definedName name="CURRY">_xlfn.LAMBDA(_xlpm.function,_xlpm.argument1,_xlfn.LAMBDA(_xlpm.argument2,_xlpm.function(_xlpm.argument1,_xlpm.argument2)))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(-1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
     <definedName name="DICEROLL">_xlfn.LAMBDA(PICK(1,2,3,4,5,6))</definedName>
@@ -706,7 +707,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -733,7 +736,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B2" t="str">
         <f ca="1"/>
@@ -741,7 +744,7 @@
       </c>
       <c r="C2" t="str">
         <f ca="1"/>
-        <v>HEADS</v>
+        <v>TAILS</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -750,7 +753,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B3" t="str">
         <f ca="1"/>
@@ -758,14 +761,14 @@
       </c>
       <c r="C3" t="str">
         <f ca="1"/>
-        <v>TAILS</v>
+        <v>HEADS</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B4" t="str">
         <f ca="1"/>
@@ -773,7 +776,7 @@
       </c>
       <c r="C4" t="str">
         <f ca="1"/>
-        <v>TAILS</v>
+        <v>HEADS</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>49</v>
@@ -782,7 +785,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B5" t="str">
         <f ca="1"/>
@@ -790,7 +793,7 @@
       </c>
       <c r="C5" t="str">
         <f ca="1"/>
-        <v>TAILS</v>
+        <v>HEADS</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -814,7 +817,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B7" t="str">
         <f ca="1"/>
@@ -822,14 +825,14 @@
       </c>
       <c r="C7" t="str">
         <f ca="1"/>
-        <v>TAILS</v>
+        <v>HEADS</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B8" t="str">
         <f ca="1"/>
@@ -837,7 +840,7 @@
       </c>
       <c r="C8" t="str">
         <f ca="1"/>
-        <v>HEADS</v>
+        <v>TAILS</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx workbook with ASSERT, ZERO?, ONE?, POSITIVE?, and NEGATIVE? functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B866061-5024-43F4-8376-EC5FB2EF4C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEA71A1-DEDC-48D2-B353-2B75FA9C07D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{FA1D3B14-03E8-4F9C-8529-CD690545B7ED}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
     <definedName name="APPLY">_xlfn.LAMBDA(_xlpm.function,_xlop.argument1,_xlop.argument2,_xlop.argument3,_xlop.argument4,_xlop.argument5,_xlop.argument6,_xlop.argument7,_xlop.argument8,_xlop.argument9,_xlop.argument10,_xlfn.SWITCH(ARITY(_xlpm.argument1,_xlpm.argument2,_xlpm.argument3,_xlpm.argument4,_xlpm.argument5,_xlpm.argument6,_xlpm.argument7,_xlpm.argument8,_xlpm.argument9,_xlpm.argument10),0,_xlpm.function(),1,_xlpm.function(_xlpm.argument1),2,_xlpm.function(_xlpm.argument1, _xlpm.argument2),3,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3),4,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4),5,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5),6,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6),7,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7),8,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8),9,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9),_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9, _xlpm.argument10)))</definedName>
     <definedName name="ARITY">_xlfn.LAMBDA(_xlop._arg1,_xlop._arg2,_xlop._arg3,_xlop._arg4,_xlop._arg5,_xlop._arg6,_xlop._arg7,_xlop._arg8,_xlop._arg9,_xlop._arg10,_xlop._arg11,_xlop._arg12,_xlop._arg13,_xlop._arg14,_xlop._arg15,_xlop._arg16,_xlop._arg17,_xlop._arg18,_xlop._arg19,_xlop._arg20,_xlop._arg21,_xlop._arg22,_xlop._arg23,_xlop._arg24,_xlop._arg25,SUM(IS(_xlpm._arg1), IS(_xlpm._arg2), IS(_xlpm._arg3), IS(_xlpm._arg4), IS(_xlpm._arg5),IS(_xlpm._arg6), IS(_xlpm._arg7), IS(_xlpm._arg8), IS(_xlpm._arg9), IS(_xlpm._arg10),IS(_xlpm._arg11), IS(_xlpm._arg12), IS(_xlpm._arg13), IS(_xlpm._arg14), IS(_xlpm._arg15),IS(_xlpm._arg16), IS(_xlpm._arg17), IS(_xlpm._arg18), IS(_xlpm._arg19), IS(_xlpm._arg20),IS(_xlpm._arg21), IS(_xlpm._arg22), IS(_xlpm._arg23), IS(_xlpm._arg24), IS(_xlpm._arg25)))</definedName>
+    <definedName name="ASSERT">_xlfn.LAMBDA(_xlpm.condition,_xlop.message,IF(_xlpm.condition,TRUE,DEFAULT(_xlpm.message,"Assertion failed")))</definedName>
     <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
@@ -49,7 +50,7 @@
     <definedName name="ID">_xlfn.LAMBDA(_xlpm.input,_xlpm.input)</definedName>
     <definedName name="IFBLANK">_xlfn.LAMBDA(_xlpm.cell_reference,_xlpm.value_if_blank,_xlop.value_if_not_blank,IF(OR(ISBLANK(_xlpm.cell_reference),EQUAL(_xlpm.cell_reference,""),_xlpm.value_if_blank,DEFAULT(_xlpm.value_if_not_blank, _xlpm.cell_reference))))</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
-    <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(1,DEFAULT(_xlpm.times,1))))</definedName>
+    <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,DEFAULT(_xlpm.times,1)))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
     <definedName name="ISATOM">_xlfn.LAMBDA(_xlpm.input,MEMBER(TYPESTRING(_xlpm.input),VLIST("Number","String","Error")))</definedName>
     <definedName name="ISHORIZONTAL">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),TRUE,FALSE))</definedName>
@@ -61,9 +62,12 @@
     <definedName name="LTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x&lt;=_xlpm.y,TRUE,FALSE))</definedName>
     <definedName name="MAGIC8BALL">_xlfn.LAMBDA(_xlop.yes_or_no_question,IF(PROVIDED(_xlpm.yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered"))</definedName>
     <definedName name="MEMBER">_xlfn.LAMBDA(_xlpm.needle,_xlpm.haystack,OR(EXACT(_xlpm.needle, _xlpm.haystack)))</definedName>
+    <definedName name="NEGATIVE?">_xlfn.LAMBDA(_xlpm.x,LESSTHAN(_xlpm.x,0))</definedName>
     <definedName name="NO">FALSE</definedName>
+    <definedName name="ONE?">_xlfn.LAMBDA(_xlpm.x,EQUAL(_xlpm.x,1))</definedName>
     <definedName name="OTHERWISE">TRUE</definedName>
     <definedName name="PICK">_xlfn.LAMBDA(_xlpm._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),CHOOSE(RANDBETWEEN(1, _xlpm.count), _xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5, _xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25)))</definedName>
+    <definedName name="POSITIVE?">_xlfn.LAMBDA(_xlpm.x,GREATERTHAN(_xlpm.x,0))</definedName>
     <definedName name="PROVIDED">_xlfn.LAMBDA(_xlop.argument,NOT(_xlfn.ISOMITTED(_xlpm.argument)))</definedName>
     <definedName name="QUESTION">_xlfn.LAMBDA(_xlpm.knowledgebase,_xlpm.fragment1,_xlop.fragment2,_xlop.fragment3,_xlop.fragment4,_xlop.fragment5,_xlop.fragment6,_xlop.fragment7,_xlop.fragment8,_xlop.fragment9,_xlop.fragment10,_xlfn.LET(_xlpm.arity,ARITY(_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10),_xlpm.template,CHOOSE(_xlpm.arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),_xlpm.subject,_xlpm.fragment2,_xlpm.question_word,LOWER(_xlpm.fragment1),CONTAINS(_xlpm.knowledgebase,FORMAT(_xlpm.template,_xlpm.subject,_xlpm.question_word,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10))))</definedName>
     <definedName name="RATIO">_xlfn.LAMBDA(_xlpm.numerator,_xlpm.denominator,_xlpm.numerator / _xlpm.denominator)</definedName>
@@ -79,6 +83,7 @@
     <definedName name="TYPESTRING">_xlfn.LAMBDA(_xlpm.input,_xlop.recursive,_xlfn.SWITCH(TYPE(_xlpm.input),1,"Number",2,"String",4,"Boolean",16,"Error",64,IF(DEFAULT(_xlpm.recursive,FALSE),_xlfn.MAP(_xlpm.input,_xlfn.LAMBDA(_xlpm.each,TYPESTRING(_xlpm.each))),"Range"),128,"Function",OTHERWISE,"Unknown"))</definedName>
     <definedName name="VLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.row_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.row_count,0),"()",_xlfn.MAKEARRAY(_xlpm.row_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,CHOOSE(_xlpm.row,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="YES">TRUE</definedName>
+    <definedName name="ZERO?">_xlfn.LAMBDA(_xlpm.x,EQUAL(_xlpm.x,0))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -124,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>DEFINE(ALL,LAMBDA(truth_values,AND(truth_values)))</t>
   </si>
@@ -204,9 +209,6 @@
     <t>DEFINE(IFOMITTED,LAMBDA(optional_argument,value_if_omitted,value_if_provided,IF(ISOMITTED(optional_argument),value_if_omitted,value_if_provided)))</t>
   </si>
   <si>
-    <t>DEFINE(INCREMENT,LAMBDA(x,[times],SUM(x,PRODUCT(1,DEFAULT(times,1)))))</t>
-  </si>
-  <si>
     <t>DEFINE(IS,LAMBDA(argument,IF(ISOMITTED(argument), 0, 1)))</t>
   </si>
   <si>
@@ -291,9 +293,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>DEFINE(APPLY,LAMBDA(function,[argument1],[argument2],[argument3],[argument4],[argument5],[argument6],[argument7],[argument8],[argument9],[argument10],SWITCH(ARITY(argument1,argument2,argument3,argument4,argument5,argument6,argument7,argument8,argument9,argument10),1,function(argument1),2,function(argument1, argument2),3,function(argument1, argument2, argument3),4,function(argument1, argument2, argument3, argument4),5,function(argument1, argument2, argument3, argument4, argument5),6,function(argument1, argument2, argument3, argument4, argument5, argument6),7,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7),8,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8),9,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9),10,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9, argument10),OTHERWISE,function())))</t>
-  </si>
-  <si>
     <t>DEFINE(ARITY,LAMBDA([_arg1], [_arg2], [_arg3], [_arg4], [_arg5],[_arg6], [_arg7], [_arg8], [_arg9], [_arg10],[_arg11], [_arg12], [_arg13], [_arg14], [_arg15],[_arg16], [_arg17], [_arg18], [_arg19], [_arg20],[_arg21], [_arg22], [_arg23], [_arg24], [_arg25],SUM(IS(_arg1), IS(_arg2), IS(_arg3), IS(_arg4), IS(_arg5),IS(_arg6), IS(_arg7), IS(_arg8), IS(_arg9), IS(_arg10),IS(_arg11), IS(_arg12), IS(_arg13), IS(_arg14), IS(_arg15),IS(_arg16), IS(_arg17), IS(_arg18), IS(_arg19), IS(_arg20),IS(_arg21), IS(_arg22), IS(_arg23), IS(_arg24), IS(_arg25))))</t>
   </si>
   <si>
@@ -313,6 +312,30 @@
   </si>
   <si>
     <t>DEFINE(TEXTBETWEEN,LAMBDA(source_text,first_boundary,second_boundary,LET(text_after_first_boundary,RIGHT(source_text,DIFFERENCE(LEN(source_text),DECREMENT(SUM(FIND(first_boundary,source_text),LEN(first_boundary))))),LEFT(text_after_first_boundary,DECREMENT(FIND(second_boundary,text_after_first_boundary))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(APPLY,LAMBDA(function,[argument1],[argument2],[argument3],[argument4],[argument5],[argument6],[argument7],[argument8],[argument9],[argument10],SWITCH(ARITY(argument1,argument2,argument3,argument4,argument5,argument6,argument7,argument8,argument9,argument10),0,function(),1,function(argument1),2,function(argument1, argument2),3,function(argument1, argument2, argument3),4,function(argument1, argument2, argument3, argument4),5,function(argument1, argument2, argument3, argument4, argument5),6,function(argument1, argument2, argument3, argument4, argument5, argument6),7,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7),8,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8),9,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9),function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9, argument10))))</t>
+  </si>
+  <si>
+    <t>DEFINE(CURRY,LAMBDA(function,argument1,LAMBDA(argument2,function(argument1,argument2))))</t>
+  </si>
+  <si>
+    <t>DEFINE(ASSERT,LAMBDA(condition,[message],IF(condition,TRUE,DEFAULT(message,"Assertion failed"))))</t>
+  </si>
+  <si>
+    <t>DEFINE(INCREMENT,LAMBDA(x,[times],SUM(x,DEFAULT(times,1))))</t>
+  </si>
+  <si>
+    <t>DEFINE(NEGATIVE?,LAMBDA(x,LESSTHAN(x,0)))</t>
+  </si>
+  <si>
+    <t>DEFINE(ONE?,LAMBDA(x,EQUAL(x,1)))</t>
+  </si>
+  <si>
+    <t>DEFINE(POSITIVE?,LAMBDA(x,GREATERTHAN(x,0)))</t>
+  </si>
+  <si>
+    <t>DEFINE(ZERO?,LAMBDA(x,EQUAL(x,0)))</t>
   </si>
 </sst>
 </file>
@@ -705,11 +728,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921C2094-74FC-46E7-B7CC-8CA3714EA1A5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -730,7 +751,7 @@
         <v>HEADS</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,7 +774,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B3" t="str">
         <f ca="1"/>
@@ -761,7 +782,7 @@
       </c>
       <c r="C3" t="str">
         <f ca="1"/>
-        <v>HEADS</v>
+        <v>TAILS</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -779,13 +800,13 @@
         <v>HEADS</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B5" t="str">
         <f ca="1"/>
@@ -793,14 +814,14 @@
       </c>
       <c r="C5" t="str">
         <f ca="1"/>
-        <v>HEADS</v>
+        <v>TAILS</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B6" t="str">
         <f ca="1"/>
@@ -808,16 +829,16 @@
       </c>
       <c r="C6" t="str">
         <f ca="1"/>
-        <v>TAILS</v>
+        <v>HEADS</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B7" t="str">
         <f ca="1"/>
@@ -825,7 +846,7 @@
       </c>
       <c r="C7" t="str">
         <f ca="1"/>
-        <v>HEADS</v>
+        <v>TAILS</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -843,13 +864,13 @@
         <v>TAILS</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="B9" t="str">
         <f ca="1"/>
@@ -857,14 +878,14 @@
       </c>
       <c r="C9" t="str">
         <f ca="1"/>
-        <v>HEADS</v>
+        <v>TAILS</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="B10" t="str">
         <f ca="1"/>
@@ -872,10 +893,10 @@
       </c>
       <c r="C10" t="str">
         <f ca="1"/>
-        <v>TAILS</v>
+        <v>HEADS</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,7 +904,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -891,7 +912,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,7 +920,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
@@ -907,7 +928,7 @@
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
@@ -915,7 +936,7 @@
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.25">
@@ -923,7 +944,7 @@
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.25">
@@ -931,7 +952,7 @@
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.25">
@@ -939,7 +960,7 @@
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.25">
@@ -947,7 +968,7 @@
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="4:4" x14ac:dyDescent="0.25">
@@ -955,7 +976,7 @@
     </row>
     <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="4:4" x14ac:dyDescent="0.25">
@@ -963,7 +984,7 @@
     </row>
     <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
@@ -971,7 +992,7 @@
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
@@ -979,7 +1000,7 @@
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="3" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
@@ -987,7 +1008,7 @@
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
@@ -995,7 +1016,7 @@
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="3" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
@@ -1003,7 +1024,7 @@
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
@@ -1011,7 +1032,7 @@
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.25">
@@ -1019,7 +1040,7 @@
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.25">
@@ -1027,7 +1048,7 @@
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
@@ -1035,7 +1056,7 @@
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
@@ -1043,7 +1064,7 @@
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
@@ -1051,7 +1072,7 @@
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="3" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
@@ -1059,7 +1080,7 @@
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
@@ -1067,7 +1088,7 @@
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="3" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
@@ -1075,7 +1096,7 @@
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
@@ -1083,7 +1104,7 @@
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.25">
@@ -1091,7 +1112,7 @@
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
@@ -1099,7 +1120,7 @@
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="3" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
@@ -1107,7 +1128,7 @@
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="3" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.25">
@@ -1115,7 +1136,7 @@
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="3" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1232,7 @@
     </row>
     <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.25">
@@ -1219,7 +1240,7 @@
     </row>
     <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="3" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.25">
@@ -1227,7 +1248,7 @@
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="3" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="4:4" x14ac:dyDescent="0.25">
@@ -1235,7 +1256,7 @@
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="3" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.25">
@@ -1251,7 +1272,7 @@
     </row>
     <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="105" spans="4:4" x14ac:dyDescent="0.25">
@@ -1267,7 +1288,7 @@
     </row>
     <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="4:4" x14ac:dyDescent="0.25">
@@ -1275,7 +1296,7 @@
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="3" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="4:4" x14ac:dyDescent="0.25">
@@ -1283,7 +1304,7 @@
     </row>
     <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
@@ -1291,7 +1312,7 @@
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.25">
@@ -1299,7 +1320,7 @@
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="3" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.25">
@@ -1307,7 +1328,7 @@
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118" s="3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.25">
@@ -1315,7 +1336,7 @@
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.25">
@@ -1323,7 +1344,7 @@
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.25">
@@ -1331,7 +1352,37 @@
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx workbook with refactored SELECTFROM, CRITERIATABLE, and INDICES functions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C2C9D1-CC99-4BD3-A015-94EC30A7A8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE37E8A-283D-49D5-AC2A-628D6284EEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10530" yWindow="3015" windowWidth="38700" windowHeight="15885" xr2:uid="{5A440F0A-E7EE-4215-8213-3BEED85B5325}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{5A440F0A-E7EE-4215-8213-3BEED85B5325}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="CONS">_xlfn.LAMBDA(_xlpm.value,_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.HSTACK(_xlpm.value,_xlpm.range),_xlfn.VSTACK(_xlpm.value,_xlpm.range)))</definedName>
     <definedName name="CONTAINS">_xlfn.LAMBDA(_xlpm.haystack,_xlpm.needle,IF(AND(EQUAL(COUNTA(_xlpm.haystack),1),EQUAL(COUNTA(_xlpm.needle),1)),ISNUMBER(SEARCH(_xlpm.needle,_xlpm.haystack)),OR(EXACT(_xlpm.needle,_xlpm.haystack))))</definedName>
     <definedName name="COUNTALL">_xlfn.LAMBDA(_xlpm.range,SUM(COUNTA(_xlpm.range),COUNTBLANK(_xlpm.range)))</definedName>
-    <definedName name="CRITERIATABLE">_xlfn.LAMBDA(_xlpm.column_names,_xlpm.row_conditions,_xlfn.LET(_xlpm.condition_strings,TRIMSPLIT(_xlpm.row_conditions,",",YES),_xlpm.condition_count,COUNTA(_xlpm.condition_strings),_xlpm.condition_operators,EXTRACTOPERATORS(_xlpm.condition_strings),_xlpm.condition_column_indices,_xlfn.MAKEARRAY(_xlpm.condition_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,_xlfn.LET(_xlpm.condition,INDEX(_xlpm.condition_strings,_xlpm.row,1),_xlpm.operator,INDEX(_xlpm.condition_operators,_xlpm.row,1),MATCH(TRIM(_xlfn.TEXTBEFORE(_xlpm.condition,_xlpm.operator)),_xlpm.column_names)))),_xlpm.condition_criteria,_xlfn.MAKEARRAY(_xlpm.condition_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,_xlfn.LET(_xlpm.condition,INDEX(_xlpm.condition_strings,_xlpm.row,1),_xlpm.operator,INDEX(_xlpm.condition_operators,_xlpm.row,1),_xlpm.result,TRIM(_xlfn.TEXTAFTER(_xlpm.condition,_xlpm.operator)),IFERROR(_xlfn.NUMBERVALUE(_xlpm.result),_xlpm.result)))),_xlfn.HSTACK(_xlpm.condition_operators,_xlpm.condition_column_indices,_xlpm.condition_criteria)))</definedName>
+    <definedName name="CRITERIATABLE">_xlfn.LAMBDA(_xlpm.column_names,_xlpm.row_conditions,_xlfn.LET(_xlpm.condition_strings,TRIMSPLIT(_xlpm.row_conditions,",",YES),_xlpm.condition_count,COUNTA(_xlpm.condition_strings),_xlpm.condition_operators,EXTRACTOPERATORS(_xlpm.condition_strings),_xlpm.condition_column_indices,_xlfn.MAKEARRAY(_xlpm.condition_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,_xlfn.LET(_xlpm.condition,INDEX(_xlpm.condition_strings,_xlpm.row,1),_xlpm.operator,INDEX(_xlpm.condition_operators,_xlpm.row,1),MATCH(TRIM(_xlfn.TEXTBEFORE(_xlpm.condition,_xlpm.operator)),_xlpm.column_names,FALSE)))),_xlpm.condition_criteria,_xlfn.MAKEARRAY(_xlpm.condition_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,_xlfn.LET(_xlpm.condition,INDEX(_xlpm.condition_strings,_xlpm.row,1),_xlpm.operator,INDEX(_xlpm.condition_operators,_xlpm.row,1),_xlpm.result,TRIM(_xlfn.TEXTAFTER(_xlpm.condition,_xlpm.operator)),IFERROR(_xlfn.NUMBERVALUE(_xlpm.result),_xlpm.result)))),_xlfn.HSTACK(_xlpm.condition_operators,_xlpm.condition_column_indices,_xlpm.condition_criteria)))</definedName>
     <definedName name="CURRY">_xlfn.LAMBDA(_xlpm.function,_xlpm.argument1,_xlfn.LAMBDA(_xlpm.argument2,_xlpm.function(_xlpm.argument1,_xlpm.argument2)))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(-1,DEFAULT(_xlpm.times,1))))</definedName>
     <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
@@ -61,7 +61,7 @@
     <definedName name="IFBLANK">_xlfn.LAMBDA(_xlpm.cell_reference,_xlpm.value_if_blank,_xlop.value_if_not_blank,IF(OR(ISBLANK(_xlpm.cell_reference),EQUAL(_xlpm.cell_reference,""),_xlpm.value_if_blank,DEFAULT(_xlpm.value_if_not_blank, _xlpm.cell_reference))))</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
     <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,DEFAULT(_xlpm.times,1)))</definedName>
-    <definedName name="INDICES">_xlfn.LAMBDA(_xlpm.subset,_xlpm.superset,_xlfn.LET(_xlpm.vertical_subset,IF(HORIZONTAL?(_xlpm.subset),TRANSPOSE(_xlpm.subset),_xlpm.subset),_xlpm.vertical_superset,IF(HORIZONTAL?(_xlpm.superset),TRANSPOSE(_xlpm.superset),_xlpm.superset),_xlfn.MAKEARRAY(COUNTA(_xlpm.vertical_subset),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,MATCH(INDEX(_xlpm.vertical_subset,_xlpm.row,1),_xlpm.vertical_superset)))))</definedName>
+    <definedName name="INDICES">_xlfn.LAMBDA(_xlpm.subset,_xlpm.superset,_xlfn.LET(_xlpm.vertical_subset,IF(HORIZONTAL?(_xlpm.subset),TRANSPOSE(_xlpm.subset),_xlpm.subset),_xlpm.vertical_superset,IF(HORIZONTAL?(_xlpm.superset),TRANSPOSE(_xlpm.superset),_xlpm.superset),_xlfn.MAKEARRAY(COUNTA(_xlpm.vertical_subset),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,MATCH(INDEX(_xlpm.vertical_subset,_xlpm.row,1),_xlpm.vertical_superset,FALSE)))))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
     <definedName name="ISATOM">_xlfn.LAMBDA(_xlpm.input,MEMBER(TYPESTRING(_xlpm.input),VLIST("Number","String","Error")))</definedName>
     <definedName name="LAST">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),INDEX(_xlpm.range,1,COUNTA(_xlpm.range)),INDEX(_xlpm.range,COUNTA(_xlpm.range),1)))</definedName>
@@ -86,11 +86,11 @@
     <definedName name="REVERSE">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.col))))),_xlfn.MAKEARRAY(ROWS(_xlpm.range),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.row)),1)))))</definedName>
     <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.CONCAT(FORMAT("You threw {1}. SL threw {2}. ",_xlpm.human,_xlpm.robot),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cut Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cut Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors."))))</definedName>
     <definedName name="ROLLDICE">_xlfn.LAMBDA(_xlop.times,IF(LTE(DEFAULT(_xlpm.times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(_xlpm.times)))))</definedName>
-    <definedName name="SELECTCOLUMNS">_xlfn.LAMBDA(_xlpm.range,_xlop.columns,IF(OR(_xlfn.ISOMITTED(_xlpm.columns),MEMBER(UPPER(DEFAULT(_xlpm.columns, "")),VLIST("*","ALL"))),_xlpm.range,_xlfn.LET(_xlpm.column_names,IF(ISTEXT(_xlpm.columns),TRIMSPLIT(_xlpm.columns,","),_xlpm.columns),_xlpm.column_indices,INDICES(_xlpm.column_names,FIRSTROW(_xlpm.range)),IF(ONE?(COUNT(_xlpm.column_indices)),_xlfn.CHOOSECOLS(_xlpm.range,_xlpm.column_indices),_xlfn.HSTACK(_xlfn.CHOOSECOLS(_xlpm.range,FIRST(_xlpm.column_indices)),SELECTCOLUMNS(_xlpm.range,REST(_xlpm.column_names)))))))</definedName>
-    <definedName name="SELECTFROM">_xlfn.LAMBDA(_xlpm.columns,_xlpm.table_range,_xlop.row_conditions,_xlfn.LET(_xlpm.row_subset,SELECTROWS(_xlpm.table_range,_xlpm.row_conditions),SELECTCOLUMNS(_xlpm.row_subset,_xlpm.columns)))</definedName>
+    <definedName name="SELECTCOLUMNS">_xlfn.LAMBDA(_xlpm.table_range,_xlop.columns,IF(OR(_xlfn.ISOMITTED(_xlpm.columns),MEMBER(UPPER(DEFAULT(_xlpm.columns, "")),VLIST("*","ALL"))),_xlpm.table_range,_xlfn.LET(_xlpm.column_names,IF(ISTEXT(_xlpm.columns),TRIMSPLIT(_xlpm.columns,","),_xlpm.columns),_xlpm.column_indices,INDICES(_xlpm.column_names,FIRSTROW(_xlpm.table_range)),IF(ONE?(COUNT(_xlpm.column_indices)),_xlfn.CHOOSECOLS(_xlpm.table_range,_xlpm.column_indices),_xlfn.HSTACK(_xlfn.CHOOSECOLS(_xlpm.table_range,FIRST(_xlpm.column_indices)),SELECTCOLUMNS(_xlpm.table_range,REST(_xlpm.column_names)))))))</definedName>
+    <definedName name="SELECTFROM">_xlfn.LAMBDA(_xlpm.columns,_xlpm.table_range,_xlop.row_conditions,SELECTCOLUMNS(SELECTROWS(_xlpm.table_range,_xlpm.row_conditions),_xlpm.columns))</definedName>
     <definedName name="SELECTROWS">_xlfn.LAMBDA(_xlpm.table_range,_xlop.row_conditions,IFOMITTED(_xlpm.row_conditions,_xlpm.table_range,_xlfn.LET(_xlpm.column_names,FIRSTROW(_xlpm.table_range),_xlfn.VSTACK(_xlpm.column_names,SIEVE(HEADLESS(_xlpm.table_range),CRITERIATABLE(_xlpm.column_names,_xlpm.row_conditions))))))</definedName>
     <definedName name="SHEETNAME">_xlfn.LAMBDA(_xlop.reference,_xlfn.LET(_xlpm.filename,FILENAME(_xlpm.reference),_xlpm.bracket_position,FIND("]",_xlpm.filename),RIGHT(_xlpm.filename,DECREMENT(LEN(_xlpm.filename),_xlpm.bracket_position))))</definedName>
-    <definedName name="SIEVE">_xlfn.LAMBDA(_xlpm.table_data,_xlpm.filter_lookup_table,_xlfn._xlws.FILTER(_xlpm.table_data,EQUAL(TRUE,_xlfn.BYROW(_xlpm.table_data,_xlfn.LAMBDA(_xlpm.row,MEETSCRITERIA(_xlpm.row,_xlpm.filter_lookup_table))))))</definedName>
+    <definedName name="SIEVE">_xlfn.LAMBDA(_xlpm.table_data,_xlpm.filter_lookup_table,_xlfn._xlws.FILTER(_xlpm.table_data,_xlfn.BYROW(_xlpm.table_data,_xlfn.LAMBDA(_xlpm.row,MEETSCRITERIA(_xlpm.row,_xlpm.filter_lookup_table)))))</definedName>
     <definedName name="SL">_xlfn.LAMBDA("0.9.0")</definedName>
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
     <definedName name="STATEMENT">_xlfn.LAMBDA(_xlpm.fragment1,_xlop.fragment2,_xlop.fragment3,_xlop.fragment4,_xlop.fragment5,_xlop.fragment6,_xlop.fragment7,_xlop.fragment8,_xlop.fragment9,_xlop.fragment10,_xlfn.LET(_xlpm.arity,ARITY(_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10),_xlpm.template,CHOOSE(_xlpm.arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),FORMAT(_xlpm.template,_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10)))</definedName>
@@ -196,9 +196,6 @@
     <t>DEFINE(COUNTALL,LAMBDA(range,SUM(COUNTA(range),COUNTBLANK(range))))</t>
   </si>
   <si>
-    <t>DEFINE(CRITERIATABLE,LAMBDA(column_names,row_conditions,LET(condition_strings,TRIMSPLIT(row_conditions,",",YES),condition_count,COUNTA(condition_strings),condition_operators,EXTRACTOPERATORS(condition_strings),condition_column_indices,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),MATCH(TRIM(TEXTBEFORE(condition,operator)),column_names)))),condition_criteria,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),result,TRIM(TEXTAFTER(condition,operator)),IFERROR(NUMBERVALUE(result),result)))),HSTACK(condition_operators,condition_column_indices,condition_criteria))))</t>
-  </si>
-  <si>
     <t>DEFINE(CURRY,LAMBDA(function,argument1,LAMBDA(argument2,function(argument1,argument2))))</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>DEFINE(INCREMENT,LAMBDA(x,[times],SUM(x,DEFAULT(times,1))))</t>
   </si>
   <si>
-    <t>DEFINE(INDICES,LAMBDA(subset,superset,LET(vertical_subset,IF(HORIZONTAL?(subset),TRANSPOSE(subset),subset),vertical_superset,IF(HORIZONTAL?(superset),TRANSPOSE(superset),superset),MAKEARRAY(COUNTA(vertical_subset),1,LAMBDA(row,_col,MATCH(INDEX(vertical_subset,row,1),vertical_superset))))))</t>
-  </si>
-  <si>
     <t>DEFINE(IS,LAMBDA(argument,IF(ISOMITTED(argument), 0, 1)))</t>
   </si>
   <si>
@@ -361,21 +355,12 @@
     <t>DEFINE(ROLLDICE,LAMBDA([times],IF(LTE(DEFAULT(times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(times))))))</t>
   </si>
   <si>
-    <t>DEFINE(SELECTFROM,LAMBDA(columns,table_range,[row_conditions],LET(row_subset,SELECTROWS(table_range,row_conditions),SELECTCOLUMNS(row_subset,columns))))</t>
-  </si>
-  <si>
-    <t>DEFINE(SELECTCOLUMNS,LAMBDA(range,[columns],IF(OR(ISOMITTED(columns),MEMBER(UPPER(DEFAULT(columns, "")),VLIST("*","ALL"))),range,LET(column_names,IF(ISTEXT(columns),TRIMSPLIT(columns,","),columns),column_indices,INDICES(column_names,FIRSTROW(range)),IF(ONE?(COUNT(column_indices)),CHOOSECOLS(range,column_indices),HSTACK(CHOOSECOLS(range,FIRST(column_indices)),SELECTCOLUMNS(range,REST(column_names))))))))</t>
-  </si>
-  <si>
     <t>DEFINE(SELECTROWS,LAMBDA(table_range,[row_conditions],IFOMITTED(row_conditions,table_range,LET(column_names,FIRSTROW(table_range),VSTACK(column_names,SIEVE(HEADLESS(table_range),CRITERIATABLE(column_names,row_conditions)))))))</t>
   </si>
   <si>
     <t>DEFINE(SHEETNAME,LAMBDA([reference],LET(filename,FILENAME(reference),bracket_position,FIND("]",filename),RIGHT(filename,DECREMENT(LEN(filename),bracket_position)))))</t>
   </si>
   <si>
-    <t>DEFINE(SIEVE,LAMBDA(table_data,filter_lookup_table,FILTER(table_data,EQUAL(TRUE,BYROW(table_data,LAMBDA(row,MEETSCRITERIA(row,filter_lookup_table)))))))</t>
-  </si>
-  <si>
     <t>DEFINE(SL,LAMBDA("0.9.0"))</t>
   </si>
   <si>
@@ -404,6 +389,21 @@
   </si>
   <si>
     <t>DEFINE(ZERO?,LAMBDA(x,EQUAL(x,0)))</t>
+  </si>
+  <si>
+    <t>DEFINE(CRITERIATABLE,LAMBDA(column_names,row_conditions,LET(condition_strings,TRIMSPLIT(row_conditions,",",YES),condition_count,COUNTA(condition_strings),condition_operators,EXTRACTOPERATORS(condition_strings),condition_column_indices,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),MATCH(TRIM(TEXTBEFORE(condition,operator)),column_names,FALSE)))),condition_criteria,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),result,TRIM(TEXTAFTER(condition,operator)),IFERROR(NUMBERVALUE(result),result)))),HSTACK(condition_operators,condition_column_indices,condition_criteria))))</t>
+  </si>
+  <si>
+    <t>DEFINE(INDICES,LAMBDA(subset,superset,LET(vertical_subset,IF(HORIZONTAL?(subset),TRANSPOSE(subset),subset),vertical_superset,IF(HORIZONTAL?(superset),TRANSPOSE(superset),superset),MAKEARRAY(COUNTA(vertical_subset),1,LAMBDA(row,_col,MATCH(INDEX(vertical_subset,row,1),vertical_superset,FALSE))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(SELECTFROM,LAMBDA(columns,table_range,[row_conditions],SELECTCOLUMNS(SELECTROWS(table_range,row_conditions),columns)))</t>
+  </si>
+  <si>
+    <t>DEFINE(SELECTCOLUMNS,LAMBDA(table_range,[columns],IF(OR(ISOMITTED(columns),MEMBER(UPPER(DEFAULT(columns, "")),VLIST("*","ALL"))),table_range,LET(column_names,IF(ISTEXT(columns),TRIMSPLIT(columns,","),columns),column_indices,INDICES(column_names,FIRSTROW(table_range)),IF(ONE?(COUNT(column_indices)),CHOOSECOLS(table_range,column_indices),HSTACK(CHOOSECOLS(table_range,FIRST(column_indices)),SELECTCOLUMNS(table_range,REST(column_names))))))))</t>
+  </si>
+  <si>
+    <t>DEFINE(SIEVE,LAMBDA(table_data,filter_lookup_table,FILTER(table_data,BYROW(table_data,LAMBDA(row,MEETSCRITERIA(row,filter_lookup_table))))))</t>
   </si>
 </sst>
 </file>
@@ -796,22 +796,16 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str" cm="1">
-        <f t="array" aca="1" ref="A1:A10" ca="1">FLIPCOIN(10)</f>
-        <v>Heads</v>
+        <f t="array" ref="A1">SL()</f>
+        <v>0.9.0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f ca="1"/>
-        <v>Tails</v>
-      </c>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f ca="1"/>
+      <c r="A3" t="str" cm="1">
+        <f t="array" aca="1" ref="A3:A12" ca="1">FLIPCOIN(10)</f>
         <v>Tails</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -842,7 +836,7 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -851,7 +845,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,8 +864,18 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f ca="1"/>
+        <v>Heads</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,352 +930,352 @@
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="1" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx workbook with IDENTITY function
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE37E8A-283D-49D5-AC2A-628D6284EEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DE49E3-DDE5-4CD4-92F9-34B10A63800E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{5A440F0A-E7EE-4215-8213-3BEED85B5325}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{9A12A885-5DD2-4ED7-B455-CBD2D675CCE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <definedName name="HEADLESS">_xlfn.LAMBDA(_xlpm.range,_xlfn.MAKEARRAY(DECREMENT(ROWS(_xlpm.range)),COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm.row,_xlpm.col,INDEX(_xlpm.range,INCREMENT(_xlpm.row),_xlpm.col))))</definedName>
     <definedName name="HLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.column_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.column_count,0),"()",_xlfn.MAKEARRAY(1,_xlpm.column_count,_xlfn.LAMBDA(_xlpm._row,_xlpm.col,CHOOSE(_xlpm.col,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="HORIZONTAL?">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),TRUE,FALSE))</definedName>
-    <definedName name="ID">_xlfn.LAMBDA(_xlpm.input,_xlpm.input)</definedName>
+    <definedName name="IDENTITY">_xlfn.LAMBDA(_xlpm.x,_xlpm.x)</definedName>
     <definedName name="IFBLANK">_xlfn.LAMBDA(_xlpm.cell_reference,_xlpm.value_if_blank,_xlop.value_if_not_blank,IF(OR(ISBLANK(_xlpm.cell_reference),EQUAL(_xlpm.cell_reference,""),_xlpm.value_if_blank,DEFAULT(_xlpm.value_if_not_blank, _xlpm.cell_reference))))</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
     <definedName name="INCREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,DEFAULT(_xlpm.times,1)))</definedName>
@@ -196,6 +196,9 @@
     <t>DEFINE(COUNTALL,LAMBDA(range,SUM(COUNTA(range),COUNTBLANK(range))))</t>
   </si>
   <si>
+    <t>DEFINE(CRITERIATABLE,LAMBDA(column_names,row_conditions,LET(condition_strings,TRIMSPLIT(row_conditions,",",YES),condition_count,COUNTA(condition_strings),condition_operators,EXTRACTOPERATORS(condition_strings),condition_column_indices,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),MATCH(TRIM(TEXTBEFORE(condition,operator)),column_names,FALSE)))),condition_criteria,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),result,TRIM(TEXTAFTER(condition,operator)),IFERROR(NUMBERVALUE(result),result)))),HSTACK(condition_operators,condition_column_indices,condition_criteria))))</t>
+  </si>
+  <si>
     <t>DEFINE(CURRY,LAMBDA(function,argument1,LAMBDA(argument2,function(argument1,argument2))))</t>
   </si>
   <si>
@@ -265,7 +268,7 @@
     <t>DEFINE(HLIST,LAMBDA([_1], [_2], [_3], [_4], [_5],[_6], [_7], [_8], [_9], [_10],[_11], [_12], [_13], [_14], [_15],[_16], [_17], [_18], [_19], [_20],[_21], [_22], [_23], [_24], [_25],LET(column_count,SUM(IS(_1), IS(_2), IS(_3), IS(_4), IS(_5),IS(_6), IS(_7), IS(_8), IS(_9), IS(_10),IS(_11), IS(_12), IS(_13), IS(_14), IS(_15),IS(_16), IS(_17), IS(_18), IS(_19), IS(_20),IS(_21), IS(_22), IS(_23), IS(_24), IS(_25)),IF(EQUAL(column_count,0),"()",MAKEARRAY(1,column_count,LAMBDA(_row,col,CHOOSE(col,_1, _2, _3, _4, _5,_6, _7, _8, _9, _10,_11, _12, _13, _14, _15,_16, _17, _18, _19, _20,_21, _22, _23, _24, _25)))))))</t>
   </si>
   <si>
-    <t>DEFINE(ID,LAMBDA(input,input))</t>
+    <t>DEFINE(IDENTITY,LAMBDA(x,x))</t>
   </si>
   <si>
     <t>DEFINE(IFBLANK,LAMBDA(cell_reference,value_if_blank,[value_if_not_blank],IF(OR(ISBLANK(cell_reference),EQUAL(cell_reference,""),value_if_blank,DEFAULT(value_if_not_blank, cell_reference)))))</t>
@@ -277,6 +280,9 @@
     <t>DEFINE(INCREMENT,LAMBDA(x,[times],SUM(x,DEFAULT(times,1))))</t>
   </si>
   <si>
+    <t>DEFINE(INDICES,LAMBDA(subset,superset,LET(vertical_subset,IF(HORIZONTAL?(subset),TRANSPOSE(subset),subset),vertical_superset,IF(HORIZONTAL?(superset),TRANSPOSE(superset),superset),MAKEARRAY(COUNTA(vertical_subset),1,LAMBDA(row,_col,MATCH(INDEX(vertical_subset,row,1),vertical_superset,FALSE))))))</t>
+  </si>
+  <si>
     <t>DEFINE(IS,LAMBDA(argument,IF(ISOMITTED(argument), 0, 1)))</t>
   </si>
   <si>
@@ -355,12 +361,21 @@
     <t>DEFINE(ROLLDICE,LAMBDA([times],IF(LTE(DEFAULT(times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(times))))))</t>
   </si>
   <si>
+    <t>DEFINE(SELECTFROM,LAMBDA(columns,table_range,[row_conditions],SELECTCOLUMNS(SELECTROWS(table_range,row_conditions),columns)))</t>
+  </si>
+  <si>
+    <t>DEFINE(SELECTCOLUMNS,LAMBDA(table_range,[columns],IF(OR(ISOMITTED(columns),MEMBER(UPPER(DEFAULT(columns, "")),VLIST("*","ALL"))),table_range,LET(column_names,IF(ISTEXT(columns),TRIMSPLIT(columns,","),columns),column_indices,INDICES(column_names,FIRSTROW(table_range)),IF(ONE?(COUNT(column_indices)),CHOOSECOLS(table_range,column_indices),HSTACK(CHOOSECOLS(table_range,FIRST(column_indices)),SELECTCOLUMNS(table_range,REST(column_names))))))))</t>
+  </si>
+  <si>
     <t>DEFINE(SELECTROWS,LAMBDA(table_range,[row_conditions],IFOMITTED(row_conditions,table_range,LET(column_names,FIRSTROW(table_range),VSTACK(column_names,SIEVE(HEADLESS(table_range),CRITERIATABLE(column_names,row_conditions)))))))</t>
   </si>
   <si>
     <t>DEFINE(SHEETNAME,LAMBDA([reference],LET(filename,FILENAME(reference),bracket_position,FIND("]",filename),RIGHT(filename,DECREMENT(LEN(filename),bracket_position)))))</t>
   </si>
   <si>
+    <t>DEFINE(SIEVE,LAMBDA(table_data,filter_lookup_table,FILTER(table_data,BYROW(table_data,LAMBDA(row,MEETSCRITERIA(row,filter_lookup_table))))))</t>
+  </si>
+  <si>
     <t>DEFINE(SL,LAMBDA("0.9.0"))</t>
   </si>
   <si>
@@ -389,21 +404,6 @@
   </si>
   <si>
     <t>DEFINE(ZERO?,LAMBDA(x,EQUAL(x,0)))</t>
-  </si>
-  <si>
-    <t>DEFINE(CRITERIATABLE,LAMBDA(column_names,row_conditions,LET(condition_strings,TRIMSPLIT(row_conditions,",",YES),condition_count,COUNTA(condition_strings),condition_operators,EXTRACTOPERATORS(condition_strings),condition_column_indices,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),MATCH(TRIM(TEXTBEFORE(condition,operator)),column_names,FALSE)))),condition_criteria,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),result,TRIM(TEXTAFTER(condition,operator)),IFERROR(NUMBERVALUE(result),result)))),HSTACK(condition_operators,condition_column_indices,condition_criteria))))</t>
-  </si>
-  <si>
-    <t>DEFINE(INDICES,LAMBDA(subset,superset,LET(vertical_subset,IF(HORIZONTAL?(subset),TRANSPOSE(subset),subset),vertical_superset,IF(HORIZONTAL?(superset),TRANSPOSE(superset),superset),MAKEARRAY(COUNTA(vertical_subset),1,LAMBDA(row,_col,MATCH(INDEX(vertical_subset,row,1),vertical_superset,FALSE))))))</t>
-  </si>
-  <si>
-    <t>DEFINE(SELECTFROM,LAMBDA(columns,table_range,[row_conditions],SELECTCOLUMNS(SELECTROWS(table_range,row_conditions),columns)))</t>
-  </si>
-  <si>
-    <t>DEFINE(SELECTCOLUMNS,LAMBDA(table_range,[columns],IF(OR(ISOMITTED(columns),MEMBER(UPPER(DEFAULT(columns, "")),VLIST("*","ALL"))),table_range,LET(column_names,IF(ISTEXT(columns),TRIMSPLIT(columns,","),columns),column_indices,INDICES(column_names,FIRSTROW(table_range)),IF(ONE?(COUNT(column_indices)),CHOOSECOLS(table_range,column_indices),HSTACK(CHOOSECOLS(table_range,FIRST(column_indices)),SELECTCOLUMNS(table_range,REST(column_names))))))))</t>
-  </si>
-  <si>
-    <t>DEFINE(SIEVE,LAMBDA(table_data,filter_lookup_table,FILTER(table_data,BYROW(table_data,LAMBDA(row,MEETSCRITERIA(row,filter_lookup_table))))))</t>
   </si>
 </sst>
 </file>
@@ -783,11 +783,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BC621F-8D9A-457C-81C8-0B86A5BF2897}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0352917B-A07A-4C94-9C8E-22AAD128092A}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -851,7 +853,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -930,355 +932,356 @@
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="1" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating 0.9.0.lisp source and pre-installed SpreadsheetLisp.xlsx workbook with latest definitions
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DE49E3-DDE5-4CD4-92F9-34B10A63800E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48B3964-AE06-4B5E-88E0-DBB0BD1C3277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{9A12A885-5DD2-4ED7-B455-CBD2D675CCE4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{97ED30AC-8B34-4AE5-86CC-C3EA482AB169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,24 +18,26 @@
   <definedNames>
     <definedName name="ALL">_xlfn.LAMBDA(_xlpm.truth_values,AND(_xlpm.truth_values))</definedName>
     <definedName name="ALPHABET">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.alphabet,_xlfn.HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(_xlpm.vertical,NO),TRANSPOSE(_xlpm.alphabet),_xlpm.alphabet)))</definedName>
-    <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
+    <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN?(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
     <definedName name="APPLY">_xlfn.LAMBDA(_xlpm.function,_xlop.argument1,_xlop.argument2,_xlop.argument3,_xlop.argument4,_xlop.argument5,_xlop.argument6,_xlop.argument7,_xlop.argument8,_xlop.argument9,_xlop.argument10,_xlfn.SWITCH(ARITY(_xlpm.argument1,_xlpm.argument2,_xlpm.argument3,_xlpm.argument4,_xlpm.argument5,_xlpm.argument6,_xlpm.argument7,_xlpm.argument8,_xlpm.argument9,_xlpm.argument10),0,_xlpm.function(),1,_xlpm.function(_xlpm.argument1),2,_xlpm.function(_xlpm.argument1, _xlpm.argument2),3,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3),4,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4),5,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5),6,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6),7,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7),8,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8),9,_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9),_xlpm.function(_xlpm.argument1, _xlpm.argument2, _xlpm.argument3, _xlpm.argument4, _xlpm.argument5, _xlpm.argument6, _xlpm.argument7, _xlpm.argument8, _xlpm.argument9, _xlpm.argument10)))</definedName>
     <definedName name="ARITY">_xlfn.LAMBDA(_xlop._arg1,_xlop._arg2,_xlop._arg3,_xlop._arg4,_xlop._arg5,_xlop._arg6,_xlop._arg7,_xlop._arg8,_xlop._arg9,_xlop._arg10,_xlop._arg11,_xlop._arg12,_xlop._arg13,_xlop._arg14,_xlop._arg15,_xlop._arg16,_xlop._arg17,_xlop._arg18,_xlop._arg19,_xlop._arg20,_xlop._arg21,_xlop._arg22,_xlop._arg23,_xlop._arg24,_xlop._arg25,SUM(IS(_xlpm._arg1), IS(_xlpm._arg2), IS(_xlpm._arg3), IS(_xlpm._arg4), IS(_xlpm._arg5),IS(_xlpm._arg6), IS(_xlpm._arg7), IS(_xlpm._arg8), IS(_xlpm._arg9), IS(_xlpm._arg10),IS(_xlpm._arg11), IS(_xlpm._arg12), IS(_xlpm._arg13), IS(_xlpm._arg14), IS(_xlpm._arg15),IS(_xlpm._arg16), IS(_xlpm._arg17), IS(_xlpm._arg18), IS(_xlpm._arg19), IS(_xlpm._arg20),IS(_xlpm._arg21), IS(_xlpm._arg22), IS(_xlpm._arg23), IS(_xlpm._arg24), IS(_xlpm._arg25)))</definedName>
     <definedName name="ASSERT">_xlfn.LAMBDA(_xlpm.condition,_xlop.message,IF(_xlpm.condition,TRUE,DEFAULT(_xlpm.message,"Assertion failed")))</definedName>
     <definedName name="CAPITALIZE">_xlfn.LAMBDA(_xlpm.text,_xlfn.CONCAT(UPPER(FIRSTLETTER(_xlpm.text)),RIGHT(_xlpm.text, DECREMENT(LEN(_xlpm.text)))))</definedName>
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
-    <definedName name="CDR">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,DECREMENT(COLUMNS(_xlpm.range)),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,INCREMENT(_xlpm.col)))),_xlfn.MAKEARRAY(DECREMENT(ROWS(_xlpm.range)),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,INCREMENT(_xlpm.row),1)))))</definedName>
+    <definedName name="CDR">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN?(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,DECREMENT(COLUMNS(_xlpm.range)),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,INCREMENT(_xlpm.col)))),_xlfn.MAKEARRAY(DECREMENT(ROWS(_xlpm.range)),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,INCREMENT(_xlpm.row),1)))))</definedName>
     <definedName name="CELLNAME">_xlfn.LAMBDA(_xlop.reference,_xlop.absolute,_xlfn.LET(_xlpm.address,IFOMITTED(_xlpm.reference,CELL("address"),CELL("address",_xlpm.reference)),_xlpm.display_absolute,DEFAULT(_xlpm.absolute,NO),IF(_xlpm.display_absolute,_xlpm.address,SUBSTITUTE(_xlpm.address,"$",""))))</definedName>
     <definedName name="COINTOSS">_xlfn.LAMBDA(PICK("Heads","Tails"))</definedName>
     <definedName name="COLUMNLETTER">_xlfn.LAMBDA(_xlop.cell_reference,TEXTBETWEEN(IFOMITTED(_xlpm.cell_reference,ADDRESS(ROW(),COLUMN()),ADDRESS(ROW(_xlpm.cell_reference),COLUMN(_xlpm.cell_reference))),"$","$"))</definedName>
-    <definedName name="CONS">_xlfn.LAMBDA(_xlpm.value,_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.HSTACK(_xlpm.value,_xlpm.range),_xlfn.VSTACK(_xlpm.value,_xlpm.range)))</definedName>
+    <definedName name="CONS">_xlfn.LAMBDA(_xlpm.value,_xlpm.range,IF(GREATERTHAN?(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.HSTACK(_xlpm.value,_xlpm.range),_xlfn.VSTACK(_xlpm.value,_xlpm.range)))</definedName>
+    <definedName name="CONSTANCY">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.x)</definedName>
     <definedName name="CONTAINS">_xlfn.LAMBDA(_xlpm.haystack,_xlpm.needle,IF(AND(EQUAL(COUNTA(_xlpm.haystack),1),EQUAL(COUNTA(_xlpm.needle),1)),ISNUMBER(SEARCH(_xlpm.needle,_xlpm.haystack)),OR(EXACT(_xlpm.needle,_xlpm.haystack))))</definedName>
-    <definedName name="COUNTALL">_xlfn.LAMBDA(_xlpm.range,SUM(COUNTA(_xlpm.range),COUNTBLANK(_xlpm.range)))</definedName>
+    <definedName name="COUNTCELLS">_xlfn.LAMBDA(_xlpm.range,SUM(COUNTA(_xlpm.range),COUNTBLANK(_xlpm.range)))</definedName>
     <definedName name="CRITERIATABLE">_xlfn.LAMBDA(_xlpm.column_names,_xlpm.row_conditions,_xlfn.LET(_xlpm.condition_strings,TRIMSPLIT(_xlpm.row_conditions,",",YES),_xlpm.condition_count,COUNTA(_xlpm.condition_strings),_xlpm.condition_operators,EXTRACTOPERATORS(_xlpm.condition_strings),_xlpm.condition_column_indices,_xlfn.MAKEARRAY(_xlpm.condition_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,_xlfn.LET(_xlpm.condition,INDEX(_xlpm.condition_strings,_xlpm.row,1),_xlpm.operator,INDEX(_xlpm.condition_operators,_xlpm.row,1),MATCH(TRIM(_xlfn.TEXTBEFORE(_xlpm.condition,_xlpm.operator)),_xlpm.column_names,FALSE)))),_xlpm.condition_criteria,_xlfn.MAKEARRAY(_xlpm.condition_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,_xlfn.LET(_xlpm.condition,INDEX(_xlpm.condition_strings,_xlpm.row,1),_xlpm.operator,INDEX(_xlpm.condition_operators,_xlpm.row,1),_xlpm.result,TRIM(_xlfn.TEXTAFTER(_xlpm.condition,_xlpm.operator)),IFERROR(_xlfn.NUMBERVALUE(_xlpm.result),_xlpm.result)))),_xlfn.HSTACK(_xlpm.condition_operators,_xlpm.condition_column_indices,_xlpm.condition_criteria)))</definedName>
+    <definedName name="CUBEROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,RATIO(1,3)))</definedName>
     <definedName name="CURRY">_xlfn.LAMBDA(_xlpm.function,_xlpm.argument1,_xlfn.LAMBDA(_xlpm.argument2,_xlpm.function(_xlpm.argument1,_xlpm.argument2)))</definedName>
     <definedName name="DECREMENT">_xlfn.LAMBDA(_xlpm.x,_xlop.times,SUM(_xlpm.x,PRODUCT(-1,DEFAULT(_xlpm.times,1))))</definedName>
-    <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
+    <definedName name="DEFAULT">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.fallback_value,IF(PROVIDED?(_xlpm.optional_argument),_xlpm.optional_argument,_xlpm.fallback_value))</definedName>
     <definedName name="DICEROLL">_xlfn.LAMBDA(PICK(1,2,3,4,5,6))</definedName>
     <definedName name="DIFFERENCE">_xlfn.LAMBDA(_xlpm.minuend,_xlpm.subtrahend,_xlpm.minuend-_xlpm.subtrahend)</definedName>
     <definedName name="EMPTYLIST?">_xlfn.LAMBDA(_xlpm.input,_xlfn.LET(_xlpm.occupied_cells,COUNTA(_xlpm.input),_xlpm.blank_cells,COUNTBLANK(_xlpm.input),IF(ONE?(SUM(_xlpm.occupied_cells,_xlpm.blank_cells)),OR(ISBLANK(_xlpm.input),EQUAL(_xlpm.input,"()"),NO))))</definedName>
@@ -48,15 +50,15 @@
     <definedName name="FIRSTLETTER">_xlfn.LAMBDA(_xlpm.text,LEFT(_xlpm.text,1))</definedName>
     <definedName name="FIRSTROW">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,0))</definedName>
     <definedName name="FIRSTWORD">_xlfn.LAMBDA(_xlpm.text,LEFT(TRIM(_xlpm.text),DECREMENT(FIND(" ",TRIM(_xlpm.text)))))</definedName>
-    <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
+    <definedName name="FLIPCOIN">_xlfn.LAMBDA(_xlop.times,_xlfn.LET(_xlpm.counter,DEFAULT(_xlpm.times, 1),IF(LTE?(_xlpm.counter, 1),COINTOSS(),_xlfn.VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(_xlpm.counter))))))</definedName>
     <definedName name="FOREACH">_xlfn.LAMBDA(_xlpm.range,_xlpm.function_to_apply,_xlfn.MAP(_xlpm.range,_xlpm.function_to_apply))</definedName>
-    <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlop.sixth_value,_xlop.seventh_value,_xlop.eigth_value,_xlop.ninth_value,_xlop.tenth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),_xlpm._after5,IF(PROVIDED(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4),_xlpm._after6,IF(PROVIDED(_xlpm.sixth_value),SUBSTITUTE(_xlpm._after5,"{6}", _xlpm.sixth_value),_xlpm._after5),_xlpm._after7,IF(PROVIDED(_xlpm.seventh_value),SUBSTITUTE(_xlpm._after6,"{7}", _xlpm.seventh_value),_xlpm._after6),_xlpm._after8,IF(PROVIDED(_xlpm.eigth_value),SUBSTITUTE(_xlpm._after7,"{8}", _xlpm.eigth_value),_xlpm._after7),_xlpm._after9,IF(PROVIDED(_xlpm.ninth_value),SUBSTITUTE(_xlpm._after8,"{9}", _xlpm.ninth_value),_xlpm._after8),IF(PROVIDED(_xlpm.tenth_value),SUBSTITUTE(_xlpm._after9,"{10}", _xlpm.tenth_value),_xlpm._after9)))</definedName>
+    <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlop.sixth_value,_xlop.seventh_value,_xlop.eigth_value,_xlop.ninth_value,_xlop.tenth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED?(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED?(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED?(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),_xlpm._after5,IF(PROVIDED?(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4),_xlpm._after6,IF(PROVIDED?(_xlpm.sixth_value),SUBSTITUTE(_xlpm._after5,"{6}", _xlpm.sixth_value),_xlpm._after5),_xlpm._after7,IF(PROVIDED?(_xlpm.seventh_value),SUBSTITUTE(_xlpm._after6,"{7}", _xlpm.seventh_value),_xlpm._after6),_xlpm._after8,IF(PROVIDED?(_xlpm.eigth_value),SUBSTITUTE(_xlpm._after7,"{8}", _xlpm.eigth_value),_xlpm._after7),_xlpm._after9,IF(PROVIDED?(_xlpm.ninth_value),SUBSTITUTE(_xlpm._after8,"{9}", _xlpm.ninth_value),_xlpm._after8),IF(PROVIDED?(_xlpm.tenth_value),SUBSTITUTE(_xlpm._after9,"{10}", _xlpm.tenth_value),_xlpm._after9)))</definedName>
     <definedName name="FULLDECK">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.full_deck,_xlfn.HSTACK({"AS","KS","QS","JS","XS","9S","8S","7S","6S","5S","4S","3S","2S"},{"AH","KH","QH","JH","XH","9H","8H","7H","6H","5H","4H","3H","2H"},{"AD","KD","QD","JD","XD","9D","8D","7D","6D","5D","4D","3D","2D"},{"AC","KC","QC","JC","XC","9C","8C","7C","6C","5C","4C","3C","2C"}),IF(DEFAULT(_xlpm.vertical,FALSE),TRANSPOSE(_xlpm.full_deck),_xlpm.full_deck)))</definedName>
-    <definedName name="GREATERTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt; _xlpm.y,TRUE,FALSE))</definedName>
-    <definedName name="GTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &gt;= _xlpm.y,TRUE,FALSE))</definedName>
+    <definedName name="GREATERTHAN?">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.x&gt;_xlpm.y)</definedName>
+    <definedName name="GTE?">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.x&gt;=_xlpm.y)</definedName>
     <definedName name="HEADLESS">_xlfn.LAMBDA(_xlpm.range,_xlfn.MAKEARRAY(DECREMENT(ROWS(_xlpm.range)),COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm.row,_xlpm.col,INDEX(_xlpm.range,INCREMENT(_xlpm.row),_xlpm.col))))</definedName>
     <definedName name="HLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.column_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.column_count,0),"()",_xlfn.MAKEARRAY(1,_xlpm.column_count,_xlfn.LAMBDA(_xlpm._row,_xlpm.col,CHOOSE(_xlpm.col,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
-    <definedName name="HORIZONTAL?">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),TRUE,FALSE))</definedName>
+    <definedName name="HORIZONTAL?">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN?(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),TRUE,FALSE))</definedName>
     <definedName name="IDENTITY">_xlfn.LAMBDA(_xlpm.x,_xlpm.x)</definedName>
     <definedName name="IFBLANK">_xlfn.LAMBDA(_xlpm.cell_reference,_xlpm.value_if_blank,_xlop.value_if_not_blank,IF(OR(ISBLANK(_xlpm.cell_reference),EQUAL(_xlpm.cell_reference,""),_xlpm.value_if_blank,DEFAULT(_xlpm.value_if_not_blank, _xlpm.cell_reference))))</definedName>
     <definedName name="IFOMITTED">_xlfn.LAMBDA(_xlpm.optional_argument,_xlpm.value_if_omitted,_xlpm.value_if_provided,IF(_xlfn.ISOMITTED(_xlpm.optional_argument),_xlpm.value_if_omitted,_xlpm.value_if_provided))</definedName>
@@ -64,28 +66,27 @@
     <definedName name="INDICES">_xlfn.LAMBDA(_xlpm.subset,_xlpm.superset,_xlfn.LET(_xlpm.vertical_subset,IF(HORIZONTAL?(_xlpm.subset),TRANSPOSE(_xlpm.subset),_xlpm.subset),_xlpm.vertical_superset,IF(HORIZONTAL?(_xlpm.superset),TRANSPOSE(_xlpm.superset),_xlpm.superset),_xlfn.MAKEARRAY(COUNTA(_xlpm.vertical_subset),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,MATCH(INDEX(_xlpm.vertical_subset,_xlpm.row,1),_xlpm.vertical_superset,FALSE)))))</definedName>
     <definedName name="IS">_xlfn.LAMBDA(_xlpm.argument,IF(_xlfn.ISOMITTED(_xlpm.argument), 0, 1))</definedName>
     <definedName name="ISATOM">_xlfn.LAMBDA(_xlpm.input,MEMBER(TYPESTRING(_xlpm.input),VLIST("Number","String","Error")))</definedName>
-    <definedName name="LAST">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),INDEX(_xlpm.range,1,COUNTA(_xlpm.range)),INDEX(_xlpm.range,COUNTA(_xlpm.range),1)))</definedName>
-    <definedName name="LENGTH">_xlfn.LAMBDA(_xlop.input,_xlfn.LET(_xlpm.cell_count,IFOMITTED(_xlpm.input,0,COUNTALL(_xlpm.input)),IF(ONE?(_xlpm.cell_count),IF(EMPTYLIST?(_xlpm.input),0,LEN(_xlpm.input)),_xlpm.cell_count)))</definedName>
-    <definedName name="LESSTHAN">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x &lt; _xlpm.y,TRUE,FALSE))</definedName>
-    <definedName name="LTE">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(_xlpm.x&lt;=_xlpm.y,TRUE,FALSE))</definedName>
-    <definedName name="MAGIC8BALL">_xlfn.LAMBDA(_xlop.yes_or_no_question,IF(PROVIDED(_xlpm.yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered"))</definedName>
+    <definedName name="LAST">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN?(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),INDEX(_xlpm.range,1,COUNTA(_xlpm.range)),INDEX(_xlpm.range,COUNTA(_xlpm.range),1)))</definedName>
+    <definedName name="LESSTHAN?">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.x&lt;_xlpm.y)</definedName>
+    <definedName name="LTE?">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.x&lt;=_xlpm.y)</definedName>
+    <definedName name="MAGIC8BALL">_xlfn.LAMBDA(_xlop.yes_or_no_question,IF(PROVIDED?(_xlpm.yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered"))</definedName>
     <definedName name="MEETSCRITERIA">_xlfn.LAMBDA(_xlpm.row_data,_xlpm.criteria_table,ALL(_xlfn.MAKEARRAY(ROWS(_xlpm.criteria_table),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,_xlfn.LET(_xlpm.function,INDEX(_xlpm.criteria_table,_xlpm.row,2),_xlpm.value,INDEX(_xlpm.row_data,1,INDEX(_xlpm.criteria_table,_xlpm.row,3)),_xlpm.criterion,INDEX(_xlpm.criteria_table,_xlpm.row,4),APPLY(_xlpm.function,_xlpm.value,_xlpm.criterion))))))</definedName>
     <definedName name="MEMBER">_xlfn.LAMBDA(_xlpm.needle,_xlpm.haystack,OR(EXACT(_xlpm.needle, _xlpm.haystack)))</definedName>
-    <definedName name="NEGATIVE?">_xlfn.LAMBDA(_xlpm.x,LESSTHAN(_xlpm.x,0))</definedName>
+    <definedName name="NEGATIVE?">_xlfn.LAMBDA(_xlpm.x,LESSTHAN?(_xlpm.x,0))</definedName>
     <definedName name="NO">FALSE</definedName>
     <definedName name="NOTEQUAL">_xlfn.LAMBDA(_xlpm.a,_xlpm.b,NOT(EQUAL(_xlpm.a,_xlpm.b)))</definedName>
     <definedName name="ONE?">_xlfn.LAMBDA(_xlpm.x,EQUAL(_xlpm.x,1))</definedName>
     <definedName name="OTHERWISE">TRUE</definedName>
     <definedName name="PICK">_xlfn.LAMBDA(_xlpm._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),CHOOSE(RANDBETWEEN(1, _xlpm.count), _xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5, _xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25)))</definedName>
-    <definedName name="POSITIVE?">_xlfn.LAMBDA(_xlpm.x,GREATERTHAN(_xlpm.x,0))</definedName>
-    <definedName name="PROVIDED">_xlfn.LAMBDA(_xlop.argument,NOT(_xlfn.ISOMITTED(_xlpm.argument)))</definedName>
+    <definedName name="POSITIVE?">_xlfn.LAMBDA(_xlpm.x,GREATERTHAN?(_xlpm.x,0))</definedName>
+    <definedName name="PROVIDED?">_xlfn.LAMBDA(_xlop.argument,NOT(_xlfn.ISOMITTED(_xlpm.argument)))</definedName>
     <definedName name="QUESTION">_xlfn.LAMBDA(_xlpm.knowledgebase,_xlpm.fragment1,_xlop.fragment2,_xlop.fragment3,_xlop.fragment4,_xlop.fragment5,_xlop.fragment6,_xlop.fragment7,_xlop.fragment8,_xlop.fragment9,_xlop.fragment10,_xlfn.LET(_xlpm.arity,ARITY(_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10),_xlpm.template,CHOOSE(_xlpm.arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),_xlpm.subject,_xlpm.fragment2,_xlpm.question_word,LOWER(_xlpm.fragment1),CONTAINS(_xlpm.knowledgebase,FORMAT(_xlpm.template,_xlpm.subject,_xlpm.question_word,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10))))</definedName>
     <definedName name="RANGE?">_xlfn.LAMBDA(_xlpm.input,EQUAL(TYPESTRING(_xlpm.input),"Range"))</definedName>
     <definedName name="RATIO">_xlfn.LAMBDA(_xlpm.numerator,_xlpm.denominator,_xlpm.numerator / _xlpm.denominator)</definedName>
     <definedName name="REST">_xlfn.LAMBDA(_xlpm.range,CDR(_xlpm.range))</definedName>
-    <definedName name="REVERSE">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.col))))),_xlfn.MAKEARRAY(ROWS(_xlpm.range),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,DECREMENT(LENGTH(_xlpm.range),DECREMENT(_xlpm.row)),1)))))</definedName>
+    <definedName name="REVERSE">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN?(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,DECREMENT(COUNTCELLS(_xlpm.range),DECREMENT(_xlpm.col))))),_xlfn.MAKEARRAY(ROWS(_xlpm.range),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,DECREMENT(COUNTCELLS(_xlpm.range),DECREMENT(_xlpm.row)),1)))))</definedName>
     <definedName name="ROCKPAPERSCISSORS">_xlfn.LAMBDA(_xlpm.throw,_xlfn.LET(_xlpm.human,CAPITALIZE(LOWER(DEFAULT(_xlpm.throw,""))),_xlpm.robot,PICK("Rock","Paper","Scissors"),_xlfn.CONCAT(FORMAT("You threw {1}. SL threw {2}. ",_xlpm.human,_xlpm.robot),_xlfn.IFS(CASE(_xlpm.human,_xlpm.robot),FORMAT("It's a tie! {1} vs. {1}",_xlpm.human),CASE(_xlpm.human,"Paper",_xlpm.robot,"Rock"),"You win! Paper covers Rock.",CASE(_xlpm.human,"Paper",_xlpm.robot,"Scissors"),"You lose! Scissors cut Paper.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(_xlpm.human,"Rock",_xlpm.robot,"Paper"),"You lose! Paper covers Rock.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Paper"),"You win! Scissors cut Paper.",CASE(_xlpm.human,"Scissors",_xlpm.robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors."))))</definedName>
-    <definedName name="ROLLDICE">_xlfn.LAMBDA(_xlop.times,IF(LTE(DEFAULT(_xlpm.times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(_xlpm.times)))))</definedName>
+    <definedName name="ROLLDICE">_xlfn.LAMBDA(_xlop.times,IF(LTE?(DEFAULT(_xlpm.times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(_xlpm.times)))))</definedName>
     <definedName name="SELECTCOLUMNS">_xlfn.LAMBDA(_xlpm.table_range,_xlop.columns,IF(OR(_xlfn.ISOMITTED(_xlpm.columns),MEMBER(UPPER(DEFAULT(_xlpm.columns, "")),VLIST("*","ALL"))),_xlpm.table_range,_xlfn.LET(_xlpm.column_names,IF(ISTEXT(_xlpm.columns),TRIMSPLIT(_xlpm.columns,","),_xlpm.columns),_xlpm.column_indices,INDICES(_xlpm.column_names,FIRSTROW(_xlpm.table_range)),IF(ONE?(COUNT(_xlpm.column_indices)),_xlfn.CHOOSECOLS(_xlpm.table_range,_xlpm.column_indices),_xlfn.HSTACK(_xlfn.CHOOSECOLS(_xlpm.table_range,FIRST(_xlpm.column_indices)),SELECTCOLUMNS(_xlpm.table_range,REST(_xlpm.column_names)))))))</definedName>
     <definedName name="SELECTFROM">_xlfn.LAMBDA(_xlpm.columns,_xlpm.table_range,_xlop.row_conditions,SELECTCOLUMNS(SELECTROWS(_xlpm.table_range,_xlpm.row_conditions),_xlpm.columns))</definedName>
     <definedName name="SELECTROWS">_xlfn.LAMBDA(_xlpm.table_range,_xlop.row_conditions,IFOMITTED(_xlpm.row_conditions,_xlpm.table_range,_xlfn.LET(_xlpm.column_names,FIRSTROW(_xlpm.table_range),_xlfn.VSTACK(_xlpm.column_names,SIEVE(HEADLESS(_xlpm.table_range),CRITERIATABLE(_xlpm.column_names,_xlpm.row_conditions))))))</definedName>
@@ -98,7 +99,7 @@
     <definedName name="TRIMALL">_xlfn.LAMBDA(_xlpm.range,_xlfn.MAKEARRAY(ROWS(_xlpm.range),COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm.row,_xlpm.col,TRIM(INDEX(_xlpm.range,_xlpm.row,_xlpm.col)))))</definedName>
     <definedName name="TRIMSPLIT">_xlfn.LAMBDA(_xlpm.source_text,_xlpm.split_at,_xlop.display_vertically,_xlfn.LET(_xlpm.result,TRIMALL(_xlfn.TEXTSPLIT(_xlpm.source_text,_xlpm.split_at)),IF(DEFAULT(_xlpm.display_vertically,FALSE),TRANSPOSE(_xlpm.result),_xlpm.result)))</definedName>
     <definedName name="TYPESTRING">_xlfn.LAMBDA(_xlpm.input,_xlop.recursive,_xlfn.SWITCH(TYPE(_xlpm.input),1,"Number",2,"String",4,"Boolean",16,"Error",64,IF(DEFAULT(_xlpm.recursive,FALSE),_xlfn.MAP(_xlpm.input,_xlfn.LAMBDA(_xlpm.each,TYPESTRING(_xlpm.each))),"Range"),128,"Function",OTHERWISE,"Unknown"))</definedName>
-    <definedName name="VERTICAL?">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN(ROWS(_xlpm.range),COLUMNS(_xlpm.range)),TRUE,FALSE))</definedName>
+    <definedName name="VERTICAL?">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN?(ROWS(_xlpm.range),COLUMNS(_xlpm.range)),TRUE,FALSE))</definedName>
     <definedName name="VLIST">_xlfn.LAMBDA(_xlop._1,_xlop._2,_xlop._3,_xlop._4,_xlop._5,_xlop._6,_xlop._7,_xlop._8,_xlop._9,_xlop._10,_xlop._11,_xlop._12,_xlop._13,_xlop._14,_xlop._15,_xlop._16,_xlop._17,_xlop._18,_xlop._19,_xlop._20,_xlop._21,_xlop._22,_xlop._23,_xlop._24,_xlop._25,_xlfn.LET(_xlpm.row_count,SUM(IS(_xlpm._1), IS(_xlpm._2), IS(_xlpm._3), IS(_xlpm._4), IS(_xlpm._5),IS(_xlpm._6), IS(_xlpm._7), IS(_xlpm._8), IS(_xlpm._9), IS(_xlpm._10),IS(_xlpm._11), IS(_xlpm._12), IS(_xlpm._13), IS(_xlpm._14), IS(_xlpm._15),IS(_xlpm._16), IS(_xlpm._17), IS(_xlpm._18), IS(_xlpm._19), IS(_xlpm._20),IS(_xlpm._21), IS(_xlpm._22), IS(_xlpm._23), IS(_xlpm._24), IS(_xlpm._25)),IF(EQUAL(_xlpm.row_count,0),"()",_xlfn.MAKEARRAY(_xlpm.row_count,1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,CHOOSE(_xlpm.row,_xlpm._1, _xlpm._2, _xlpm._3, _xlpm._4, _xlpm._5,_xlpm._6, _xlpm._7, _xlpm._8, _xlpm._9, _xlpm._10,_xlpm._11, _xlpm._12, _xlpm._13, _xlpm._14, _xlpm._15,_xlpm._16, _xlpm._17, _xlpm._18, _xlpm._19, _xlpm._20,_xlpm._21, _xlpm._22, _xlpm._23, _xlpm._24, _xlpm._25))))))</definedName>
     <definedName name="YES">TRUE</definedName>
     <definedName name="ZERO?">_xlfn.LAMBDA(_xlpm.x,EQUAL(_xlpm.x,0))</definedName>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>DEFINE(ALL,LAMBDA(truth_values,AND(truth_values)))</t>
   </si>
@@ -154,7 +155,7 @@
     <t>DEFINE(ALPHABET,LAMBDA([vertical],LET(alphabet,HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(vertical,NO),TRANSPOSE(alphabet),alphabet))))</t>
   </si>
   <si>
-    <t>DEFINE(APPEND,LAMBDA(head,body,IF(GREATERTHAN(COLUMNS(body),ROWS(body)),HSTACK(head,body),VSTACK(head,body))))</t>
+    <t>DEFINE(APPEND,LAMBDA(head,body,IF(GREATERTHAN?(COLUMNS(body),ROWS(body)),HSTACK(head,body),VSTACK(head,body))))</t>
   </si>
   <si>
     <t>DEFINE(APPLY,LAMBDA(function,[argument1],[argument2],[argument3],[argument4],[argument5],[argument6],[argument7],[argument8],[argument9],[argument10],SWITCH(ARITY(argument1,argument2,argument3,argument4,argument5,argument6,argument7,argument8,argument9,argument10),0,function(),1,function(argument1),2,function(argument1, argument2),3,function(argument1, argument2, argument3),4,function(argument1, argument2, argument3, argument4),5,function(argument1, argument2, argument3, argument4, argument5),6,function(argument1, argument2, argument3, argument4, argument5, argument6),7,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7),8,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8),9,function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9),function(argument1, argument2, argument3, argument4, argument5, argument6, argument7, argument8, argument9, argument10))))</t>
@@ -178,7 +179,7 @@
     <t>DEFINE(CELLNAME,LAMBDA([reference],[absolute],LET(address,IFOMITTED(reference,CELL("address"),CELL("address",reference)),display_absolute,DEFAULT(absolute,NO),IF(display_absolute,address,SUBSTITUTE(address,"$","")))))</t>
   </si>
   <si>
-    <t>DEFINE(CDR,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),MAKEARRAY(1,DECREMENT(COLUMNS(range)),LAMBDA(_row,col,INDEX(range,1,INCREMENT(col)))),MAKEARRAY(DECREMENT(ROWS(range)),1,LAMBDA(row,_col,INDEX(range,INCREMENT(row),1))))))</t>
+    <t>DEFINE(CDR,LAMBDA(range,IF(GREATERTHAN?(COLUMNS(range),ROWS(range)),MAKEARRAY(1,DECREMENT(COLUMNS(range)),LAMBDA(_row,col,INDEX(range,1,INCREMENT(col)))),MAKEARRAY(DECREMENT(ROWS(range)),1,LAMBDA(row,_col,INDEX(range,INCREMENT(row),1))))))</t>
   </si>
   <si>
     <t>DEFINE(COINTOSS,LAMBDA(PICK("Heads","Tails")))</t>
@@ -187,25 +188,31 @@
     <t>DEFINE(COLUMNLETTER,LAMBDA([cell_reference],TEXTBETWEEN(IFOMITTED(cell_reference,ADDRESS(ROW(),COLUMN()),ADDRESS(ROW(cell_reference),COLUMN(cell_reference))),"$","$")))</t>
   </si>
   <si>
-    <t>DEFINE(CONS,LAMBDA(value,range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),HSTACK(value,range),VSTACK(value,range))))</t>
+    <t>DEFINE(CONS,LAMBDA(value,range,IF(GREATERTHAN?(COLUMNS(range),ROWS(range)),HSTACK(value,range),VSTACK(value,range))))</t>
+  </si>
+  <si>
+    <t>DEFINE(CONSTANCY,LAMBDA(x,y,x))</t>
   </si>
   <si>
     <t>DEFINE(CONTAINS,LAMBDA(haystack,needle,IF(AND(EQUAL(COUNTA(haystack),1),EQUAL(COUNTA(needle),1)),ISNUMBER(SEARCH(needle,haystack)),OR(EXACT(needle,haystack)))))</t>
   </si>
   <si>
-    <t>DEFINE(COUNTALL,LAMBDA(range,SUM(COUNTA(range),COUNTBLANK(range))))</t>
+    <t>DEFINE(COUNTCELLS,LAMBDA(range,SUM(COUNTA(range),COUNTBLANK(range))))</t>
   </si>
   <si>
     <t>DEFINE(CRITERIATABLE,LAMBDA(column_names,row_conditions,LET(condition_strings,TRIMSPLIT(row_conditions,",",YES),condition_count,COUNTA(condition_strings),condition_operators,EXTRACTOPERATORS(condition_strings),condition_column_indices,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),MATCH(TRIM(TEXTBEFORE(condition,operator)),column_names,FALSE)))),condition_criteria,MAKEARRAY(condition_count,1,LAMBDA(row,_col,LET(condition,INDEX(condition_strings,row,1),operator,INDEX(condition_operators,row,1),result,TRIM(TEXTAFTER(condition,operator)),IFERROR(NUMBERVALUE(result),result)))),HSTACK(condition_operators,condition_column_indices,condition_criteria))))</t>
   </si>
   <si>
+    <t>DEFINE(CUBEROOT,LAMBDA(x,POWER(x,RATIO(1,3))))</t>
+  </si>
+  <si>
     <t>DEFINE(CURRY,LAMBDA(function,argument1,LAMBDA(argument2,function(argument1,argument2))))</t>
   </si>
   <si>
     <t>DEFINE(DECREMENT,LAMBDA(x,[times],SUM(x,PRODUCT(-1,DEFAULT(times,1)))))</t>
   </si>
   <si>
-    <t>DEFINE(DEFAULT,LAMBDA(optional_argument,fallback_value,IF(PROVIDED(optional_argument),optional_argument,fallback_value)))</t>
+    <t>DEFINE(DEFAULT,LAMBDA(optional_argument,fallback_value,IF(PROVIDED?(optional_argument),optional_argument,fallback_value)))</t>
   </si>
   <si>
     <t>DEFINE(DICEROLL,LAMBDA(PICK(1,2,3,4,5,6)))</t>
@@ -244,22 +251,22 @@
     <t>DEFINE(FIRSTWORD,LAMBDA(text,LEFT(TRIM(text),DECREMENT(FIND(" ",TRIM(text))))))</t>
   </si>
   <si>
-    <t>DEFINE(FLIPCOIN,LAMBDA([times],LET(counter,DEFAULT(times, 1),IF(LTE(counter, 1),COINTOSS(),VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(counter)))))))</t>
+    <t>DEFINE(FLIPCOIN,LAMBDA([times],LET(counter,DEFAULT(times, 1),IF(LTE?(counter, 1),COINTOSS(),VSTACK(COINTOSS(),FLIPCOIN(DECREMENT(counter)))))))</t>
   </si>
   <si>
     <t>DEFINE(FOREACH,LAMBDA(range,function_to_apply,MAP(range,function_to_apply)))</t>
   </si>
   <si>
-    <t>DEFINE(FORMAT,LAMBDA(template_text,first_value,[second_value],[third_value],[fourth_value],[fifth_value],[sixth_value],[seventh_value],[eigth_value],[ninth_value],[tenth_value],LET(_after1,SUBSTITUTE(template_text,"{1}", first_value),_after2,IF(PROVIDED(second_value),SUBSTITUTE(_after1,"{2}", second_value),_after1),_after3,IF(PROVIDED(third_value),SUBSTITUTE(_after2,"{3}", third_value),_after2),_after4,IF(PROVIDED(fourth_value),SUBSTITUTE(_after3,"{4}", fourth_value),_after3),_after5,IF(PROVIDED(fifth_value),SUBSTITUTE(_after4,"{5}", fifth_value),_after4),_after6,IF(PROVIDED(sixth_value),SUBSTITUTE(_after5,"{6}", sixth_value),_after5),_after7,IF(PROVIDED(seventh_value),SUBSTITUTE(_after6,"{7}", seventh_value),_after6),_after8,IF(PROVIDED(eigth_value),SUBSTITUTE(_after7,"{8}", eigth_value),_after7),_after9,IF(PROVIDED(ninth_value),SUBSTITUTE(_after8,"{9}", ninth_value),_after8),IF(PROVIDED(tenth_value),SUBSTITUTE(_after9,"{10}", tenth_value),_after9))))</t>
+    <t>DEFINE(FORMAT,LAMBDA(template_text,first_value,[second_value],[third_value],[fourth_value],[fifth_value],[sixth_value],[seventh_value],[eigth_value],[ninth_value],[tenth_value],LET(_after1,SUBSTITUTE(template_text,"{1}", first_value),_after2,IF(PROVIDED?(second_value),SUBSTITUTE(_after1,"{2}", second_value),_after1),_after3,IF(PROVIDED?(third_value),SUBSTITUTE(_after2,"{3}", third_value),_after2),_after4,IF(PROVIDED?(fourth_value),SUBSTITUTE(_after3,"{4}", fourth_value),_after3),_after5,IF(PROVIDED?(fifth_value),SUBSTITUTE(_after4,"{5}", fifth_value),_after4),_after6,IF(PROVIDED?(sixth_value),SUBSTITUTE(_after5,"{6}", sixth_value),_after5),_after7,IF(PROVIDED?(seventh_value),SUBSTITUTE(_after6,"{7}", seventh_value),_after6),_after8,IF(PROVIDED?(eigth_value),SUBSTITUTE(_after7,"{8}", eigth_value),_after7),_after9,IF(PROVIDED?(ninth_value),SUBSTITUTE(_after8,"{9}", ninth_value),_after8),IF(PROVIDED?(tenth_value),SUBSTITUTE(_after9,"{10}", tenth_value),_after9))))</t>
   </si>
   <si>
     <t>DEFINE(FULLDECK,LAMBDA([vertical],LET(full_deck,HSTACK({"AS","KS","QS","JS","XS","9S","8S","7S","6S","5S","4S","3S","2S"},{"AH","KH","QH","JH","XH","9H","8H","7H","6H","5H","4H","3H","2H"},{"AD","KD","QD","JD","XD","9D","8D","7D","6D","5D","4D","3D","2D"},{"AC","KC","QC","JC","XC","9C","8C","7C","6C","5C","4C","3C","2C"}),IF(DEFAULT(vertical,FALSE),TRANSPOSE(full_deck),full_deck))))</t>
   </si>
   <si>
-    <t>DEFINE(GREATERTHAN,LAMBDA(x,y,IF(x &gt; y,TRUE,FALSE)))</t>
-  </si>
-  <si>
-    <t>DEFINE(GTE,LAMBDA(x,y,IF(x &gt;= y,TRUE,FALSE)))</t>
+    <t>DEFINE(GREATERTHAN?,LAMBDA(x,y,x&gt;y))</t>
+  </si>
+  <si>
+    <t>DEFINE(GTE?,LAMBDA(x,y,x&gt;=y))</t>
   </si>
   <si>
     <t>DEFINE(HEADLESS,LAMBDA(range,MAKEARRAY(DECREMENT(ROWS(range)),COLUMNS(range),LAMBDA(row,col,INDEX(range,INCREMENT(row),col)))))</t>
@@ -289,28 +296,25 @@
     <t>DEFINE(ISATOM,LAMBDA(input,MEMBER(TYPESTRING(input),VLIST("Number","String","Error"))))</t>
   </si>
   <si>
-    <t>DEFINE(HORIZONTAL?,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),TRUE,FALSE)))</t>
+    <t>DEFINE(HORIZONTAL?,LAMBDA(range,IF(GREATERTHAN?(COLUMNS(range),ROWS(range)),TRUE,FALSE)))</t>
   </si>
   <si>
     <t>DEFINE(RANGE?,LAMBDA(input,EQUAL(TYPESTRING(input),"Range")))</t>
   </si>
   <si>
-    <t>DEFINE(VERTICAL?,LAMBDA(range,IF(GREATERTHAN(ROWS(range),COLUMNS(range)),TRUE,FALSE)))</t>
-  </si>
-  <si>
-    <t>DEFINE(LAST,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),INDEX(range,1,COUNTA(range)),INDEX(range,COUNTA(range),1))))</t>
-  </si>
-  <si>
-    <t>DEFINE(LENGTH,LAMBDA([input],LET(cell_count,IFOMITTED(input,0,COUNTALL(input)),IF(ONE?(cell_count),IF(EMPTYLIST?(input),0,LEN(input)),cell_count))))</t>
-  </si>
-  <si>
-    <t>DEFINE(LESSTHAN,LAMBDA(x,y,IF(x &lt; y,TRUE,FALSE)))</t>
-  </si>
-  <si>
-    <t>DEFINE(LTE,LAMBDA(x,y,IF(x&lt;=y,TRUE,FALSE)))</t>
-  </si>
-  <si>
-    <t>DEFINE(MAGIC8BALL,LAMBDA([yes_or_no_question],IF(PROVIDED(yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered")))</t>
+    <t>DEFINE(VERTICAL?,LAMBDA(range,IF(GREATERTHAN?(ROWS(range),COLUMNS(range)),TRUE,FALSE)))</t>
+  </si>
+  <si>
+    <t>DEFINE(LAST,LAMBDA(range,IF(GREATERTHAN?(COLUMNS(range),ROWS(range)),INDEX(range,1,COUNTA(range)),INDEX(range,COUNTA(range),1))))</t>
+  </si>
+  <si>
+    <t>DEFINE(LESSTHAN?,LAMBDA(x,y,x&lt;y))</t>
+  </si>
+  <si>
+    <t>DEFINE(LTE?,LAMBDA(x,y,x&lt;=y))</t>
+  </si>
+  <si>
+    <t>DEFINE(MAGIC8BALL,LAMBDA([yes_or_no_question],IF(PROVIDED?(yes_or_no_question),PICK("It is certain","Reply hazy, try again","It is decidedly so","Without a doubt","Don't count on it","Yes, definitely","Ask again later","You may rely on it","My reply is no","As I see it, yes","Better not tell you now","Most likely","My sources say no","Outlook good","Cannot predict now","Yes","Outlook not so good","Signs point to yes","Concentrate and ask again","Very doubtful"),"Ask, and you will be answered")))</t>
   </si>
   <si>
     <t>DEFINE(MEETSCRITERIA,LAMBDA(row_data,criteria_table,ALL(MAKEARRAY(ROWS(criteria_table),1,LAMBDA(row,_col,LET(function,INDEX(criteria_table,row,2),value,INDEX(row_data,1,INDEX(criteria_table,row,3)),criterion,INDEX(criteria_table,row,4),APPLY(function,value,criterion)))))))</t>
@@ -319,7 +323,7 @@
     <t>DEFINE(MEMBER,LAMBDA(needle,haystack,OR(EXACT(needle, haystack))))</t>
   </si>
   <si>
-    <t>DEFINE(NEGATIVE?,LAMBDA(x,LESSTHAN(x,0)))</t>
+    <t>DEFINE(NEGATIVE?,LAMBDA(x,LESSTHAN?(x,0)))</t>
   </si>
   <si>
     <t>DEFINE(NO,FALSE)</t>
@@ -337,10 +341,10 @@
     <t>DEFINE(PICK,LAMBDA(_1, [_2], [_3], [_4], [_5],[_6], [_7], [_8], [_9], [_10],[_11], [_12], [_13], [_14], [_15],[_16], [_17], [_18], [_19], [_20],[_21], [_22], [_23], [_24], [_25],LET(count,SUM(IS(_1), IS(_2), IS(_3), IS(_4), IS(_5),IS(_6), IS(_7), IS(_8), IS(_9), IS(_10),IS(_11), IS(_12), IS(_13), IS(_14), IS(_15),IS(_16), IS(_17), IS(_18), IS(_19), IS(_20),IS(_21), IS(_22), IS(_23), IS(_24), IS(_25)),CHOOSE(RANDBETWEEN(1, count), _1, _2, _3, _4, _5, _6, _7, _8, _9, _10,_11, _12, _13, _14, _15,_16, _17, _18, _19, _20,_21, _22, _23, _24, _25))))</t>
   </si>
   <si>
-    <t>DEFINE(POSITIVE?,LAMBDA(x,GREATERTHAN(x,0)))</t>
-  </si>
-  <si>
-    <t>DEFINE(PROVIDED,LAMBDA([argument],NOT(ISOMITTED(argument))))</t>
+    <t>DEFINE(POSITIVE?,LAMBDA(x,GREATERTHAN?(x,0)))</t>
+  </si>
+  <si>
+    <t>DEFINE(PROVIDED?,LAMBDA([argument],NOT(ISOMITTED(argument))))</t>
   </si>
   <si>
     <t>DEFINE(QUESTION,LAMBDA(knowledgebase,fragment1,[fragment2],[fragment3],[fragment4],[fragment5],[fragment6],[fragment7],[fragment8],[fragment9],[fragment10],LET(arity,ARITY(fragment1,fragment2,fragment3,fragment4,fragment5,fragment6,fragment7,fragment8,fragment9,fragment10),template,CHOOSE(arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),subject,fragment2,question_word,LOWER(fragment1),CONTAINS(knowledgebase,FORMAT(template,subject,question_word,fragment3,fragment4,fragment5,fragment6,fragment7,fragment8,fragment9,fragment10)))))</t>
@@ -352,13 +356,13 @@
     <t>DEFINE(REST,LAMBDA(range,CDR(range)))</t>
   </si>
   <si>
-    <t>DEFINE(REVERSE,LAMBDA(range,IF(GREATERTHAN(COLUMNS(range),ROWS(range)),MAKEARRAY(1,COLUMNS(range),LAMBDA(_row,col,INDEX(range,1,DECREMENT(LENGTH(range),DECREMENT(col))))),MAKEARRAY(ROWS(range),1,LAMBDA(row,_col,INDEX(range,DECREMENT(LENGTH(range),DECREMENT(row)),1))))))</t>
+    <t>DEFINE(REVERSE,LAMBDA(range,IF(GREATERTHAN?(COLUMNS(range),ROWS(range)),MAKEARRAY(1,COLUMNS(range),LAMBDA(_row,col,INDEX(range,1,DECREMENT(COUNTCELLS(range),DECREMENT(col))))),MAKEARRAY(ROWS(range),1,LAMBDA(row,_col,INDEX(range,DECREMENT(COUNTCELLS(range),DECREMENT(row)),1))))))</t>
   </si>
   <si>
     <t>DEFINE(ROCKPAPERSCISSORS,LAMBDA(throw,LET(human,CAPITALIZE(LOWER(DEFAULT(throw,""))),robot,PICK("Rock","Paper","Scissors"),CONCAT(FORMAT("You threw {1}. SL threw {2}. ",human,robot),IFS(CASE(human,robot),FORMAT("It's a tie! {1} vs. {1}",human),CASE(human,"Paper",robot,"Rock"),"You win! Paper covers Rock.",CASE(human,"Paper",robot,"Scissors"),"You lose! Scissors cut Paper.",CASE(human,"Rock",robot,"Scissors"),"You win! Rock crushes Scissors.",CASE(human,"Rock",robot,"Paper"),"You lose! Paper covers Rock.",CASE(human,"Scissors",robot,"Paper"),"You win! Scissors cut Paper.",CASE(human,"Scissors",robot,"Rock"),"You lose! Rock crushes Scissors.",OTHERWISE,"Invalid throw. Please choose Rock, Paper, or Scissors.")))))</t>
   </si>
   <si>
-    <t>DEFINE(ROLLDICE,LAMBDA([times],IF(LTE(DEFAULT(times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(times))))))</t>
+    <t>DEFINE(ROLLDICE,LAMBDA([times],IF(LTE?(DEFAULT(times,1),1),DICEROLL(),CONS(DICEROLL(),ROLLDICE(DECREMENT(times))))))</t>
   </si>
   <si>
     <t>DEFINE(SELECTFROM,LAMBDA(columns,table_range,[row_conditions],SELECTCOLUMNS(SELECTROWS(table_range,row_conditions),columns)))</t>
@@ -783,13 +787,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0352917B-A07A-4C94-9C8E-22AAD128092A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDAF5AA-D241-40A4-8000-F3CC7642628A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C171"/>
+  <dimension ref="A1:C173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -817,13 +819,13 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -832,7 +834,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,7 +864,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,8 +1282,12 @@
         <v>85</v>
       </c>
     </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating pre-installed SpreadsheetLisp.xlsx workbook with initial logical functions: _1_is_2., _1_is_not_2., _1_are_2., _Is_1_2?
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48B3964-AE06-4B5E-88E0-DBB0BD1C3277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B61680-2677-42E2-9E3C-649AB3CFAD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{97ED30AC-8B34-4AE5-86CC-C3EA482AB169}"/>
   </bookViews>
@@ -16,6 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_1_are_2.">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,FORMAT("{1} are {2}.",CAPITALIZE(_xlpm._1),_xlpm._2))</definedName>
+    <definedName name="_1_is_2.">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,FORMAT("{1} is {2}.",CAPITALIZE(_xlpm._1),_xlpm._2))</definedName>
+    <definedName name="_1_is_not_2.">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,FORMAT("{1} is not {2}.",CAPITALIZE(_xlpm._1),_xlpm._2))</definedName>
+    <definedName name="_Is_1_2?">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,_xlpm.knowledgebase,_xlfn.LET(_xlpm.affirmation,CONTAINS(_xlpm.knowledgebase,FORMAT("{1} is {2}.",CAPITALIZE(_xlpm._1),_xlpm._2)),_xlpm.negation,CONTAINS(_xlpm.knowledgebase,FORMAT("{1} is not {2}.",CAPITALIZE(_xlpm._1),_xlpm._2)),_xlpm.template,_xlfn.IFS(AND(_xlpm.affirmation,_xlpm.negation),"Yes and no. {1} simultaneously is and is not {2}.",_xlpm.affirmation,"Yes. {1} is {2}.",_xlpm.negation,"No. {1} is not {2}.",OTHERWISE,"Unknown."),FORMAT(_xlpm.template,_xlpm._1,_xlpm._2)))</definedName>
     <definedName name="ALL">_xlfn.LAMBDA(_xlpm.truth_values,AND(_xlpm.truth_values))</definedName>
     <definedName name="ALPHABET">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.alphabet,_xlfn.HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(_xlpm.vertical,NO),TRANSPOSE(_xlpm.alphabet),_xlpm.alphabet)))</definedName>
     <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN?(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
@@ -26,7 +30,7 @@
     <definedName name="CAR">_xlfn.LAMBDA(_xlpm.range,INDEX(_xlpm.range,1,1))</definedName>
     <definedName name="CASE">_xlfn.LAMBDA(_xlpm._1a,_xlpm._1b,_xlop._2a,_xlop._2b,_xlop._3a,_xlop._3b,_xlop._4a,_xlop._4b,_xlop._5a,_xlop._5b,_xlop._6a,_xlop._6b,_xlop._7a,_xlop._7b,_xlop._8a,_xlop._8b,_xlop._9a,_xlop._9b,_xlop._10a,_xlop._10b,_xlfn.LET(_xlpm.case1,EQUAL(_xlpm._1a, _xlpm._1b),_xlpm.case2,IFOMITTED(_xlpm._2a, TRUE, EQUAL(_xlpm._2a, _xlpm._2b)),_xlpm.case3,IFOMITTED(_xlpm._3a, TRUE, EQUAL(_xlpm._3a, _xlpm._3b)),_xlpm.case4,IFOMITTED(_xlpm._4a, TRUE, EQUAL(_xlpm._4a, _xlpm._4b)),_xlpm.case5,IFOMITTED(_xlpm._5a, TRUE, EQUAL(_xlpm._5a, _xlpm._5b)),_xlpm.case6,IFOMITTED(_xlpm._6a, TRUE, EQUAL(_xlpm._6a, _xlpm._6b)),_xlpm.case7,IFOMITTED(_xlpm._7a, TRUE, EQUAL(_xlpm._7a, _xlpm._7b)),_xlpm.case8,IFOMITTED(_xlpm._8a, TRUE, EQUAL(_xlpm._8a, _xlpm._8b)),_xlpm.case9,IFOMITTED(_xlpm._9a, TRUE, EQUAL(_xlpm._9a, _xlpm._9b)),_xlpm.case10,IFOMITTED(_xlpm._10a, TRUE, EQUAL(_xlpm._10a, _xlpm._10b)),AND(_xlpm.case1,_xlpm.case2,_xlpm.case3,_xlpm.case4,_xlpm.case5,_xlpm.case6,_xlpm.case7,_xlpm.case8,_xlpm.case9,_xlpm.case10)))</definedName>
     <definedName name="CDR">_xlfn.LAMBDA(_xlpm.range,IF(GREATERTHAN?(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.MAKEARRAY(1,DECREMENT(COLUMNS(_xlpm.range)),_xlfn.LAMBDA(_xlpm._row,_xlpm.col,INDEX(_xlpm.range,1,INCREMENT(_xlpm.col)))),_xlfn.MAKEARRAY(DECREMENT(ROWS(_xlpm.range)),1,_xlfn.LAMBDA(_xlpm.row,_xlpm._col,INDEX(_xlpm.range,INCREMENT(_xlpm.row),1)))))</definedName>
-    <definedName name="CELLNAME">_xlfn.LAMBDA(_xlop.reference,_xlop.absolute,_xlfn.LET(_xlpm.address,IFOMITTED(_xlpm.reference,CELL("address"),CELL("address",_xlpm.reference)),_xlpm.display_absolute,DEFAULT(_xlpm.absolute,NO),IF(_xlpm.display_absolute,_xlpm.address,SUBSTITUTE(_xlpm.address,"$",""))))</definedName>
+    <definedName name="CELLNAME">_xlfn.LAMBDA(_xlop.reference,_xlop.absolute?,_xlfn.LET(_xlpm.address,IFOMITTED(_xlpm.reference,CELL("address"),CELL("address",_xlpm.reference)),_xlpm.display_absolute,DEFAULT(_xlpm.absolute?,NO),IF(_xlpm.display_absolute,_xlpm.address,SUBSTITUTE(_xlpm.address,"$",""))))</definedName>
     <definedName name="COINTOSS">_xlfn.LAMBDA(PICK("Heads","Tails"))</definedName>
     <definedName name="COLUMNLETTER">_xlfn.LAMBDA(_xlop.cell_reference,TEXTBETWEEN(IFOMITTED(_xlpm.cell_reference,ADDRESS(ROW(),COLUMN()),ADDRESS(ROW(_xlpm.cell_reference),COLUMN(_xlpm.cell_reference))),"$","$"))</definedName>
     <definedName name="CONS">_xlfn.LAMBDA(_xlpm.value,_xlpm.range,IF(GREATERTHAN?(COLUMNS(_xlpm.range),ROWS(_xlpm.range)),_xlfn.HSTACK(_xlpm.value,_xlpm.range),_xlfn.VSTACK(_xlpm.value,_xlpm.range)))</definedName>
@@ -96,6 +100,8 @@
     <definedName name="SQUAREROOT">_xlfn.LAMBDA(_xlpm.x,POWER(_xlpm.x,0.5))</definedName>
     <definedName name="STATEMENT">_xlfn.LAMBDA(_xlpm.fragment1,_xlop.fragment2,_xlop.fragment3,_xlop.fragment4,_xlop.fragment5,_xlop.fragment6,_xlop.fragment7,_xlop.fragment8,_xlop.fragment9,_xlop.fragment10,_xlfn.LET(_xlpm.arity,ARITY(_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10),_xlpm.template,CHOOSE(_xlpm.arity,"('{1}').","('{1}', '{2}').","('{1}', '{2}', '{3}').","('{1}', '{2}', '{3}', '{4}').","('{1}', '{2}', '{3}', '{4}', '{5}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}').","('{1}', '{2}', '{3}', '{4}', '{5}', '{6}', '{7}', '{8}', '{9}', '{10}')."),FORMAT(_xlpm.template,_xlpm.fragment1,_xlpm.fragment2,_xlpm.fragment3,_xlpm.fragment4,_xlpm.fragment5,_xlpm.fragment6,_xlpm.fragment7,_xlpm.fragment8,_xlpm.fragment9,_xlpm.fragment10)))</definedName>
     <definedName name="TEXTBETWEEN">_xlfn.LAMBDA(_xlpm.source_text,_xlpm.first_boundary,_xlpm.second_boundary,_xlfn.LET(_xlpm.text_after_first_boundary,RIGHT(_xlpm.source_text,DIFFERENCE(LEN(_xlpm.source_text),DECREMENT(SUM(FIND(_xlpm.first_boundary,_xlpm.source_text),LEN(_xlpm.first_boundary))))),LEFT(_xlpm.text_after_first_boundary,DECREMENT(FIND(_xlpm.second_boundary,_xlpm.text_after_first_boundary)))))</definedName>
+    <definedName name="TEXTTOCOLUMNS">_xlfn.LAMBDA(_xlpm.text,_xlpm.delimiter,_xlfn.TEXTSPLIT(_xlpm.text,_xlpm.delimiter))</definedName>
+    <definedName name="TEXTTOROWS">_xlfn.LAMBDA(_xlpm.text,_xlpm.delimiter,TRANSPOSE(_xlfn.TEXTSPLIT(_xlpm.text,_xlpm.delimiter)))</definedName>
     <definedName name="TRIMALL">_xlfn.LAMBDA(_xlpm.range,_xlfn.MAKEARRAY(ROWS(_xlpm.range),COLUMNS(_xlpm.range),_xlfn.LAMBDA(_xlpm.row,_xlpm.col,TRIM(INDEX(_xlpm.range,_xlpm.row,_xlpm.col)))))</definedName>
     <definedName name="TRIMSPLIT">_xlfn.LAMBDA(_xlpm.source_text,_xlpm.split_at,_xlop.display_vertically,_xlfn.LET(_xlpm.result,TRIMALL(_xlfn.TEXTSPLIT(_xlpm.source_text,_xlpm.split_at)),IF(DEFAULT(_xlpm.display_vertically,FALSE),TRANSPOSE(_xlpm.result),_xlpm.result)))</definedName>
     <definedName name="TYPESTRING">_xlfn.LAMBDA(_xlpm.input,_xlop.recursive,_xlfn.SWITCH(TYPE(_xlpm.input),1,"Number",2,"String",4,"Boolean",16,"Error",64,IF(DEFAULT(_xlpm.recursive,FALSE),_xlfn.MAP(_xlpm.input,_xlfn.LAMBDA(_xlpm.each,TYPESTRING(_xlpm.each))),"Range"),128,"Function",OTHERWISE,"Unknown"))</definedName>
@@ -147,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>DEFINE(ALL,LAMBDA(truth_values,AND(truth_values)))</t>
   </si>
@@ -176,9 +182,6 @@
     <t>DEFINE(CASE,LAMBDA(_1a, _1b, [_2a], [_2b], [_3a], [_3b], [_4a], [_4b], [_5a], [_5b],[_6a], [_6b], [_7a], [_7b], [_8a], [_8b], [_9a], [_9b], [_10a], [_10b],LET(case1,EQUAL(_1a, _1b),case2,IFOMITTED(_2a, TRUE, EQUAL(_2a, _2b)),case3,IFOMITTED(_3a, TRUE, EQUAL(_3a, _3b)),case4,IFOMITTED(_4a, TRUE, EQUAL(_4a, _4b)),case5,IFOMITTED(_5a, TRUE, EQUAL(_5a, _5b)),case6,IFOMITTED(_6a, TRUE, EQUAL(_6a, _6b)),case7,IFOMITTED(_7a, TRUE, EQUAL(_7a, _7b)),case8,IFOMITTED(_8a, TRUE, EQUAL(_8a, _8b)),case9,IFOMITTED(_9a, TRUE, EQUAL(_9a, _9b)),case10,IFOMITTED(_10a, TRUE, EQUAL(_10a, _10b)),AND(case1,case2,case3,case4,case5,case6,case7,case8,case9,case10))))</t>
   </si>
   <si>
-    <t>DEFINE(CELLNAME,LAMBDA([reference],[absolute],LET(address,IFOMITTED(reference,CELL("address"),CELL("address",reference)),display_absolute,DEFAULT(absolute,NO),IF(display_absolute,address,SUBSTITUTE(address,"$","")))))</t>
-  </si>
-  <si>
     <t>DEFINE(CDR,LAMBDA(range,IF(GREATERTHAN?(COLUMNS(range),ROWS(range)),MAKEARRAY(1,DECREMENT(COLUMNS(range)),LAMBDA(_row,col,INDEX(range,1,INCREMENT(col)))),MAKEARRAY(DECREMENT(ROWS(range)),1,LAMBDA(row,_col,INDEX(range,INCREMENT(row),1))))))</t>
   </si>
   <si>
@@ -408,13 +411,34 @@
   </si>
   <si>
     <t>DEFINE(ZERO?,LAMBDA(x,EQUAL(x,0)))</t>
+  </si>
+  <si>
+    <t>DEFINE(_1_are_2.,LAMBDA(_1,_2,FORMAT("{1} are {2}.",CAPITALIZE(_1),_2)))</t>
+  </si>
+  <si>
+    <t>DEFINE(_1_is_2.,LAMBDA(_1,_2,FORMAT("{1} is {2}.",CAPITALIZE(_1),_2)))</t>
+  </si>
+  <si>
+    <t>DEFINE(_1_is_not_2.,LAMBDA(_1,_2,FORMAT("{1} is not {2}.",CAPITALIZE(_1),_2)))</t>
+  </si>
+  <si>
+    <t>DEFINE(_Is_1_2?,LAMBDA(_1,_2,knowledgebase,LET(affirmation,CONTAINS(knowledgebase,FORMAT("{1} is {2}.",CAPITALIZE(_1),_2)),negation,CONTAINS(knowledgebase,FORMAT("{1} is not {2}.",CAPITALIZE(_1),_2)),template,IFS(AND(affirmation,negation),"Yes and no. {1} simultaneously is and is not {2}.",affirmation,"Yes. {1} is {2}.",negation,"No. {1} is not {2}.",OTHERWISE,"Unknown."),FORMAT(template,_1,_2))))</t>
+  </si>
+  <si>
+    <t>DEFINE(CELLNAME,LAMBDA([reference],[absolute?],LET(address,IFOMITTED(reference,CELL("address"),CELL("address",reference)),display_absolute,DEFAULT(absolute?,NO),IF(display_absolute,address,SUBSTITUTE(address,"$","")))))</t>
+  </si>
+  <si>
+    <t>DEFINE(TEXTTOCOLUMNS,LAMBDA(text,delimiter,TEXTSPLIT(text,delimiter)))</t>
+  </si>
+  <si>
+    <t>DEFINE(TEXTTOROWS,LAMBDA(text,delimiter,TRANSPOSE(TEXTSPLIT(text,delimiter))))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +448,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -451,9 +483,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,502 +827,543 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDAF5AA-D241-40A4-8000-F3CC7642628A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="str" cm="1">
+      <c r="A1" s="3" t="str" cm="1">
         <f t="array" ref="A1">SL()</f>
         <v>0.9.0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="str" cm="1">
+      <c r="A3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="A3:A12" ca="1">FLIPCOIN(10)</f>
         <v>Tails</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+      <c r="A4" s="2" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+      <c r="A5" s="2" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+      <c r="A6" s="2" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f ca="1"/>
-        <v>Heads</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f ca="1"/>
-        <v>Heads</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f ca="1"/>
-        <v>Tails</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="str" cm="1">
+        <f t="array" ref="A14">_1_is_2.("Spreadsheet Lisp", "fun to use")</f>
+        <v>Spreadsheet Lisp is fun to use.</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="str" cm="1">
+        <f t="array" ref="A15">_Is_1_2?("Spreadsheet Lisp", "fun to use", A14)</f>
+        <v>Yes. Spreadsheet Lisp is fun to use.</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C173" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Capitalizing output of _Is_1_2? function
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B61680-2677-42E2-9E3C-649AB3CFAD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB064C4A-214A-4235-A26A-E9DEB56FD48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{97ED30AC-8B34-4AE5-86CC-C3EA482AB169}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="_1_are_2.">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,FORMAT("{1} are {2}.",CAPITALIZE(_xlpm._1),_xlpm._2))</definedName>
     <definedName name="_1_is_2.">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,FORMAT("{1} is {2}.",CAPITALIZE(_xlpm._1),_xlpm._2))</definedName>
     <definedName name="_1_is_not_2.">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,FORMAT("{1} is not {2}.",CAPITALIZE(_xlpm._1),_xlpm._2))</definedName>
-    <definedName name="_Is_1_2?">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,_xlpm.knowledgebase,_xlfn.LET(_xlpm.affirmation,CONTAINS(_xlpm.knowledgebase,FORMAT("{1} is {2}.",CAPITALIZE(_xlpm._1),_xlpm._2)),_xlpm.negation,CONTAINS(_xlpm.knowledgebase,FORMAT("{1} is not {2}.",CAPITALIZE(_xlpm._1),_xlpm._2)),_xlpm.template,_xlfn.IFS(AND(_xlpm.affirmation,_xlpm.negation),"Yes and no. {1} simultaneously is and is not {2}.",_xlpm.affirmation,"Yes. {1} is {2}.",_xlpm.negation,"No. {1} is not {2}.",OTHERWISE,"Unknown."),FORMAT(_xlpm.template,_xlpm._1,_xlpm._2)))</definedName>
+    <definedName name="_Is_1_2?">_xlfn.LAMBDA(_xlpm._1,_xlpm._2,_xlpm.knowledgebase,_xlfn.LET(_xlpm.affirmation,CONTAINS(_xlpm.knowledgebase,FORMAT("{1} is {2}.",CAPITALIZE(_xlpm._1),_xlpm._2)),_xlpm.negation,CONTAINS(_xlpm.knowledgebase,FORMAT("{1} is not {2}.",CAPITALIZE(_xlpm._1),_xlpm._2)),_xlpm.template,_xlfn.IFS(AND(_xlpm.affirmation,_xlpm.negation),"Yes and no. {1} simultaneously is and is not {2}.",_xlpm.affirmation,"Yes. {1} is {2}.",_xlpm.negation,"No. {1} is not {2}.",OTHERWISE,"Unknown."),FORMAT(_xlpm.template,CAPITALIZE(_xlpm._1),_xlpm._2)))</definedName>
     <definedName name="ALL">_xlfn.LAMBDA(_xlpm.truth_values,AND(_xlpm.truth_values))</definedName>
     <definedName name="ALPHABET">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.alphabet,_xlfn.HSTACK({"A","B","C","D","E","F"},{"G","H","I","J","K","L"},{"M","N","O","P","Q","R"},{"S","T","U","V","W","X","Y","Z"}),IF(DEFAULT(_xlpm.vertical,NO),TRANSPOSE(_xlpm.alphabet),_xlpm.alphabet)))</definedName>
     <definedName name="APPEND">_xlfn.LAMBDA(_xlpm.head,_xlpm.body,IF(GREATERTHAN?(COLUMNS(_xlpm.body),ROWS(_xlpm.body)),_xlfn.HSTACK(_xlpm.head,_xlpm.body),_xlfn.VSTACK(_xlpm.head,_xlpm.body)))</definedName>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>DEFINE(ALL,LAMBDA(truth_values,AND(truth_values)))</t>
   </si>
@@ -432,6 +432,12 @@
   </si>
   <si>
     <t>DEFINE(TEXTTOROWS,LAMBDA(text,delimiter,TRANSPOSE(TEXTSPLIT(text,delimiter))))</t>
+  </si>
+  <si>
+    <t>Water is wet.</t>
+  </si>
+  <si>
+    <t>Water is not wet.</t>
   </si>
 </sst>
 </file>
@@ -858,7 +864,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -894,7 +900,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f ca="1"/>
-        <v>Heads</v>
+        <v>Tails</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
@@ -903,7 +909,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
         <f ca="1"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -941,42 +947,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="str" cm="1">
+        <f t="array" ref="A19">_Is_1_2?("water", "wet", A17:A18)</f>
+        <v>Yes and no. Water simultaneously is and is not wet.</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Removing the three ISO/INTL functions which were unrecognized by Excel to fix BUILTINS composition
</commit_message>
<xml_diff>
--- a/lisp/SpreadsheetLisp.xlsx
+++ b/lisp/SpreadsheetLisp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragti\Documents\SpreadsheetInstitute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6ACEFD-87F9-40D5-A4CB-9C40EFB9B892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A9F04B-E84E-43B0-B614-1876AA087520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{94612E55-53D2-476D-ADAE-92312FD76347}"/>
   </bookViews>
@@ -35,11 +35,11 @@
     <definedName name="BUILTINS.F">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("F.DIST", _xleta.F.DIST),_xlfn.HSTACK("F.DIST.RT", _xleta.F.DIST.RT),_xlfn.HSTACK("F.INV", _xleta.F.INV),_xlfn.HSTACK("F.INV.RT", _xleta.F.INV.RT),_xlfn.HSTACK("F.TEST", _xleta.F.TEST),_xlfn.HSTACK("FACT", _xleta.FACT),_xlfn.HSTACK("FACTDOUBLE", _xleta.FACTDOUBLE),_xlfn.HSTACK("FALSE", FALSE),_xlfn.HSTACK("FDIST", _xleta.FDIST),_xlfn.HSTACK("FIELDFUNCTION", _xleta.FIELDFUNCTION),_xlfn.HSTACK("FIELDVALUE", _xleta.FIELDVALUE),_xlfn.HSTACK("FILTER", _xleta.FILTER),_xlfn.HSTACK("FILTERXML", _xleta.FILTERXML),_xlfn.HSTACK("FIND", _xleta.FIND),_xlfn.HSTACK("FINDB", _xleta.FINDB),_xlfn.HSTACK("FINV", _xleta.FINV),_xlfn.HSTACK("FISHER", _xleta.FISHER),_xlfn.HSTACK("FISHERINV", _xleta.FISHERINV),_xlfn.HSTACK("FIXED", _xleta.FIXED),_xlfn.HSTACK("FLOOR", _xleta.FLOOR),_xlfn.HSTACK("FLOOR.MATH", _xleta.FLOOR.MATH),_xlfn.HSTACK("FLOOR.PRECISE", _xleta.FLOOR.PRECISE),_xlfn.HSTACK("FORECAST", _xleta.FORECAST),_xlfn.HSTACK("FORECAST.ETS", _xleta.FORECAST.ETS),_xlfn.HSTACK("FORECAST.ETS.CONFINT", _xleta.FORECAST.ETS.CONFINT),_xlfn.HSTACK("FORECAST.ETS.SEASONALITY", _xleta.FORECAST.ETS.SEASONALITY),_xlfn.HSTACK("FORECAST.ETS.STAT", _xleta.FORECAST.ETS.STAT),_xlfn.HSTACK("FORECAST.LINEAR", _xleta.FORECAST.LINEAR),_xlfn.HSTACK("FORMULATEXT", _xleta.FORMULATEXT),_xlfn.HSTACK("FREQUENCY", _xleta.FREQUENCY),_xlfn.HSTACK("FTEST", _xleta.FTEST),_xlfn.HSTACK("FV", _xleta.FV),_xlfn.HSTACK("FVSCHEDULE", _xleta.FVSCHEDULE)))</definedName>
     <definedName name="BUILTINS.G">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("GAMMA", _xleta.GAMMA),_xlfn.HSTACK("GAMMA.DIST", _xleta.GAMMA.DIST),_xlfn.HSTACK("GAMMA.INV", _xleta.GAMMA.INV),_xlfn.HSTACK("GAMMADIST", _xleta.GAMMADIST),_xlfn.HSTACK("GAMMAINV", _xleta.GAMMAINV),_xlfn.HSTACK("GAMMALN", _xleta.GAMMALN),_xlfn.HSTACK("GAMMALN.PRECISE", _xleta.GAMMALN.PRECISE),_xlfn.HSTACK("GAUSS", _xleta.GAUSS),_xlfn.HSTACK("GCD", _xleta.GCD),_xlfn.HSTACK("GEOMEAN", _xleta.GEOMEAN),_xlfn.HSTACK("GESTEP", _xleta.GESTEP),_xlfn.HSTACK("GETPIVOTDATA", _xleta.GETPIVOTDATA),_xlfn.HSTACK("GROUPBY", _xleta.GROUPBY),_xlfn.HSTACK("GROWTH", _xleta.GROWTH)))</definedName>
     <definedName name="BUILTINS.H">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("HARMEAN", _xleta.HARMEAN),_xlfn.HSTACK("HEX2BIN", _xleta.HEX2BIN),_xlfn.HSTACK("HEX2DEC", _xleta.HEX2DEC),_xlfn.HSTACK("HEX2OCT", _xleta.HEX2OCT),_xlfn.HSTACK("HLOOKUP", _xleta.HLOOKUP),_xlfn.HSTACK("HOUR", _xleta.HOUR),_xlfn.HSTACK("HSTACK", _xleta.HSTACK),_xlfn.HSTACK("HYPERLINK", _xleta.HYPERLINK),_xlfn.HSTACK("HYPGEOM.DIST", _xleta.HYPGEOM.DIST),_xlfn.HSTACK("HYPGEOMDIST", _xleta.HYPGEOMDIST)))</definedName>
-    <definedName name="BUILTINS.I">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("IF", _xleta.IF),_xlfn.HSTACK("IFERROR", _xleta.IFERROR),_xlfn.HSTACK("IFNA", _xleta.IFNA),_xlfn.HSTACK("IFS", _xleta.IFS),_xlfn.HSTACK("IMABS", _xleta.IMABS),_xlfn.HSTACK("IMAGE", _xleta.IMAGE),_xlfn.HSTACK("IMAGINARY", _xleta.IMAGINARY),_xlfn.HSTACK("IMARGUMENT", _xleta.IMARGUMENT),_xlfn.HSTACK("IMCONJUGATE", _xleta.IMCONJUGATE),_xlfn.HSTACK("IMCOS", _xleta.IMCOS),_xlfn.HSTACK("IMCOSH", _xleta.IMCOSH),_xlfn.HSTACK("IMCOT", _xleta.IMCOT),_xlfn.HSTACK("IMCSC", _xleta.IMCSC),_xlfn.HSTACK("IMCSCH", _xleta.IMCSCH),_xlfn.HSTACK("IMDIV", _xleta.IMDIV),_xlfn.HSTACK("IMEXP", _xleta.IMEXP),_xlfn.HSTACK("IMLN", _xleta.IMLN),_xlfn.HSTACK("IMLOG10", _xleta.IMLOG10),_xlfn.HSTACK("IMLOG2", _xleta.IMLOG2),_xlfn.HSTACK("IMPOWER", _xleta.IMPOWER),_xlfn.HSTACK("IMPRODUCT", _xleta.IMPRODUCT),_xlfn.HSTACK("IMREAL", _xleta.IMREAL),_xlfn.HSTACK("IMSEC", _xleta.IMSEC),_xlfn.HSTACK("IMSECH", _xleta.IMSECH),_xlfn.HSTACK("IMSIN", _xleta.IMSIN),_xlfn.HSTACK("IMSINH", _xleta.IMSINH),_xlfn.HSTACK("IMSQRT", _xleta.IMSQRT),_xlfn.HSTACK("IMSUB", _xleta.IMSUB),_xlfn.HSTACK("IMSUM", _xleta.IMSUM),_xlfn.HSTACK("IMTAN", _xleta.IMTAN),_xlfn.HSTACK("INDEX", _xleta.INDEX),_xlfn.HSTACK("INDIRECT", _xleta.INDIRECT),_xlfn.HSTACK("INFO", _xleta.INFO),_xlfn.HSTACK("INT", _xleta.INT),_xlfn.HSTACK("INTERCEPT", _xleta.INTERCEPT),_xlfn.HSTACK("INTRATE", _xleta.INTRATE),_xlfn.HSTACK("IPMT", _xleta.IPMT),_xlfn.HSTACK("IRR", _xleta.IRR),_xlfn.HSTACK("ISBLANK", _xleta.ISBLANK),_xlfn.HSTACK("ISERR", _xleta.ISERR),_xlfn.HSTACK("ISERROR", _xleta.ISERROR),_xlfn.HSTACK("ISEVEN", _xleta.ISEVEN),_xlfn.HSTACK("ISFORMULA", _xleta.ISFORMULA),_xlfn.HSTACK("ISLOGICAL", _xleta.ISLOGICAL),_xlfn.HSTACK("ISNA", _xleta.ISNA),_xlfn.HSTACK("ISNONTEXT", _xleta.ISNONTEXT),_xlfn.HSTACK("ISNUMBER", _xleta.ISNUMBER),_xlfn.HSTACK("ISO.CEILING", ISO.CEILING),_xlfn.HSTACK("ISODD", _xleta.ISODD),_xlfn.HSTACK("ISOMITTED", _xleta.ISOMITTED),_xlfn.HSTACK("ISOWEEKNUM", _xleta.ISOWEEKNUM),_xlfn.HSTACK("ISPMT", _xleta.ISPMT),_xlfn.HSTACK("ISREF", _xleta.ISREF),_xlfn.HSTACK("ISTEXT", _xleta.ISTEXT)))</definedName>
+    <definedName name="BUILTINS.I">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("IF", _xleta.IF),_xlfn.HSTACK("IFERROR", _xleta.IFERROR),_xlfn.HSTACK("IFNA", _xleta.IFNA),_xlfn.HSTACK("IFS", _xleta.IFS),_xlfn.HSTACK("IMABS", _xleta.IMABS),_xlfn.HSTACK("IMAGE", _xleta.IMAGE),_xlfn.HSTACK("IMAGINARY", _xleta.IMAGINARY),_xlfn.HSTACK("IMARGUMENT", _xleta.IMARGUMENT),_xlfn.HSTACK("IMCONJUGATE", _xleta.IMCONJUGATE),_xlfn.HSTACK("IMCOS", _xleta.IMCOS),_xlfn.HSTACK("IMCOSH", _xleta.IMCOSH),_xlfn.HSTACK("IMCOT", _xleta.IMCOT),_xlfn.HSTACK("IMCSC", _xleta.IMCSC),_xlfn.HSTACK("IMCSCH", _xleta.IMCSCH),_xlfn.HSTACK("IMDIV", _xleta.IMDIV),_xlfn.HSTACK("IMEXP", _xleta.IMEXP),_xlfn.HSTACK("IMLN", _xleta.IMLN),_xlfn.HSTACK("IMLOG10", _xleta.IMLOG10),_xlfn.HSTACK("IMLOG2", _xleta.IMLOG2),_xlfn.HSTACK("IMPOWER", _xleta.IMPOWER),_xlfn.HSTACK("IMPRODUCT", _xleta.IMPRODUCT),_xlfn.HSTACK("IMREAL", _xleta.IMREAL),_xlfn.HSTACK("IMSEC", _xleta.IMSEC),_xlfn.HSTACK("IMSECH", _xleta.IMSECH),_xlfn.HSTACK("IMSIN", _xleta.IMSIN),_xlfn.HSTACK("IMSINH", _xleta.IMSINH),_xlfn.HSTACK("IMSQRT", _xleta.IMSQRT),_xlfn.HSTACK("IMSUB", _xleta.IMSUB),_xlfn.HSTACK("IMSUM", _xleta.IMSUM),_xlfn.HSTACK("IMTAN", _xleta.IMTAN),_xlfn.HSTACK("INDEX", _xleta.INDEX),_xlfn.HSTACK("INDIRECT", _xleta.INDIRECT),_xlfn.HSTACK("INFO", _xleta.INFO),_xlfn.HSTACK("INT", _xleta.INT),_xlfn.HSTACK("INTERCEPT", _xleta.INTERCEPT),_xlfn.HSTACK("INTRATE", _xleta.INTRATE),_xlfn.HSTACK("IPMT", _xleta.IPMT),_xlfn.HSTACK("IRR", _xleta.IRR),_xlfn.HSTACK("ISBLANK", _xleta.ISBLANK),_xlfn.HSTACK("ISERR", _xleta.ISERR),_xlfn.HSTACK("ISERROR", _xleta.ISERROR),_xlfn.HSTACK("ISEVEN", _xleta.ISEVEN),_xlfn.HSTACK("ISFORMULA", _xleta.ISFORMULA),_xlfn.HSTACK("ISLOGICAL", _xleta.ISLOGICAL),_xlfn.HSTACK("ISNA", _xleta.ISNA),_xlfn.HSTACK("ISNONTEXT", _xleta.ISNONTEXT),_xlfn.HSTACK("ISNUMBER", _xleta.ISNUMBER),_xlfn.HSTACK("ISODD", _xleta.ISODD),_xlfn.HSTACK("ISOMITTED", _xleta.ISOMITTED),_xlfn.HSTACK("ISOWEEKNUM", _xleta.ISOWEEKNUM),_xlfn.HSTACK("ISPMT", _xleta.ISPMT),_xlfn.HSTACK("ISREF", _xleta.ISREF),_xlfn.HSTACK("ISTEXT", _xleta.ISTEXT)))</definedName>
     <definedName name="BUILTINS.K">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("KURT", _xleta.KURT)))</definedName>
     <definedName name="BUILTINS.L">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("LARGE", _xleta.LARGE),_xlfn.HSTACK("LCM", _xleta.LCM),_xlfn.HSTACK("LEFT", _xleta.LEFT),_xlfn.HSTACK("LEFTB", _xleta.LEFTB),_xlfn.HSTACK("LEN", _xleta.LEN),_xlfn.HSTACK("LENB", _xleta.LENB),_xlfn.HSTACK("LINEST", _xleta.LINEST),_xlfn.HSTACK("LN", _xleta.LN),_xlfn.HSTACK("LOG", _xleta.LOG),_xlfn.HSTACK("LOG10", Sheet1!LOG10),_xlfn.HSTACK("LOGEST", _xleta.LOGEST),_xlfn.HSTACK("LOGINV", _xleta.LOGINV),_xlfn.HSTACK("LOGNORM.DIST", _xleta.LOGNORM.DIST),_xlfn.HSTACK("LOGNORM.INV", _xleta.LOGNORM.INV),_xlfn.HSTACK("LOGNORMDIST", _xleta.LOGNORMDIST),_xlfn.HSTACK("LOOKUP", _xleta.LOOKUP),_xlfn.HSTACK("LOWER", _xleta.LOWER)))</definedName>
     <definedName name="BUILTINS.M">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("MAKEARRAY", _xleta.MAKEARRAY),_xlfn.HSTACK("MAP", _xleta.MAP),_xlfn.HSTACK("MATCH", _xleta.MATCH),_xlfn.HSTACK("MAX", _xleta.MAX),_xlfn.HSTACK("MAXA", _xleta.MAXA),_xlfn.HSTACK("MAXIFS", _xleta.MAXIFS),_xlfn.HSTACK("MDETERM", _xleta.MDETERM),_xlfn.HSTACK("MDURATION", _xleta.MDURATION),_xlfn.HSTACK("MEDIAN", _xleta.MEDIAN),_xlfn.HSTACK("MID", _xleta.MID),_xlfn.HSTACK("MIDB", _xleta.MIDB),_xlfn.HSTACK("MIN", _xleta.MIN),_xlfn.HSTACK("MINA", _xleta.MINA),_xlfn.HSTACK("MINIFS", _xleta.MINIFS),_xlfn.HSTACK("MINUTE", _xleta.MINUTE),_xlfn.HSTACK("MINVERSE", _xleta.MINVERSE),_xlfn.HSTACK("MIRR", _xleta.MIRR),_xlfn.HSTACK("MMULT", _xleta.MMULT),_xlfn.HSTACK("MOD", _xleta.MOD),_xlfn.HSTACK("MODE", _xleta.MODE),_xlfn.HSTACK("MODE.MULT", _xleta.MODE.MULT),_xlfn.HSTACK("MODE.SNGL", _xleta.MODE.SNGL),_xlfn.HSTACK("MONTH", _xleta.MONTH),_xlfn.HSTACK("MROUND", _xleta.MROUND),_xlfn.HSTACK("MULTINOMIAL", _xleta.MULTINOMIAL),_xlfn.HSTACK("MUNIT", _xleta.MUNIT)))</definedName>
-    <definedName name="BUILTINS.N">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("N", _xleta.N),_xlfn.HSTACK("NA", _xleta.NA),_xlfn.HSTACK("NEGBINOM.DIST", _xleta.NEGBINOM.DIST),_xlfn.HSTACK("NEGBINOMDIST", _xleta.NEGBINOMDIST),_xlfn.HSTACK("NETWORKDAYS", _xleta.NETWORKDAYS),_xlfn.HSTACK("NETWORKDAYS.INTL", NETWORKDAYS.INTL),_xlfn.HSTACK("NOMINAL", _xleta.NOMINAL),_xlfn.HSTACK("NORM.DIST", _xleta.NORM.DIST),_xlfn.HSTACK("NORM.INV", _xleta.NORM.INV),_xlfn.HSTACK("NORM.S.DIST", _xleta.NORM.S.DIST),_xlfn.HSTACK("NORM.S.INV", _xleta.NORM.S.INV),_xlfn.HSTACK("NORMDIST", _xleta.NORMDIST),_xlfn.HSTACK("NORMINV", _xleta.NORMINV),_xlfn.HSTACK("NORMSDIST", _xleta.NORMSDIST),_xlfn.HSTACK("NORMSINV", _xleta.NORMSINV),_xlfn.HSTACK("NOT", _xleta.NOT),_xlfn.HSTACK("NOW", _xleta.NOW),_xlfn.HSTACK("NPER", _xleta.NPER),_xlfn.HSTACK("NPV", _xleta.NPV),_xlfn.HSTACK("NUMBERVALUE", _xleta.NUMBERVALUE)))</definedName>
+    <definedName name="BUILTINS.N">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("N", _xleta.N),_xlfn.HSTACK("NA", _xleta.NA),_xlfn.HSTACK("NEGBINOM.DIST", _xleta.NEGBINOM.DIST),_xlfn.HSTACK("NEGBINOMDIST", _xleta.NEGBINOMDIST),_xlfn.HSTACK("NETWORKDAYS", _xleta.NETWORKDAYS),_xlfn.HSTACK("NOMINAL", _xleta.NOMINAL),_xlfn.HSTACK("NORM.DIST", _xleta.NORM.DIST),_xlfn.HSTACK("NORM.INV", _xleta.NORM.INV),_xlfn.HSTACK("NORM.S.DIST", _xleta.NORM.S.DIST),_xlfn.HSTACK("NORM.S.INV", _xleta.NORM.S.INV),_xlfn.HSTACK("NORMDIST", _xleta.NORMDIST),_xlfn.HSTACK("NORMINV", _xleta.NORMINV),_xlfn.HSTACK("NORMSDIST", _xleta.NORMSDIST),_xlfn.HSTACK("NORMSINV", _xleta.NORMSINV),_xlfn.HSTACK("NOT", _xleta.NOT),_xlfn.HSTACK("NOW", _xleta.NOW),_xlfn.HSTACK("NPER", _xleta.NPER),_xlfn.HSTACK("NPV", _xleta.NPV),_xlfn.HSTACK("NUMBERVALUE", _xleta.NUMBERVALUE)))</definedName>
     <definedName name="BUILTINS.O">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("OCT2BIN", _xleta.OCT2BIN),_xlfn.HSTACK("OCT2DEC", _xleta.OCT2DEC),_xlfn.HSTACK("OCT2HEX", _xleta.OCT2HEX),_xlfn.HSTACK("ODD", _xleta.ODD),_xlfn.HSTACK("ODDFPRICE", _xleta.ODDFPRICE),_xlfn.HSTACK("ODDFYIELD", _xleta.ODDFYIELD),_xlfn.HSTACK("ODDLPRICE", _xleta.ODDLPRICE),_xlfn.HSTACK("ODDLYIELD", _xleta.ODDLYIELD),_xlfn.HSTACK("OFFSET", _xleta.OFFSET),_xlfn.HSTACK("OR", _xleta.OR)))</definedName>
     <definedName name="BUILTINS.P">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("PDURATION", _xleta.PDURATION),_xlfn.HSTACK("PEARSON", _xleta.PEARSON),_xlfn.HSTACK("PERCENTILE", _xleta.PERCENTILE),_xlfn.HSTACK("PERCENTILE.EXC", _xleta.PERCENTILE.EXC),_xlfn.HSTACK("PERCENTILE.INC", _xleta.PERCENTILE.INC),_xlfn.HSTACK("PERCENTOF", _xleta.PERCENTOF),_xlfn.HSTACK("PERCENTRANK", _xleta.PERCENTRANK),_xlfn.HSTACK("PERCENTRANK.EXC", _xleta.PERCENTRANK.EXC),_xlfn.HSTACK("PERCENTRANK.INC", _xleta.PERCENTRANK.INC),_xlfn.HSTACK("PERMUT", _xleta.PERMUT),_xlfn.HSTACK("PERMUTATIONA", _xleta.PERMUTATIONA),_xlfn.HSTACK("PHI", _xleta.PHI),_xlfn.HSTACK("PHONETIC", _xleta.PHONETIC),_xlfn.HSTACK("PI", _xleta.PI),_xlfn.HSTACK("PIVOTBY", _xleta.PIVOTBY),_xlfn.HSTACK("PMT", _xleta.PMT),_xlfn.HSTACK("POISSON", _xleta.POISSON),_xlfn.HSTACK("POISSON.DIST", _xleta.POISSON.DIST),_xlfn.HSTACK("POWER", _xleta.POWER),_xlfn.HSTACK("PPMT", _xleta.PPMT),_xlfn.HSTACK("PRICE", _xleta.PRICE),_xlfn.HSTACK("PRICEDISC", _xleta.PRICEDISC),_xlfn.HSTACK("PRICEMAT", _xleta.PRICEMAT),_xlfn.HSTACK("PROB", _xleta.PROB),_xlfn.HSTACK("PRODUCT", _xleta.PRODUCT),_xlfn.HSTACK("PROPER", _xleta.PROPER),_xlfn.HSTACK("PV", _xleta.PV)))</definedName>
     <definedName name="BUILTINS.Q">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("QUARTILE", _xleta.QUARTILE),_xlfn.HSTACK("QUARTILE.EXC", _xleta.QUARTILE.EXC),_xlfn.HSTACK("QUARTILE.INC", _xleta.QUARTILE.INC),_xlfn.HSTACK("QUOTIENT", _xleta.QUOTIENT)))</definedName>
@@ -48,7 +48,7 @@
     <definedName name="BUILTINS.T">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("T", _xleta.T),_xlfn.HSTACK("T.DIST", _xleta.T.DIST),_xlfn.HSTACK("T.DIST.2T", _xleta.T.DIST.2T),_xlfn.HSTACK("T.DIST.RT", _xleta.T.DIST.RT),_xlfn.HSTACK("T.INV", _xleta.T.INV),_xlfn.HSTACK("T.INV.2T", _xleta.T.INV.2T),_xlfn.HSTACK("T.TEST", _xleta.T.TEST),_xlfn.HSTACK("TAKE", _xleta.TAKE),_xlfn.HSTACK("TAN", _xleta.TAN),_xlfn.HSTACK("TANH", _xleta.TANH),_xlfn.HSTACK("TBILLEQ", _xleta.TBILLEQ),_xlfn.HSTACK("TBILLPRICE", _xleta.TBILLPRICE),_xlfn.HSTACK("TBILLYIELD", _xleta.TBILLYIELD),_xlfn.HSTACK("TDIST", _xleta.TDIST),_xlfn.HSTACK("TEXT", _xleta.TEXT),_xlfn.HSTACK("TEXTAFTER", _xleta.TEXTAFTER),_xlfn.HSTACK("TEXTBEFORE", _xleta.TEXTBEFORE),_xlfn.HSTACK("TEXTJOIN", _xleta.TEXTJOIN),_xlfn.HSTACK("TEXTSPLIT", _xleta.TEXTSPLIT),_xlfn.HSTACK("TIME", _xleta.TIME),_xlfn.HSTACK("TIMEVALUE", _xleta.TIMEVALUE),_xlfn.HSTACK("TINV", _xleta.TINV),_xlfn.HSTACK("TOCOL", _xleta.TOCOL),_xlfn.HSTACK("TODAY", _xleta.TODAY),_xlfn.HSTACK("TOROW", _xleta.TOROW),_xlfn.HSTACK("TRANSLATE", _xleta.TRANSLATE),_xlfn.HSTACK("TRANSPOSE", _xleta.TRANSPOSE),_xlfn.HSTACK("TREND", _xleta.TREND),_xlfn.HSTACK("TRIM", _xleta.TRIM),_xlfn.HSTACK("TRIMMEAN", _xleta.TRIMMEAN),_xlfn.HSTACK("TRIMRANGE", _xleta.TRIMRANGE),_xlfn.HSTACK("TRUE", TRUE),_xlfn.HSTACK("TRUNC", _xleta.TRUNC),_xlfn.HSTACK("TTEST", _xleta.TTEST),_xlfn.HSTACK("TYPE", _xleta.TYPE)))</definedName>
     <definedName name="BUILTINS.U">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("UNICHAR", _xleta.UNICHAR),_xlfn.HSTACK("UNICODE", _xleta.UNICODE),_xlfn.HSTACK("UNIQUE", _xleta.UNIQUE),_xlfn.HSTACK("UPPER", _xleta.UPPER)))</definedName>
     <definedName name="BUILTINS.V">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("VALUE", _xleta.VALUE),_xlfn.HSTACK("VALUETOTEXT", _xleta.VALUETOTEXT),_xlfn.HSTACK("VAR", _xleta.VAR),_xlfn.HSTACK("VAR.P", _xleta.VAR.P),_xlfn.HSTACK("VAR.S", _xleta.VAR.S),_xlfn.HSTACK("VARA", _xleta.VARA),_xlfn.HSTACK("VARP", _xleta.VARP),_xlfn.HSTACK("VARPA", _xleta.VARPA),_xlfn.HSTACK("VDB", _xleta.VDB),_xlfn.HSTACK("VLOOKUP", _xleta.VLOOKUP),_xlfn.HSTACK("VSTACK", _xleta.VSTACK)))</definedName>
-    <definedName name="BUILTINS.W">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("WEBSERVICE", _xleta.WEBSERVICE),_xlfn.HSTACK("WEEKDAY", _xleta.WEEKDAY),_xlfn.HSTACK("WEEKNUM", _xleta.WEEKNUM),_xlfn.HSTACK("WEIBULL", _xleta.WEIBULL),_xlfn.HSTACK("WEIBULL.DIST", _xleta.WEIBULL.DIST),_xlfn.HSTACK("WORKDAY", _xleta.WORKDAY),_xlfn.HSTACK("WORKDAY.INTL", WORKDAY.INTL),_xlfn.HSTACK("WRAPCOLS", _xleta.WRAPCOLS),_xlfn.HSTACK("WRAPROWS", _xleta.WRAPROWS)))</definedName>
+    <definedName name="BUILTINS.W">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("WEBSERVICE", _xleta.WEBSERVICE),_xlfn.HSTACK("WEEKDAY", _xleta.WEEKDAY),_xlfn.HSTACK("WEEKNUM", _xleta.WEEKNUM),_xlfn.HSTACK("WEIBULL", _xleta.WEIBULL),_xlfn.HSTACK("WEIBULL.DIST", _xleta.WEIBULL.DIST),_xlfn.HSTACK("WORKDAY", _xleta.WORKDAY),_xlfn.HSTACK("WRAPCOLS", _xleta.WRAPCOLS),_xlfn.HSTACK("WRAPROWS", _xleta.WRAPROWS)))</definedName>
     <definedName name="BUILTINS.X">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("XIRR", _xleta.XIRR),_xlfn.HSTACK("XLOOKUP", _xleta.XLOOKUP),_xlfn.HSTACK("XMATCH", _xleta.XMATCH),_xlfn.HSTACK("XNPV", _xleta.XNPV),_xlfn.HSTACK("XOR", _xleta.XOR)))</definedName>
     <definedName name="BUILTINS.Y">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("YEAR", _xleta.YEAR),_xlfn.HSTACK("YEARFRAC", _xleta.YEARFRAC),_xlfn.HSTACK("YIELD", _xleta.YIELD),_xlfn.HSTACK("YIELDDISC", _xleta.YIELDDISC),_xlfn.HSTACK("YIELDMAT", _xleta.YIELDMAT)))</definedName>
     <definedName name="BUILTINS.Z">_xlfn.LAMBDA(_xlfn.VSTACK(_xlfn.HSTACK("Z.TEST", _xleta.Z.TEST),_xlfn.HSTACK("ZTEST", _xleta.ZTEST)))</definedName>
@@ -84,7 +84,7 @@
     <definedName name="FOREACH">_xlfn.LAMBDA(_xlpm.range,_xlpm.function_to_apply,_xlfn.MAP(_xlpm.range,_xlpm.function_to_apply))</definedName>
     <definedName name="FORMAT">_xlfn.LAMBDA(_xlpm.template_text,_xlpm.first_value,_xlop.second_value,_xlop.third_value,_xlop.fourth_value,_xlop.fifth_value,_xlop.sixth_value,_xlop.seventh_value,_xlop.eigth_value,_xlop.ninth_value,_xlop.tenth_value,_xlfn.LET(_xlpm._after1,SUBSTITUTE(_xlpm.template_text,"{1}", _xlpm.first_value),_xlpm._after2,IF(PROVIDED?(_xlpm.second_value),SUBSTITUTE(_xlpm._after1,"{2}", _xlpm.second_value),_xlpm._after1),_xlpm._after3,IF(PROVIDED?(_xlpm.third_value),SUBSTITUTE(_xlpm._after2,"{3}", _xlpm.third_value),_xlpm._after2),_xlpm._after4,IF(PROVIDED?(_xlpm.fourth_value),SUBSTITUTE(_xlpm._after3,"{4}", _xlpm.fourth_value),_xlpm._after3),_xlpm._after5,IF(PROVIDED?(_xlpm.fifth_value),SUBSTITUTE(_xlpm._after4,"{5}", _xlpm.fifth_value),_xlpm._after4),_xlpm._after6,IF(PROVIDED?(_xlpm.sixth_value),SUBSTITUTE(_xlpm._after5,"{6}", _xlpm.sixth_value),_xlpm._after5),_xlpm._after7,IF(PROVIDED?(_xlpm.seventh_value),SUBSTITUTE(_xlpm._after6,"{7}", _xlpm.seventh_value),_xlpm._after6),_xlpm._after8,IF(PROVIDED?(_xlpm.eigth_value),SUBSTITUTE(_xlpm._after7,"{8}", _xlpm.eigth_value),_xlpm._after7),_xlpm._after9,IF(PROVIDED?(_xlpm.ninth_value),SUBSTITUTE(_xlpm._after8,"{9}", _xlpm.ninth_value),_xlpm._after8),IF(PROVIDED?(_xlpm.tenth_value),SUBSTITUTE(_xlpm._after9,"{10}", _xlpm.tenth_value),_xlpm._after9)))</definedName>
     <definedName name="FULLDECK">_xlfn.LAMBDA(_xlop.vertical,_xlfn.LET(_xlpm.full_deck,_xlfn.HSTACK({"AS","KS","QS","JS","XS","9S","8S","7S","6S","5S","4S","3S","2S"},{"AH","KH","QH","JH","XH","9H","8H","7H","6H","5H","4H","3H","2H"},{"AD","KD","QD","JD","XD","9D","8D","7D","6D","5D","4D","3D","2D"},{"AC","KC","QC","JC","XC","9C","8C","7C","6C","5C","4C","3C","2C"}),IF(DEFAULT(_xlpm.vertical,FALSE),TRANSPOSE(_xlpm.full_deck),_xlpm.full_deck)))</definedName>
-    <definedName name="FUNCTION">_xlfn.LAMBDA(_xlop.name,VLOOKUP(DEFAULT(_xlpm.name, "FUNCTION"),FUNCTIONS(),2,0))</definedName>
+    <definedName name="FUNCTION">_xlfn.LAMBDA(_xlop.name,VLOOKUP(UPPER(DEFAULT(_xlpm.name, "FUNCTION")),FUNCTIONS(),2,0))</definedName>
     <definedName name="FUNCTIONS">_xlfn.LAMBDA(_xlfn._xlws.SORT(_xlfn.VSTACK(BUILTINS(),SL())))</definedName>
     <definedName name="GREATERTHAN?">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.x&gt;_xlpm.y)</definedName>
     <definedName name="GTE?">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.x&gt;=_xlpm.y)</definedName>
@@ -196,25 +196,196 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Water is wet.</t>
   </si>
   <si>
     <t>Water is not wet.</t>
+  </si>
+  <si>
+    <t>            HSTACK("IF", IF),</t>
+  </si>
+  <si>
+    <t>HSTACK("IF", IF),</t>
+  </si>
+  <si>
+    <t>HSTACK("IFERROR", IFERROR),</t>
+  </si>
+  <si>
+    <t>HSTACK("IFNA", IFNA),</t>
+  </si>
+  <si>
+    <t>HSTACK("IFS", IFS),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMABS", IMABS),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMAGE", IMAGE),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMAGINARY", IMAGINARY),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMARGUMENT", IMARGUMENT),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMCONJUGATE", IMCONJUGATE),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMCOS", IMCOS),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMCOSH", IMCOSH),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMCOT", IMCOT),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMCSC", IMCSC),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMCSCH", IMCSCH),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMDIV", IMDIV),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMEXP", IMEXP),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMLN", IMLN),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMLOG10", IMLOG10),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMLOG2", IMLOG2),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMPOWER", IMPOWER),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMPRODUCT", IMPRODUCT),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMREAL", IMREAL),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMSEC", IMSEC),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMSECH", IMSECH),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMSIN", IMSIN),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMSINH", IMSINH),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMSQRT", IMSQRT),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMSUB", IMSUB),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMSUM", IMSUM),</t>
+  </si>
+  <si>
+    <t>HSTACK("IMTAN", IMTAN),</t>
+  </si>
+  <si>
+    <t>HSTACK("INDEX", INDEX),</t>
+  </si>
+  <si>
+    <t>HSTACK("INDIRECT", INDIRECT),</t>
+  </si>
+  <si>
+    <t>HSTACK("INFO", INFO),</t>
+  </si>
+  <si>
+    <t>HSTACK("INT", INT),</t>
+  </si>
+  <si>
+    <t>HSTACK("INTERCEPT", INTERCEPT),</t>
+  </si>
+  <si>
+    <t>HSTACK("INTRATE", INTRATE),</t>
+  </si>
+  <si>
+    <t>HSTACK("IPMT", IPMT),</t>
+  </si>
+  <si>
+    <t>HSTACK("IRR", IRR),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISBLANK", ISBLANK),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISERR", ISERR),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISERROR", ISERROR),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISEVEN", ISEVEN),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISFORMULA", ISFORMULA),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISLOGICAL", ISLOGICAL),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISNA", ISNA),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISNONTEXT", ISNONTEXT),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISNUMBER", ISNUMBER),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISO.CEILING", ISO.CEILING),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISODD", ISODD),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISOMITTED", ISOMITTED),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISOWEEKNUM", ISOWEEKNUM),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISPMT", ISPMT),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISREF", ISREF),</t>
+  </si>
+  <si>
+    <t>HSTACK("ISTEXT", ISTEXT)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE6EDF3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,10 +408,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,7 +809,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94344BE4-A561-4B34-A305-2CE4884C8C8F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -644,9 +818,10 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="str" cm="1">
         <f t="array" aca="1" ref="A1:B121" ca="1">SL()</f>
         <v>_1_are_2.</v>
@@ -655,198 +830,198 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" cm="1">
+        <f t="array" aca="1" ref="D1" ca="1">APPLY(FUNCTION("INCREMENT"), 1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f ca="1"/>
+        <v>_1_is_2.</v>
+      </c>
+      <c r="B2" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f ca="1"/>
+        <v>_1_is_not_2.</v>
+      </c>
+      <c r="B3" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f ca="1"/>
-        <v>_1_is_2.</v>
-      </c>
-      <c r="B2" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f ca="1"/>
+        <v>_Is_1_2?</v>
+      </c>
+      <c r="B4" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f ca="1"/>
-        <v>_1_is_not_2.</v>
-      </c>
-      <c r="B3" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D3" t="str" cm="1">
-        <f t="array" ref="D3">_Is_1_2?("water", "wet", D1:D2)</f>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f ca="1"/>
+        <v>ALL</v>
+      </c>
+      <c r="B5" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5" t="str" cm="1">
+        <f t="array" ref="D5">_Is_1_2?("water", "wet", D3:D4)</f>
         <v>Yes and no. Water simultaneously is and is not wet.</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f ca="1"/>
-        <v>_Is_1_2?</v>
-      </c>
-      <c r="B4" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f ca="1"/>
-        <v>ALL</v>
-      </c>
-      <c r="B5" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D5" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="D5:D14" ca="1">FLIPCOIN(10)</f>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f ca="1"/>
+        <v>ALPHABET</v>
+      </c>
+      <c r="B6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f ca="1"/>
+        <v>APPEND</v>
+      </c>
+      <c r="B7" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D7" t="str" cm="1">
+        <f t="array" aca="1" ref="D7:D16" ca="1">FLIPCOIN(10)</f>
         <v>Tails</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f ca="1"/>
-        <v>ALPHABET</v>
-      </c>
-      <c r="B6" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D6" s="1" t="str">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f ca="1"/>
+        <v>APPLY</v>
+      </c>
+      <c r="B8" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D8" t="str">
+        <f ca="1"/>
+        <v>Heads</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f ca="1"/>
+        <v>ARITY</v>
+      </c>
+      <c r="B9" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D9" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f ca="1"/>
-        <v>APPEND</v>
-      </c>
-      <c r="B7" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D7" s="1" t="str">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f ca="1"/>
+        <v>ASSERT</v>
+      </c>
+      <c r="B10" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D10" t="str">
+        <f ca="1"/>
+        <v>Heads</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f ca="1"/>
+        <v>BUILTINS</v>
+      </c>
+      <c r="B11" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f ca="1"/>
-        <v>APPLY</v>
-      </c>
-      <c r="B8" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D8" s="1" t="str">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f ca="1"/>
+        <v>BUILTINS.A</v>
+      </c>
+      <c r="B12" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f ca="1"/>
-        <v>ARITY</v>
-      </c>
-      <c r="B9" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D9" s="1" t="str">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f ca="1"/>
+        <v>BUILTINS.B</v>
+      </c>
+      <c r="B13" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" t="str">
         <f ca="1"/>
         <v>Tails</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f ca="1"/>
-        <v>ASSERT</v>
-      </c>
-      <c r="B10" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D10" s="1" t="str">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f ca="1"/>
+        <v>BUILTINS.C</v>
+      </c>
+      <c r="B14" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f ca="1"/>
-        <v>BUILTINS</v>
-      </c>
-      <c r="B11" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D11" s="1" t="str">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f ca="1"/>
+        <v>BUILTINS.D</v>
+      </c>
+      <c r="B15" t="e" vm="1">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D15" t="str">
         <f ca="1"/>
         <v>Heads</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f ca="1"/>
-        <v>BUILTINS.A</v>
-      </c>
-      <c r="B12" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f ca="1"/>
-        <v>Heads</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f ca="1"/>
-        <v>BUILTINS.B</v>
-      </c>
-      <c r="B13" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f ca="1"/>
-        <v>Heads</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f ca="1"/>
-        <v>BUILTINS.C</v>
-      </c>
-      <c r="B14" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f ca="1"/>
-        <v>Heads</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f ca="1"/>
-        <v>BUILTINS.D</v>
-      </c>
-      <c r="B15" t="e" vm="1">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f ca="1"/>
         <v>BUILTINS.E</v>
@@ -855,8 +1030,15 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f ca="1"/>
+        <v>Tails</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f ca="1"/>
         <v>BUILTINS.F</v>
@@ -865,8 +1047,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f ca="1"/>
         <v>BUILTINS.G</v>
@@ -875,8 +1060,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f ca="1"/>
         <v>BUILTINS.H</v>
@@ -885,8 +1073,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f ca="1"/>
         <v>BUILTINS.I</v>
@@ -895,8 +1086,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f ca="1"/>
         <v>BUILTINS.K</v>
@@ -905,8 +1099,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f ca="1"/>
         <v>BUILTINS.L</v>
@@ -915,8 +1112,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f ca="1"/>
         <v>BUILTINS.M</v>
@@ -925,8 +1125,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f ca="1"/>
         <v>BUILTINS.N</v>
@@ -935,8 +1138,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f ca="1"/>
         <v>BUILTINS.O</v>
@@ -945,8 +1151,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f ca="1"/>
         <v>BUILTINS.P</v>
@@ -955,8 +1164,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f ca="1"/>
         <v>BUILTINS.Q</v>
@@ -965,8 +1177,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f ca="1"/>
         <v>BUILTINS.R</v>
@@ -975,8 +1190,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f ca="1"/>
         <v>BUILTINS.S</v>
@@ -985,8 +1203,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f ca="1"/>
         <v>BUILTINS.T</v>
@@ -995,8 +1216,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f ca="1"/>
         <v>BUILTINS.U</v>
@@ -1005,8 +1229,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G31" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f ca="1"/>
         <v>BUILTINS.V</v>
@@ -1015,8 +1242,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f ca="1"/>
         <v>BUILTINS.W</v>
@@ -1025,8 +1255,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G33" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f ca="1"/>
         <v>BUILTINS.X</v>
@@ -1035,8 +1268,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G34" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f ca="1"/>
         <v>BUILTINS.Y</v>
@@ -1045,8 +1281,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G35" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f ca="1"/>
         <v>BUILTINS.Z</v>
@@ -1055,8 +1294,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G36" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f ca="1"/>
         <v>CAPITALIZE</v>
@@ -1065,8 +1307,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G37" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f ca="1"/>
         <v>CAR</v>
@@ -1075,8 +1320,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G38" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f ca="1"/>
         <v>CASE</v>
@@ -1085,8 +1333,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G39" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f ca="1"/>
         <v>CDR</v>
@@ -1095,8 +1346,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G40" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f ca="1"/>
         <v>CELLNAME</v>
@@ -1105,8 +1359,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G41" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f ca="1"/>
         <v>COINTOSS</v>
@@ -1115,8 +1372,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G42" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f ca="1"/>
         <v>COLUMNLETTER</v>
@@ -1125,8 +1385,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G43" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f ca="1"/>
         <v>CONS</v>
@@ -1135,8 +1398,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G44" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f ca="1"/>
         <v>CONSTANCY</v>
@@ -1145,8 +1411,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G45" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f ca="1"/>
         <v>CONTAINS</v>
@@ -1155,8 +1424,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G46" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f ca="1"/>
         <v>COUNTCELLS</v>
@@ -1165,8 +1437,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G47" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f ca="1"/>
         <v>CRITERIATABLE</v>
@@ -1175,8 +1450,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G48" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f ca="1"/>
         <v>CUBEROOT</v>
@@ -1185,8 +1463,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G49" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f ca="1"/>
         <v>CURRY</v>
@@ -1195,8 +1476,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G50" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f ca="1"/>
         <v>DECREMENT</v>
@@ -1205,8 +1489,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G51" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f ca="1"/>
         <v>DEFAULT</v>
@@ -1215,8 +1502,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G52" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f ca="1"/>
         <v>DICEROLL</v>
@@ -1225,8 +1515,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G53" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f ca="1"/>
         <v>DIFFERENCE</v>
@@ -1235,8 +1528,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G54" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f ca="1"/>
         <v>EMPTYLIST?</v>
@@ -1245,8 +1541,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G55" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f ca="1"/>
         <v>EQUAL</v>
@@ -1255,8 +1554,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G56" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f ca="1"/>
         <v>EXTRACTOPERATOR</v>
@@ -1265,8 +1567,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G57" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f ca="1"/>
         <v>EXTRACTOPERATORS</v>
@@ -1275,8 +1580,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G58" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f ca="1"/>
         <v>FILENAME</v>
@@ -1285,8 +1593,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G59" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f ca="1"/>
         <v>FIRST</v>
@@ -1295,8 +1606,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G60" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f ca="1"/>
         <v>FIRSTCOLUMN</v>
@@ -1305,8 +1619,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G61" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f ca="1"/>
         <v>FIRSTLETTER</v>
@@ -1315,8 +1632,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G62" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f ca="1"/>
         <v>FIRSTROW</v>
@@ -1325,8 +1645,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G63" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f ca="1"/>
         <v>FIRSTWORD</v>
@@ -1335,8 +1658,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G64" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f ca="1"/>
         <v>FLIPCOIN</v>
@@ -1345,8 +1671,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G65" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f ca="1"/>
         <v>FOREACH</v>
@@ -1355,8 +1684,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G66" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f ca="1"/>
         <v>FORMAT</v>
@@ -1365,8 +1697,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G67" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f ca="1"/>
         <v>FULLDECK</v>
@@ -1375,8 +1710,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G68" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f ca="1"/>
         <v>FUNCTION</v>
@@ -1385,8 +1723,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G69" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f ca="1"/>
         <v>FUNCTIONS</v>
@@ -1395,8 +1736,11 @@
         <f ca="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G70" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f ca="1"/>
         <v>GREATERTHAN?</v>
@@ -1406,7 +1750,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f ca="1"/>
         <v>GTE?</v>
@@ -1416,7 +1760,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f ca="1"/>
         <v>HEADLESS</v>
@@ -1426,7 +1770,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f ca="1"/>
         <v>HLIST</v>
@@ -1436,7 +1780,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f ca="1"/>
         <v>HORIZONTAL?</v>
@@ -1446,7 +1790,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f ca="1"/>
         <v>IDENTITY</v>
@@ -1456,7 +1800,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f ca="1"/>
         <v>IFBLANK</v>
@@ -1466,7 +1810,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f ca="1"/>
         <v>IFOMITTED</v>
@@ -1476,7 +1820,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f ca="1"/>
         <v>INCREMENT</v>
@@ -1486,7 +1830,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f ca="1"/>
         <v>INDICES</v>

</xml_diff>